<commit_message>
Python script creates parameter csv's problem free
</commit_message>
<xml_diff>
--- a/InitializationData/Simulation_Parameters.xlsx
+++ b/InitializationData/Simulation_Parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/fce19_ic_ac_uk/Documents/Programming/GithubRepos/Vulcan/InitializationData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feyzi\OneDrive - Imperial College London\Programming\GithubRepos\Vulcan\InitializationData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="14_{C0C84F9E-D570-49CC-826A-B72FAEB8A355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45A37A4C-C249-4BDD-9F69-DA31DF5662C5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2789D3D-72AF-47F8-8963-7AEAFB4BBD7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2196" yWindow="2868" windowWidth="9288" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initialization_Parameters" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="203">
   <si>
     <t>household_init_c_std</t>
   </si>
@@ -619,6 +619,24 @@
   </si>
   <si>
     <t>max_production_climbdown</t>
+  </si>
+  <si>
+    <t>Agent Randomness Parameters</t>
+  </si>
+  <si>
+    <t>bank_randomness</t>
+  </si>
+  <si>
+    <t>household_randomness</t>
+  </si>
+  <si>
+    <t>consumer_firm_randomness</t>
+  </si>
+  <si>
+    <t>capital_firm_randomness</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -947,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -962,6 +980,9 @@
       <c r="A1" s="1" t="s">
         <v>130</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -2025,7 +2046,7 @@
   <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2037,6 +2058,9 @@
       <c r="A1" s="1" t="s">
         <v>170</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -2358,12 +2382,78 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6246507C-746B-43E5-B640-89BA4FF02F66}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>201</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2372,8 +2462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2595549C-8B86-4913-AB74-2D11D251B047}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Completed easy user configuration
</commit_message>
<xml_diff>
--- a/InitializationData/Simulation_Parameters.xlsx
+++ b/InitializationData/Simulation_Parameters.xlsx
@@ -5,20 +5,33 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feyzi\OneDrive - Imperial College London\Programming\GithubRepos\Vulcan\InitializationData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/fce19_ic_ac_uk/Documents/Programming/GithubRepos/Vulcan/InitializationData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6332634C-3D08-4B9D-8691-6AE2AF47708E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{6332634C-3D08-4B9D-8691-6AE2AF47708E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{758073A9-BF27-4EC3-B7C8-C3114BDC1406}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initialization_Parameters" sheetId="1" r:id="rId1"/>
     <sheet name="Main_Loop_Parameters" sheetId="2" r:id="rId2"/>
     <sheet name="Randomness_Parameters" sheetId="3" r:id="rId3"/>
-    <sheet name="Consumer_Sectors" sheetId="4" r:id="rId4"/>
+    <sheet name="Consumer_Firm_Sectors" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1014,7 +1027,9 @@
   </sheetPr>
   <dimension ref="A1:B134"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2094,7 +2109,9 @@
   </sheetPr>
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2120,7 +2137,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="4">
-        <v>36</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2128,7 +2145,7 @@
         <v>34</v>
       </c>
       <c r="B4" s="4">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2136,7 +2153,7 @@
         <v>35</v>
       </c>
       <c r="B5" s="4">
-        <v>45</v>
+        <v>400</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2144,7 +2161,7 @@
         <v>36</v>
       </c>
       <c r="B6" s="4">
-        <v>5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2152,7 +2169,8 @@
         <v>37</v>
       </c>
       <c r="B7" s="4">
-        <v>50</v>
+        <f>B5+B6</f>
+        <v>450</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2515,8 +2533,8 @@
   </sheetPr>
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Work in progress to add bakruptcies and co2
</commit_message>
<xml_diff>
--- a/InitializationData/Simulation_Parameters.xlsx
+++ b/InitializationData/Simulation_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/fce19_ic_ac_uk/Documents/Programming/GithubRepos/Vulcan/InitializationData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{6332634C-3D08-4B9D-8691-6AE2AF47708E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{758073A9-BF27-4EC3-B7C8-C3114BDC1406}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{D7B19F01-C027-476C-9166-DE9C897A9ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14321C29-8429-4BD4-ADF2-F2B84D54398B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initialization_Parameters" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="205">
   <si>
     <t>sector_name</t>
   </si>
@@ -515,9 +515,6 @@
     <t>firm_cons_init_quantity_sold_ratio</t>
   </si>
   <si>
-    <t>firm_cons_init_good_price_</t>
-  </si>
-  <si>
     <t>firm_cap_init_total_assets_mean</t>
   </si>
   <si>
@@ -645,6 +642,15 @@
   </si>
   <si>
     <t>firm_cap_init_good_price</t>
+  </si>
+  <si>
+    <t>emissions_per_unit</t>
+  </si>
+  <si>
+    <t>firm_cap_init_emissions_per_unit</t>
+  </si>
+  <si>
+    <t>firm_cons_init_good_price</t>
   </si>
 </sst>
 </file>
@@ -1025,10 +1031,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B134"/>
+  <dimension ref="A1:B136"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1742,180 +1748,180 @@
     </row>
     <row r="90" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>159</v>
+        <v>204</v>
       </c>
       <c r="B90" s="3">
         <v>9.5</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="5" t="s">
+      <c r="A91" t="s">
+        <v>203</v>
+      </c>
+      <c r="B91" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="5" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>160</v>
-      </c>
-      <c r="B92" s="4">
-        <v>10000</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B93" s="4">
-        <v>2500</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B94" s="4">
-        <v>1</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B95" s="4">
-        <v>999999999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>164</v>
-      </c>
-      <c r="B96" s="3">
-        <v>0.05</v>
+        <v>162</v>
+      </c>
+      <c r="B96" s="4">
+        <v>999999999</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B97" s="3">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B98" s="3">
-        <v>5.0000000000000001E-3</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B99" s="3">
-        <v>0.2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B100" s="3">
-        <v>0.03</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B101" s="3">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B102" s="3">
-        <v>1E-3</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B103" s="3">
-        <v>0.15</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>172</v>
-      </c>
-      <c r="B104" s="4">
-        <v>1000</v>
+        <v>170</v>
+      </c>
+      <c r="B104" s="3">
+        <v>0.15</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B105" s="4">
-        <v>300</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B106" s="4">
-        <v>100</v>
+        <v>300</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B107" s="4">
-        <v>999999</v>
+        <v>100</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B108" s="4">
-        <v>20</v>
+        <v>999999</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B109" s="4">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B110" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B111" s="4">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B112" s="4">
         <v>100</v>
@@ -1923,15 +1929,15 @@
     </row>
     <row r="113" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B113" s="4">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B114" s="4">
         <v>10</v>
@@ -1939,161 +1945,177 @@
     </row>
     <row r="115" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B115" s="4">
-        <v>999</v>
+        <v>10</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B116" s="4">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B117" s="4">
-        <v>200</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B118" s="4">
-        <v>100</v>
+        <v>200</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B119" s="4">
-        <v>9999</v>
+        <v>100</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B120" s="4">
-        <v>100</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B121" s="4">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B122" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B123" s="4">
-        <v>9999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B124" s="4">
-        <v>60</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B125" s="4">
-        <v>5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B126" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B127" s="4">
-        <v>999999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>196</v>
-      </c>
-      <c r="B128" s="3">
-        <v>1.5</v>
+        <v>194</v>
+      </c>
+      <c r="B128" s="4">
+        <v>999999</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B129" s="3">
-        <v>0.25</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B130" s="3">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>199</v>
-      </c>
-      <c r="B131" s="4">
-        <v>4</v>
+        <v>197</v>
+      </c>
+      <c r="B131" s="3">
+        <v>0.1</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>200</v>
-      </c>
-      <c r="B132" s="3">
-        <v>0.4</v>
+        <v>198</v>
+      </c>
+      <c r="B132" s="4">
+        <v>4</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B133" s="3">
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>202</v>
-      </c>
-      <c r="B134" s="4">
+        <v>200</v>
+      </c>
+      <c r="B134" s="3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>201</v>
+      </c>
+      <c r="B135" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>203</v>
+      </c>
+      <c r="B136" s="2">
         <v>100</v>
       </c>
     </row>
@@ -2109,7 +2131,7 @@
   </sheetPr>
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2531,10 +2553,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2548,9 +2570,10 @@
     <col min="7" max="7" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2578,8 +2601,11 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J1" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2607,8 +2633,11 @@
       <c r="I2" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J2" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2636,8 +2665,11 @@
       <c r="I3" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2665,8 +2697,11 @@
       <c r="I4" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J4" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -2694,8 +2729,11 @@
       <c r="I5" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J5" s="4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -2723,8 +2761,11 @@
       <c r="I6" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J6" s="4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2752,8 +2793,11 @@
       <c r="I7" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J7" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2781,8 +2825,11 @@
       <c r="I8" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J8" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2810,8 +2857,11 @@
       <c r="I9" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J9" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2839,8 +2889,11 @@
       <c r="I10" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J10" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2868,8 +2921,11 @@
       <c r="I11" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J11" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2897,8 +2953,11 @@
       <c r="I12" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J12" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -2925,6 +2984,9 @@
       </c>
       <c r="I13" s="3">
         <v>0.1</v>
+      </c>
+      <c r="J13" s="4">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding emission funcs to cons goods
</commit_message>
<xml_diff>
--- a/InitializationData/Simulation_Parameters.xlsx
+++ b/InitializationData/Simulation_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/fce19_ic_ac_uk/Documents/Programming/GithubRepos/Vulcan/InitializationData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{D7B19F01-C027-476C-9166-DE9C897A9ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14321C29-8429-4BD4-ADF2-F2B84D54398B}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="13_ncr:1_{D7B19F01-C027-476C-9166-DE9C897A9ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24E47B77-FFA4-4BBA-AE56-C89490E24AC2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initialization_Parameters" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="212">
   <si>
     <t>sector_name</t>
   </si>
@@ -110,27 +110,15 @@
     <t>Bank</t>
   </si>
   <si>
-    <t>bank_randomness</t>
-  </si>
-  <si>
     <t>Households</t>
   </si>
   <si>
-    <t>household_randomness</t>
-  </si>
-  <si>
     <t>Consumer Firms</t>
   </si>
   <si>
-    <t>consumer_firm_randomness</t>
-  </si>
-  <si>
     <t>Capital Firms</t>
   </si>
   <si>
-    <t>capital_firm_randomness</t>
-  </si>
-  <si>
     <t>Simulation Parameters</t>
   </si>
   <si>
@@ -651,13 +639,49 @@
   </si>
   <si>
     <t>firm_cons_init_good_price</t>
+  </si>
+  <si>
+    <t>bank_random_experimentation</t>
+  </si>
+  <si>
+    <t>Firms</t>
+  </si>
+  <si>
+    <t>firm_random_experimentation</t>
+  </si>
+  <si>
+    <t>household_random_experimentation</t>
+  </si>
+  <si>
+    <t>household_majority_sentiment_adoption</t>
+  </si>
+  <si>
+    <t>firm_random_dividend_changes</t>
+  </si>
+  <si>
+    <t>household_rand_spending_weight_change_prob</t>
+  </si>
+  <si>
+    <t>household_rand_spending_weight_change</t>
+  </si>
+  <si>
+    <t>household_majority_sentiment_adoption_prob</t>
+  </si>
+  <si>
+    <t>household_rand_emission_weight_change_prob</t>
+  </si>
+  <si>
+    <t>household_rand_emission_weight_change</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -673,6 +697,27 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -706,7 +751,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -725,6 +770,25 @@
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1033,7 +1097,7 @@
   </sheetPr>
   <dimension ref="A1:B136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+    <sheetView topLeftCell="A86" workbookViewId="0">
       <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
@@ -1045,7 +1109,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>22</v>
@@ -1058,7 +1122,7 @@
     </row>
     <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B3" s="3">
         <v>0.02</v>
@@ -1066,12 +1130,12 @@
     </row>
     <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B5" s="3">
         <v>0.15</v>
@@ -1079,7 +1143,7 @@
     </row>
     <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B6" s="3">
         <v>0.1</v>
@@ -1087,7 +1151,7 @@
     </row>
     <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B7" s="3">
         <v>0.9</v>
@@ -1095,7 +1159,7 @@
     </row>
     <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B8" s="3">
         <v>0.5</v>
@@ -1103,7 +1167,7 @@
     </row>
     <row r="9" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B9" s="3">
         <v>0.5</v>
@@ -1111,7 +1175,7 @@
     </row>
     <row r="10" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B10" s="3">
         <v>0.1</v>
@@ -1119,7 +1183,7 @@
     </row>
     <row r="11" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B11" s="3">
         <v>0.1</v>
@@ -1127,7 +1191,7 @@
     </row>
     <row r="12" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B12" s="3">
         <v>0.9</v>
@@ -1135,7 +1199,7 @@
     </row>
     <row r="13" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B13" s="3">
         <v>0.2</v>
@@ -1143,7 +1207,7 @@
     </row>
     <row r="14" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B14" s="3">
         <v>0.05</v>
@@ -1151,7 +1215,7 @@
     </row>
     <row r="15" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B15" s="4">
         <v>0</v>
@@ -1159,7 +1223,7 @@
     </row>
     <row r="16" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B16" s="3">
         <v>0.4</v>
@@ -1167,7 +1231,7 @@
     </row>
     <row r="17" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B17" s="3">
         <v>0.3</v>
@@ -1175,7 +1239,7 @@
     </row>
     <row r="18" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B18" s="3">
         <v>0.05</v>
@@ -1183,7 +1247,7 @@
     </row>
     <row r="19" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B19" s="4">
         <v>0</v>
@@ -1191,7 +1255,7 @@
     </row>
     <row r="20" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B20" s="3">
         <v>0.7</v>
@@ -1199,7 +1263,7 @@
     </row>
     <row r="21" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B21" s="3">
         <v>0.25</v>
@@ -1207,7 +1271,7 @@
     </row>
     <row r="22" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B22" s="3">
         <v>0.2</v>
@@ -1215,7 +1279,7 @@
     </row>
     <row r="23" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B23" s="3">
         <v>0.01</v>
@@ -1223,7 +1287,7 @@
     </row>
     <row r="24" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B24" s="3">
         <v>0.99</v>
@@ -1231,7 +1295,7 @@
     </row>
     <row r="25" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B25" s="3">
         <v>0.2</v>
@@ -1239,7 +1303,7 @@
     </row>
     <row r="26" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B26" s="3">
         <v>0.05</v>
@@ -1247,7 +1311,7 @@
     </row>
     <row r="27" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B27" s="4">
         <v>0</v>
@@ -1255,7 +1319,7 @@
     </row>
     <row r="28" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B28" s="3">
         <v>0.5</v>
@@ -1263,7 +1327,7 @@
     </row>
     <row r="29" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B29" s="3">
         <v>0.3</v>
@@ -1271,7 +1335,7 @@
     </row>
     <row r="30" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B30" s="3">
         <v>0.05</v>
@@ -1279,7 +1343,7 @@
     </row>
     <row r="31" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B31" s="3">
         <v>0.1</v>
@@ -1287,7 +1351,7 @@
     </row>
     <row r="32" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B32" s="3">
         <v>0.6</v>
@@ -1295,7 +1359,7 @@
     </row>
     <row r="33" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B33" s="4">
         <v>1000</v>
@@ -1303,7 +1367,7 @@
     </row>
     <row r="34" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B34" s="4">
         <v>300</v>
@@ -1311,7 +1375,7 @@
     </row>
     <row r="35" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B35" s="4">
         <v>0</v>
@@ -1319,7 +1383,7 @@
     </row>
     <row r="36" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B36" s="4">
         <v>2000</v>
@@ -1327,7 +1391,7 @@
     </row>
     <row r="37" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B37" s="4">
         <v>4</v>
@@ -1335,7 +1399,7 @@
     </row>
     <row r="38" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B38" s="4">
         <v>2</v>
@@ -1343,7 +1407,7 @@
     </row>
     <row r="39" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B39" s="4">
         <v>0</v>
@@ -1351,7 +1415,7 @@
     </row>
     <row r="40" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B40" s="4">
         <v>100</v>
@@ -1359,7 +1423,7 @@
     </row>
     <row r="41" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B41" s="4">
         <v>950</v>
@@ -1367,7 +1431,7 @@
     </row>
     <row r="42" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B42" s="4">
         <v>300</v>
@@ -1375,7 +1439,7 @@
     </row>
     <row r="43" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B43" s="4">
         <v>100</v>
@@ -1383,7 +1447,7 @@
     </row>
     <row r="44" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B44" s="4">
         <v>999999</v>
@@ -1391,7 +1455,7 @@
     </row>
     <row r="45" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B45" s="4">
         <v>500</v>
@@ -1399,7 +1463,7 @@
     </row>
     <row r="46" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B46" s="4">
         <v>600</v>
@@ -1407,12 +1471,12 @@
     </row>
     <row r="47" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B48" s="4">
         <v>10000</v>
@@ -1420,7 +1484,7 @@
     </row>
     <row r="49" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B49" s="4">
         <v>2500</v>
@@ -1428,7 +1492,7 @@
     </row>
     <row r="50" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B50" s="4">
         <v>1</v>
@@ -1436,7 +1500,7 @@
     </row>
     <row r="51" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B51" s="4">
         <v>999999999</v>
@@ -1444,7 +1508,7 @@
     </row>
     <row r="52" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B52" s="3">
         <v>0.05</v>
@@ -1452,7 +1516,7 @@
     </row>
     <row r="53" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B53" s="3">
         <v>0.02</v>
@@ -1460,7 +1524,7 @@
     </row>
     <row r="54" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B54" s="3">
         <v>5.0000000000000001E-3</v>
@@ -1468,7 +1532,7 @@
     </row>
     <row r="55" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B55" s="3">
         <v>0.2</v>
@@ -1476,7 +1540,7 @@
     </row>
     <row r="56" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B56" s="3">
         <v>0.03</v>
@@ -1484,7 +1548,7 @@
     </row>
     <row r="57" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B57" s="3">
         <v>0.02</v>
@@ -1492,7 +1556,7 @@
     </row>
     <row r="58" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B58" s="3">
         <v>1E-3</v>
@@ -1500,7 +1564,7 @@
     </row>
     <row r="59" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B59" s="3">
         <v>0.15</v>
@@ -1508,7 +1572,7 @@
     </row>
     <row r="60" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B60" s="4">
         <v>1000</v>
@@ -1516,7 +1580,7 @@
     </row>
     <row r="61" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B61" s="4">
         <v>300</v>
@@ -1524,7 +1588,7 @@
     </row>
     <row r="62" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B62" s="4">
         <v>100</v>
@@ -1532,7 +1596,7 @@
     </row>
     <row r="63" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B63" s="4">
         <v>999999</v>
@@ -1540,7 +1604,7 @@
     </row>
     <row r="64" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B64" s="4">
         <v>20</v>
@@ -1548,7 +1612,7 @@
     </row>
     <row r="65" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B65" s="4">
         <v>5</v>
@@ -1556,7 +1620,7 @@
     </row>
     <row r="66" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B66" s="4">
         <v>1</v>
@@ -1564,7 +1628,7 @@
     </row>
     <row r="67" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B67" s="4">
         <v>100</v>
@@ -1572,7 +1636,7 @@
     </row>
     <row r="68" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B68" s="4">
         <v>1000</v>
@@ -1580,7 +1644,7 @@
     </row>
     <row r="69" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B69" s="4">
         <v>100</v>
@@ -1588,7 +1652,7 @@
     </row>
     <row r="70" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B70" s="4">
         <v>100</v>
@@ -1596,7 +1660,7 @@
     </row>
     <row r="71" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B71" s="4">
         <v>1999</v>
@@ -1604,7 +1668,7 @@
     </row>
     <row r="72" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B72" s="4">
         <v>10</v>
@@ -1612,7 +1676,7 @@
     </row>
     <row r="73" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B73" s="4">
         <v>2</v>
@@ -1620,7 +1684,7 @@
     </row>
     <row r="74" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B74" s="4">
         <v>1</v>
@@ -1628,7 +1692,7 @@
     </row>
     <row r="75" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B75" s="4">
         <v>99</v>
@@ -1636,7 +1700,7 @@
     </row>
     <row r="76" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B76" s="4">
         <v>1000</v>
@@ -1644,7 +1708,7 @@
     </row>
     <row r="77" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B77" s="4">
         <v>100</v>
@@ -1652,7 +1716,7 @@
     </row>
     <row r="78" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B78" s="4">
         <v>1</v>
@@ -1660,7 +1724,7 @@
     </row>
     <row r="79" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B79" s="4">
         <v>999999</v>
@@ -1668,7 +1732,7 @@
     </row>
     <row r="80" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B80" s="4">
         <v>60</v>
@@ -1676,7 +1740,7 @@
     </row>
     <row r="81" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B81" s="4">
         <v>5</v>
@@ -1684,7 +1748,7 @@
     </row>
     <row r="82" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B82" s="4">
         <v>1</v>
@@ -1692,7 +1756,7 @@
     </row>
     <row r="83" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B83" s="4">
         <v>999999</v>
@@ -1700,7 +1764,7 @@
     </row>
     <row r="84" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B84" s="3">
         <v>1.5</v>
@@ -1708,7 +1772,7 @@
     </row>
     <row r="85" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B85" s="3">
         <v>0.25</v>
@@ -1716,7 +1780,7 @@
     </row>
     <row r="86" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B86" s="3">
         <v>0.1</v>
@@ -1724,7 +1788,7 @@
     </row>
     <row r="87" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B87" s="4">
         <v>4</v>
@@ -1732,7 +1796,7 @@
     </row>
     <row r="88" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B88" s="3">
         <v>0.4</v>
@@ -1740,7 +1804,7 @@
     </row>
     <row r="89" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B89" s="3">
         <v>0.25</v>
@@ -1748,7 +1812,7 @@
     </row>
     <row r="90" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B90" s="3">
         <v>9.5</v>
@@ -1756,7 +1820,7 @@
     </row>
     <row r="91" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B91" s="3">
         <v>10</v>
@@ -1764,12 +1828,12 @@
     </row>
     <row r="92" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B93" s="4">
         <v>10000</v>
@@ -1777,7 +1841,7 @@
     </row>
     <row r="94" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B94" s="4">
         <v>2500</v>
@@ -1785,7 +1849,7 @@
     </row>
     <row r="95" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B95" s="4">
         <v>1</v>
@@ -1793,7 +1857,7 @@
     </row>
     <row r="96" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B96" s="4">
         <v>999999999</v>
@@ -1801,7 +1865,7 @@
     </row>
     <row r="97" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B97" s="3">
         <v>0.05</v>
@@ -1809,7 +1873,7 @@
     </row>
     <row r="98" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B98" s="3">
         <v>0.02</v>
@@ -1817,7 +1881,7 @@
     </row>
     <row r="99" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B99" s="3">
         <v>5.0000000000000001E-3</v>
@@ -1825,7 +1889,7 @@
     </row>
     <row r="100" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B100" s="3">
         <v>0.2</v>
@@ -1833,7 +1897,7 @@
     </row>
     <row r="101" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B101" s="3">
         <v>0.03</v>
@@ -1841,7 +1905,7 @@
     </row>
     <row r="102" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B102" s="3">
         <v>0.02</v>
@@ -1849,7 +1913,7 @@
     </row>
     <row r="103" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B103" s="3">
         <v>1E-3</v>
@@ -1857,7 +1921,7 @@
     </row>
     <row r="104" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B104" s="3">
         <v>0.15</v>
@@ -1865,7 +1929,7 @@
     </row>
     <row r="105" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B105" s="4">
         <v>1000</v>
@@ -1873,7 +1937,7 @@
     </row>
     <row r="106" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B106" s="4">
         <v>300</v>
@@ -1881,7 +1945,7 @@
     </row>
     <row r="107" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B107" s="4">
         <v>100</v>
@@ -1889,7 +1953,7 @@
     </row>
     <row r="108" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B108" s="4">
         <v>999999</v>
@@ -1897,7 +1961,7 @@
     </row>
     <row r="109" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B109" s="4">
         <v>20</v>
@@ -1905,7 +1969,7 @@
     </row>
     <row r="110" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B110" s="4">
         <v>5</v>
@@ -1913,7 +1977,7 @@
     </row>
     <row r="111" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B111" s="4">
         <v>1</v>
@@ -1921,7 +1985,7 @@
     </row>
     <row r="112" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B112" s="4">
         <v>100</v>
@@ -1929,7 +1993,7 @@
     </row>
     <row r="113" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B113" s="4">
         <v>100</v>
@@ -1937,7 +2001,7 @@
     </row>
     <row r="114" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B114" s="4">
         <v>10</v>
@@ -1945,7 +2009,7 @@
     </row>
     <row r="115" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B115" s="4">
         <v>10</v>
@@ -1953,7 +2017,7 @@
     </row>
     <row r="116" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B116" s="4">
         <v>999</v>
@@ -1961,7 +2025,7 @@
     </row>
     <row r="117" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B117" s="4">
         <v>1000</v>
@@ -1969,7 +2033,7 @@
     </row>
     <row r="118" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B118" s="4">
         <v>200</v>
@@ -1977,7 +2041,7 @@
     </row>
     <row r="119" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B119" s="4">
         <v>100</v>
@@ -1985,7 +2049,7 @@
     </row>
     <row r="120" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B120" s="4">
         <v>9999</v>
@@ -1993,7 +2057,7 @@
     </row>
     <row r="121" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B121" s="4">
         <v>100</v>
@@ -2001,7 +2065,7 @@
     </row>
     <row r="122" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B122" s="4">
         <v>10</v>
@@ -2009,7 +2073,7 @@
     </row>
     <row r="123" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B123" s="4">
         <v>1</v>
@@ -2017,7 +2081,7 @@
     </row>
     <row r="124" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B124" s="4">
         <v>9999</v>
@@ -2025,7 +2089,7 @@
     </row>
     <row r="125" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B125" s="4">
         <v>60</v>
@@ -2033,7 +2097,7 @@
     </row>
     <row r="126" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B126" s="4">
         <v>5</v>
@@ -2041,7 +2105,7 @@
     </row>
     <row r="127" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B127" s="4">
         <v>1</v>
@@ -2049,7 +2113,7 @@
     </row>
     <row r="128" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B128" s="4">
         <v>999999</v>
@@ -2057,7 +2121,7 @@
     </row>
     <row r="129" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B129" s="3">
         <v>1.5</v>
@@ -2065,7 +2129,7 @@
     </row>
     <row r="130" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B130" s="3">
         <v>0.25</v>
@@ -2073,7 +2137,7 @@
     </row>
     <row r="131" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B131" s="3">
         <v>0.1</v>
@@ -2081,7 +2145,7 @@
     </row>
     <row r="132" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B132" s="4">
         <v>4</v>
@@ -2089,7 +2153,7 @@
     </row>
     <row r="133" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B133" s="3">
         <v>0.4</v>
@@ -2097,7 +2161,7 @@
     </row>
     <row r="134" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B134" s="3">
         <v>0.25</v>
@@ -2105,7 +2169,7 @@
     </row>
     <row r="135" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B135" s="4">
         <v>100</v>
@@ -2113,7 +2177,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B136" s="2">
         <v>100</v>
@@ -2143,7 +2207,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>22</v>
@@ -2151,12 +2215,12 @@
     </row>
     <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B3" s="4">
         <v>60</v>
@@ -2164,7 +2228,7 @@
     </row>
     <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B4" s="4">
         <v>10000</v>
@@ -2172,7 +2236,7 @@
     </row>
     <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B5" s="4">
         <v>400</v>
@@ -2180,7 +2244,7 @@
     </row>
     <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B6" s="4">
         <v>50</v>
@@ -2188,7 +2252,7 @@
     </row>
     <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B7" s="4">
         <f>B5+B6</f>
@@ -2197,7 +2261,7 @@
     </row>
     <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B8" s="4">
         <v>100</v>
@@ -2205,7 +2269,7 @@
     </row>
     <row r="9" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B9" s="4">
         <v>12</v>
@@ -2213,12 +2277,12 @@
     </row>
     <row r="10" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B11" s="3">
         <v>0.05</v>
@@ -2226,7 +2290,7 @@
     </row>
     <row r="12" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B12" s="4">
         <v>3</v>
@@ -2234,7 +2298,7 @@
     </row>
     <row r="13" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B13" s="3">
         <v>0.2</v>
@@ -2242,7 +2306,7 @@
     </row>
     <row r="14" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B14" s="3">
         <v>0.1</v>
@@ -2250,7 +2314,7 @@
     </row>
     <row r="15" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B15" s="3">
         <v>0.1</v>
@@ -2258,7 +2322,7 @@
     </row>
     <row r="16" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B16" s="4">
         <v>6</v>
@@ -2266,7 +2330,7 @@
     </row>
     <row r="17" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B17" s="3">
         <v>0.2</v>
@@ -2274,7 +2338,7 @@
     </row>
     <row r="18" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B18" s="4">
         <v>0</v>
@@ -2282,7 +2346,7 @@
     </row>
     <row r="19" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B19" s="4">
         <v>0</v>
@@ -2290,12 +2354,12 @@
     </row>
     <row r="20" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B21" s="3">
         <v>0.01</v>
@@ -2303,7 +2367,7 @@
     </row>
     <row r="22" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B22" s="4">
         <v>1000</v>
@@ -2311,7 +2375,7 @@
     </row>
     <row r="23" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B23" s="4">
         <v>1</v>
@@ -2319,7 +2383,7 @@
     </row>
     <row r="24" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B24" s="4">
         <v>1</v>
@@ -2327,7 +2391,7 @@
     </row>
     <row r="25" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B25" s="3">
         <v>0.25</v>
@@ -2335,12 +2399,12 @@
     </row>
     <row r="26" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B27" s="3">
         <v>0.01</v>
@@ -2348,7 +2412,7 @@
     </row>
     <row r="28" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B28" s="4">
         <v>10</v>
@@ -2356,7 +2420,7 @@
     </row>
     <row r="29" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B29" s="4">
         <v>1</v>
@@ -2364,7 +2428,7 @@
     </row>
     <row r="30" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B30" s="4">
         <v>20</v>
@@ -2372,7 +2436,7 @@
     </row>
     <row r="31" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B31" s="3">
         <v>0.25</v>
@@ -2380,7 +2444,7 @@
     </row>
     <row r="32" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B32" s="4">
         <v>100</v>
@@ -2388,12 +2452,12 @@
     </row>
     <row r="33" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B34" s="3">
         <v>1.5</v>
@@ -2401,7 +2465,7 @@
     </row>
     <row r="35" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B35" s="3">
         <v>1.05</v>
@@ -2409,7 +2473,7 @@
     </row>
     <row r="36" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B36" s="3">
         <v>1.004</v>
@@ -2417,7 +2481,7 @@
     </row>
     <row r="37" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B37" s="4">
         <v>1</v>
@@ -2425,7 +2489,7 @@
     </row>
     <row r="38" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B38" s="4">
         <v>10</v>
@@ -2433,7 +2497,7 @@
     </row>
     <row r="39" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B39" s="4">
         <v>12</v>
@@ -2441,7 +2505,7 @@
     </row>
     <row r="40" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B40" s="4">
         <v>100</v>
@@ -2449,7 +2513,7 @@
     </row>
     <row r="41" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B41" s="4">
         <v>60</v>
@@ -2457,7 +2521,7 @@
     </row>
     <row r="42" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B42" s="4">
         <v>100</v>
@@ -2473,21 +2537,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="10" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2498,49 +2564,87 @@
     </row>
     <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="4">
+        <v>201</v>
+      </c>
+      <c r="B3" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="4">
+        <v>204</v>
+      </c>
+      <c r="B5" s="12">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="4">
-        <v>0</v>
+    <row r="6" spans="1:2" s="8" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="B6" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="8" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="B7" s="13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="8" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="B8" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="8" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="B9" s="13"/>
+    </row>
+    <row r="10" spans="1:2" s="8" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="B10" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" s="8" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>203</v>
+      </c>
+      <c r="B13" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="B14" s="11">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2602,7 +2706,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Editing code to implement co2 features
</commit_message>
<xml_diff>
--- a/InitializationData/Simulation_Parameters.xlsx
+++ b/InitializationData/Simulation_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/fce19_ic_ac_uk/Documents/Programming/GithubRepos/Vulcan/InitializationData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="13_ncr:1_{D7B19F01-C027-476C-9166-DE9C897A9ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24E47B77-FFA4-4BBA-AE56-C89490E24AC2}"/>
+  <xr:revisionPtr revIDLastSave="137" documentId="13_ncr:1_{D7B19F01-C027-476C-9166-DE9C897A9ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10C53146-7F5C-4CF6-83DC-683621770A1B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initialization_Parameters" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="218">
   <si>
     <t>sector_name</t>
   </si>
@@ -672,6 +672,24 @@
   </si>
   <si>
     <t>household_rand_emission_weight_change</t>
+  </si>
+  <si>
+    <t>emission_sensitivity_mean</t>
+  </si>
+  <si>
+    <t>emission_sensitivity_min</t>
+  </si>
+  <si>
+    <t>emission_sensitivity_max</t>
+  </si>
+  <si>
+    <t>CO2 Emissions</t>
+  </si>
+  <si>
+    <t>emisssion_sensitivity_std</t>
+  </si>
+  <si>
+    <t>emission_sensitivity_threshold</t>
   </si>
 </sst>
 </file>
@@ -771,11 +789,8 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -789,6 +804,9 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1095,23 +1113,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B136"/>
+  <dimension ref="A1:B141"/>
   <sheetViews>
-    <sheetView topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="A141" sqref="A141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="41.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="13" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1217,7 +1235,7 @@
       <c r="A15" t="s">
         <v>81</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1249,7 +1267,7 @@
       <c r="A19" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1313,7 +1331,7 @@
       <c r="A27" t="s">
         <v>93</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1361,7 +1379,7 @@
       <c r="A33" t="s">
         <v>99</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -1369,7 +1387,7 @@
       <c r="A34" t="s">
         <v>100</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B34" s="3">
         <v>300</v>
       </c>
     </row>
@@ -1377,7 +1395,7 @@
       <c r="A35" t="s">
         <v>101</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1385,7 +1403,7 @@
       <c r="A36" t="s">
         <v>102</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -1393,7 +1411,7 @@
       <c r="A37" t="s">
         <v>103</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37" s="3">
         <v>4</v>
       </c>
     </row>
@@ -1401,7 +1419,7 @@
       <c r="A38" t="s">
         <v>104</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38" s="3">
         <v>2</v>
       </c>
     </row>
@@ -1409,7 +1427,7 @@
       <c r="A39" t="s">
         <v>105</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1417,7 +1435,7 @@
       <c r="A40" t="s">
         <v>106</v>
       </c>
-      <c r="B40" s="4">
+      <c r="B40" s="3">
         <v>100</v>
       </c>
     </row>
@@ -1425,7 +1443,7 @@
       <c r="A41" t="s">
         <v>107</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" s="3">
         <v>950</v>
       </c>
     </row>
@@ -1433,7 +1451,7 @@
       <c r="A42" t="s">
         <v>108</v>
       </c>
-      <c r="B42" s="4">
+      <c r="B42" s="3">
         <v>300</v>
       </c>
     </row>
@@ -1441,7 +1459,7 @@
       <c r="A43" t="s">
         <v>109</v>
       </c>
-      <c r="B43" s="4">
+      <c r="B43" s="3">
         <v>100</v>
       </c>
     </row>
@@ -1449,7 +1467,7 @@
       <c r="A44" t="s">
         <v>110</v>
       </c>
-      <c r="B44" s="4">
+      <c r="B44" s="3">
         <v>999999</v>
       </c>
     </row>
@@ -1457,7 +1475,7 @@
       <c r="A45" t="s">
         <v>111</v>
       </c>
-      <c r="B45" s="4">
+      <c r="B45" s="3">
         <v>500</v>
       </c>
     </row>
@@ -1465,7 +1483,7 @@
       <c r="A46" t="s">
         <v>112</v>
       </c>
-      <c r="B46" s="4">
+      <c r="B46" s="3">
         <v>600</v>
       </c>
     </row>
@@ -1478,7 +1496,7 @@
       <c r="A48" t="s">
         <v>113</v>
       </c>
-      <c r="B48" s="4">
+      <c r="B48" s="3">
         <v>10000</v>
       </c>
     </row>
@@ -1486,7 +1504,7 @@
       <c r="A49" t="s">
         <v>114</v>
       </c>
-      <c r="B49" s="4">
+      <c r="B49" s="3">
         <v>2500</v>
       </c>
     </row>
@@ -1494,7 +1512,7 @@
       <c r="A50" t="s">
         <v>115</v>
       </c>
-      <c r="B50" s="4">
+      <c r="B50" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1502,7 +1520,7 @@
       <c r="A51" t="s">
         <v>116</v>
       </c>
-      <c r="B51" s="4">
+      <c r="B51" s="3">
         <v>999999999</v>
       </c>
     </row>
@@ -1574,7 +1592,7 @@
       <c r="A60" t="s">
         <v>125</v>
       </c>
-      <c r="B60" s="4">
+      <c r="B60" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -1582,7 +1600,7 @@
       <c r="A61" t="s">
         <v>126</v>
       </c>
-      <c r="B61" s="4">
+      <c r="B61" s="3">
         <v>300</v>
       </c>
     </row>
@@ -1590,7 +1608,7 @@
       <c r="A62" t="s">
         <v>127</v>
       </c>
-      <c r="B62" s="4">
+      <c r="B62" s="3">
         <v>100</v>
       </c>
     </row>
@@ -1598,7 +1616,7 @@
       <c r="A63" t="s">
         <v>128</v>
       </c>
-      <c r="B63" s="4">
+      <c r="B63" s="3">
         <v>999999</v>
       </c>
     </row>
@@ -1606,7 +1624,7 @@
       <c r="A64" t="s">
         <v>129</v>
       </c>
-      <c r="B64" s="4">
+      <c r="B64" s="3">
         <v>20</v>
       </c>
     </row>
@@ -1614,7 +1632,7 @@
       <c r="A65" t="s">
         <v>130</v>
       </c>
-      <c r="B65" s="4">
+      <c r="B65" s="3">
         <v>5</v>
       </c>
     </row>
@@ -1622,7 +1640,7 @@
       <c r="A66" t="s">
         <v>131</v>
       </c>
-      <c r="B66" s="4">
+      <c r="B66" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1630,7 +1648,7 @@
       <c r="A67" t="s">
         <v>132</v>
       </c>
-      <c r="B67" s="4">
+      <c r="B67" s="3">
         <v>100</v>
       </c>
     </row>
@@ -1638,7 +1656,7 @@
       <c r="A68" t="s">
         <v>133</v>
       </c>
-      <c r="B68" s="4">
+      <c r="B68" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -1646,7 +1664,7 @@
       <c r="A69" t="s">
         <v>134</v>
       </c>
-      <c r="B69" s="4">
+      <c r="B69" s="3">
         <v>100</v>
       </c>
     </row>
@@ -1654,7 +1672,7 @@
       <c r="A70" t="s">
         <v>135</v>
       </c>
-      <c r="B70" s="4">
+      <c r="B70" s="3">
         <v>100</v>
       </c>
     </row>
@@ -1662,7 +1680,7 @@
       <c r="A71" t="s">
         <v>136</v>
       </c>
-      <c r="B71" s="4">
+      <c r="B71" s="3">
         <v>1999</v>
       </c>
     </row>
@@ -1670,7 +1688,7 @@
       <c r="A72" t="s">
         <v>137</v>
       </c>
-      <c r="B72" s="4">
+      <c r="B72" s="3">
         <v>10</v>
       </c>
     </row>
@@ -1678,7 +1696,7 @@
       <c r="A73" t="s">
         <v>138</v>
       </c>
-      <c r="B73" s="4">
+      <c r="B73" s="3">
         <v>2</v>
       </c>
     </row>
@@ -1686,7 +1704,7 @@
       <c r="A74" t="s">
         <v>139</v>
       </c>
-      <c r="B74" s="4">
+      <c r="B74" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1694,7 +1712,7 @@
       <c r="A75" t="s">
         <v>140</v>
       </c>
-      <c r="B75" s="4">
+      <c r="B75" s="3">
         <v>99</v>
       </c>
     </row>
@@ -1702,7 +1720,7 @@
       <c r="A76" t="s">
         <v>141</v>
       </c>
-      <c r="B76" s="4">
+      <c r="B76" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -1710,7 +1728,7 @@
       <c r="A77" t="s">
         <v>142</v>
       </c>
-      <c r="B77" s="4">
+      <c r="B77" s="3">
         <v>100</v>
       </c>
     </row>
@@ -1718,7 +1736,7 @@
       <c r="A78" t="s">
         <v>143</v>
       </c>
-      <c r="B78" s="4">
+      <c r="B78" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1726,7 +1744,7 @@
       <c r="A79" t="s">
         <v>144</v>
       </c>
-      <c r="B79" s="4">
+      <c r="B79" s="3">
         <v>999999</v>
       </c>
     </row>
@@ -1734,7 +1752,7 @@
       <c r="A80" t="s">
         <v>145</v>
       </c>
-      <c r="B80" s="4">
+      <c r="B80" s="3">
         <v>60</v>
       </c>
     </row>
@@ -1742,7 +1760,7 @@
       <c r="A81" t="s">
         <v>146</v>
       </c>
-      <c r="B81" s="4">
+      <c r="B81" s="3">
         <v>5</v>
       </c>
     </row>
@@ -1750,7 +1768,7 @@
       <c r="A82" t="s">
         <v>147</v>
       </c>
-      <c r="B82" s="4">
+      <c r="B82" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1758,7 +1776,7 @@
       <c r="A83" t="s">
         <v>148</v>
       </c>
-      <c r="B83" s="4">
+      <c r="B83" s="3">
         <v>999999</v>
       </c>
     </row>
@@ -1790,7 +1808,7 @@
       <c r="A87" t="s">
         <v>152</v>
       </c>
-      <c r="B87" s="4">
+      <c r="B87" s="3">
         <v>4</v>
       </c>
     </row>
@@ -1835,7 +1853,7 @@
       <c r="A93" t="s">
         <v>155</v>
       </c>
-      <c r="B93" s="4">
+      <c r="B93" s="3">
         <v>10000</v>
       </c>
     </row>
@@ -1843,7 +1861,7 @@
       <c r="A94" t="s">
         <v>156</v>
       </c>
-      <c r="B94" s="4">
+      <c r="B94" s="3">
         <v>2500</v>
       </c>
     </row>
@@ -1851,7 +1869,7 @@
       <c r="A95" t="s">
         <v>157</v>
       </c>
-      <c r="B95" s="4">
+      <c r="B95" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1859,7 +1877,7 @@
       <c r="A96" t="s">
         <v>158</v>
       </c>
-      <c r="B96" s="4">
+      <c r="B96" s="3">
         <v>999999999</v>
       </c>
     </row>
@@ -1931,7 +1949,7 @@
       <c r="A105" t="s">
         <v>167</v>
       </c>
-      <c r="B105" s="4">
+      <c r="B105" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -1939,7 +1957,7 @@
       <c r="A106" t="s">
         <v>168</v>
       </c>
-      <c r="B106" s="4">
+      <c r="B106" s="3">
         <v>300</v>
       </c>
     </row>
@@ -1947,7 +1965,7 @@
       <c r="A107" t="s">
         <v>169</v>
       </c>
-      <c r="B107" s="4">
+      <c r="B107" s="3">
         <v>100</v>
       </c>
     </row>
@@ -1955,7 +1973,7 @@
       <c r="A108" t="s">
         <v>170</v>
       </c>
-      <c r="B108" s="4">
+      <c r="B108" s="3">
         <v>999999</v>
       </c>
     </row>
@@ -1963,7 +1981,7 @@
       <c r="A109" t="s">
         <v>171</v>
       </c>
-      <c r="B109" s="4">
+      <c r="B109" s="3">
         <v>20</v>
       </c>
     </row>
@@ -1971,7 +1989,7 @@
       <c r="A110" t="s">
         <v>172</v>
       </c>
-      <c r="B110" s="4">
+      <c r="B110" s="3">
         <v>5</v>
       </c>
     </row>
@@ -1979,7 +1997,7 @@
       <c r="A111" t="s">
         <v>173</v>
       </c>
-      <c r="B111" s="4">
+      <c r="B111" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1987,7 +2005,7 @@
       <c r="A112" t="s">
         <v>174</v>
       </c>
-      <c r="B112" s="4">
+      <c r="B112" s="3">
         <v>100</v>
       </c>
     </row>
@@ -1995,7 +2013,7 @@
       <c r="A113" t="s">
         <v>175</v>
       </c>
-      <c r="B113" s="4">
+      <c r="B113" s="3">
         <v>100</v>
       </c>
     </row>
@@ -2003,7 +2021,7 @@
       <c r="A114" t="s">
         <v>176</v>
       </c>
-      <c r="B114" s="4">
+      <c r="B114" s="3">
         <v>10</v>
       </c>
     </row>
@@ -2011,7 +2029,7 @@
       <c r="A115" t="s">
         <v>177</v>
       </c>
-      <c r="B115" s="4">
+      <c r="B115" s="3">
         <v>10</v>
       </c>
     </row>
@@ -2019,7 +2037,7 @@
       <c r="A116" t="s">
         <v>178</v>
       </c>
-      <c r="B116" s="4">
+      <c r="B116" s="3">
         <v>999</v>
       </c>
     </row>
@@ -2027,7 +2045,7 @@
       <c r="A117" t="s">
         <v>179</v>
       </c>
-      <c r="B117" s="4">
+      <c r="B117" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -2035,7 +2053,7 @@
       <c r="A118" t="s">
         <v>180</v>
       </c>
-      <c r="B118" s="4">
+      <c r="B118" s="3">
         <v>200</v>
       </c>
     </row>
@@ -2043,7 +2061,7 @@
       <c r="A119" t="s">
         <v>181</v>
       </c>
-      <c r="B119" s="4">
+      <c r="B119" s="3">
         <v>100</v>
       </c>
     </row>
@@ -2051,7 +2069,7 @@
       <c r="A120" t="s">
         <v>182</v>
       </c>
-      <c r="B120" s="4">
+      <c r="B120" s="3">
         <v>9999</v>
       </c>
     </row>
@@ -2059,7 +2077,7 @@
       <c r="A121" t="s">
         <v>183</v>
       </c>
-      <c r="B121" s="4">
+      <c r="B121" s="3">
         <v>100</v>
       </c>
     </row>
@@ -2067,7 +2085,7 @@
       <c r="A122" t="s">
         <v>184</v>
       </c>
-      <c r="B122" s="4">
+      <c r="B122" s="3">
         <v>10</v>
       </c>
     </row>
@@ -2075,7 +2093,7 @@
       <c r="A123" t="s">
         <v>185</v>
       </c>
-      <c r="B123" s="4">
+      <c r="B123" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2083,7 +2101,7 @@
       <c r="A124" t="s">
         <v>186</v>
       </c>
-      <c r="B124" s="4">
+      <c r="B124" s="3">
         <v>9999</v>
       </c>
     </row>
@@ -2091,7 +2109,7 @@
       <c r="A125" t="s">
         <v>187</v>
       </c>
-      <c r="B125" s="4">
+      <c r="B125" s="3">
         <v>60</v>
       </c>
     </row>
@@ -2099,7 +2117,7 @@
       <c r="A126" t="s">
         <v>188</v>
       </c>
-      <c r="B126" s="4">
+      <c r="B126" s="3">
         <v>5</v>
       </c>
     </row>
@@ -2107,7 +2125,7 @@
       <c r="A127" t="s">
         <v>189</v>
       </c>
-      <c r="B127" s="4">
+      <c r="B127" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2115,7 +2133,7 @@
       <c r="A128" t="s">
         <v>190</v>
       </c>
-      <c r="B128" s="4">
+      <c r="B128" s="3">
         <v>999999</v>
       </c>
     </row>
@@ -2147,7 +2165,7 @@
       <c r="A132" t="s">
         <v>194</v>
       </c>
-      <c r="B132" s="4">
+      <c r="B132" s="3">
         <v>4</v>
       </c>
     </row>
@@ -2171,7 +2189,7 @@
       <c r="A135" t="s">
         <v>197</v>
       </c>
-      <c r="B135" s="4">
+      <c r="B135" s="3">
         <v>100</v>
       </c>
     </row>
@@ -2179,8 +2197,45 @@
       <c r="A136" t="s">
         <v>199</v>
       </c>
-      <c r="B136" s="2">
+      <c r="B136" s="1">
         <v>100</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" s="7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>213</v>
+      </c>
+      <c r="B138" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>214</v>
+      </c>
+      <c r="B139" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>216</v>
+      </c>
+      <c r="B140" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>217</v>
+      </c>
+      <c r="B141" s="1">
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>
@@ -2539,21 +2594,21 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2566,7 +2621,7 @@
       <c r="A3" t="s">
         <v>201</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="11">
         <v>1</v>
       </c>
     </row>
@@ -2579,55 +2634,55 @@
       <c r="A5" t="s">
         <v>204</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="8" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:2" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="B6" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" s="8" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="B6" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="12">
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="8" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:2" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="B8" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" s="8" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="B8" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="B9" s="13"/>
-    </row>
-    <row r="10" spans="1:2" s="8" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="B9" s="12"/>
+    </row>
+    <row r="10" spans="1:2" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="B10" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" s="8" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+      <c r="B10" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="5" t="s">
         <v>202</v>
       </c>
     </row>
@@ -2635,15 +2690,15 @@
       <c r="A13" t="s">
         <v>203</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="10">
         <v>1</v>
       </c>
     </row>
@@ -2657,10 +2712,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2677,7 +2732,7 @@
     <col min="10" max="10" width="16.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2708,8 +2763,11 @@
       <c r="J1" s="2" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K1" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2740,8 +2798,11 @@
       <c r="J2" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K2" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2772,8 +2833,11 @@
       <c r="J3" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K3" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2804,8 +2868,11 @@
       <c r="J4" s="4">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K4" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -2836,8 +2903,11 @@
       <c r="J5" s="4">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K5" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -2868,8 +2938,11 @@
       <c r="J6" s="4">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K6" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2900,8 +2973,11 @@
       <c r="J7" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K7" s="3">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2932,8 +3008,11 @@
       <c r="J8" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K8" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2964,8 +3043,11 @@
       <c r="J9" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K9" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2996,8 +3078,11 @@
       <c r="J10" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K10" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -3028,8 +3113,11 @@
       <c r="J11" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K11" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -3060,8 +3148,11 @@
       <c r="J12" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K12" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -3091,6 +3182,9 @@
       </c>
       <c r="J13" s="4">
         <v>5</v>
+      </c>
+      <c r="K13" s="3">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implementing co2 and optional randomness
</commit_message>
<xml_diff>
--- a/InitializationData/Simulation_Parameters.xlsx
+++ b/InitializationData/Simulation_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/fce19_ic_ac_uk/Documents/Programming/GithubRepos/Vulcan/InitializationData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="137" documentId="13_ncr:1_{D7B19F01-C027-476C-9166-DE9C897A9ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10C53146-7F5C-4CF6-83DC-683621770A1B}"/>
+  <xr:revisionPtr revIDLastSave="250" documentId="13_ncr:1_{D7B19F01-C027-476C-9166-DE9C897A9ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACA683DB-CC7E-461B-AA2D-88FC2F5AC7DF}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initialization_Parameters" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="214">
   <si>
     <t>sector_name</t>
   </si>
@@ -158,12 +158,6 @@
     <t>household_tax_rate</t>
   </si>
   <si>
-    <t>household_p_seek_better_job</t>
-  </si>
-  <si>
-    <t>household_sector_spending_randomization</t>
-  </si>
-  <si>
     <t>standard_employment_contract_length</t>
   </si>
   <si>
@@ -641,36 +635,6 @@
     <t>firm_cons_init_good_price</t>
   </si>
   <si>
-    <t>bank_random_experimentation</t>
-  </si>
-  <si>
-    <t>Firms</t>
-  </si>
-  <si>
-    <t>firm_random_experimentation</t>
-  </si>
-  <si>
-    <t>household_random_experimentation</t>
-  </si>
-  <si>
-    <t>household_majority_sentiment_adoption</t>
-  </si>
-  <si>
-    <t>firm_random_dividend_changes</t>
-  </si>
-  <si>
-    <t>household_rand_spending_weight_change_prob</t>
-  </si>
-  <si>
-    <t>household_rand_spending_weight_change</t>
-  </si>
-  <si>
-    <t>household_majority_sentiment_adoption_prob</t>
-  </si>
-  <si>
-    <t>household_rand_emission_weight_change_prob</t>
-  </si>
-  <si>
     <t>household_rand_emission_weight_change</t>
   </si>
   <si>
@@ -690,6 +654,30 @@
   </si>
   <si>
     <t>emission_sensitivity_threshold</t>
+  </si>
+  <si>
+    <t>household_rand_sentiment_adoption</t>
+  </si>
+  <si>
+    <t>household_rand_sector_spending_weight_change</t>
+  </si>
+  <si>
+    <t>household_rand_job_search</t>
+  </si>
+  <si>
+    <t>firm_cons_rand_sentiment_adoption</t>
+  </si>
+  <si>
+    <t>firm_cap_rand_sentiment_adoption</t>
+  </si>
+  <si>
+    <t>firm_cons_rand_dividend_change</t>
+  </si>
+  <si>
+    <t>firm_cap_rand_desired_inventory_factor_change</t>
+  </si>
+  <si>
+    <t>firm_cons_rand_desired_inventory_factor_change</t>
   </si>
 </sst>
 </file>
@@ -699,7 +687,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -727,13 +715,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -769,7 +750,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -790,7 +771,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -799,14 +780,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1115,8 +1093,8 @@
   </sheetPr>
   <dimension ref="A1:B141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="A141" sqref="A141"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1127,9 +1105,9 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1140,7 +1118,7 @@
     </row>
     <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B3" s="3">
         <v>0.02</v>
@@ -1153,7 +1131,7 @@
     </row>
     <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B5" s="3">
         <v>0.15</v>
@@ -1161,7 +1139,7 @@
     </row>
     <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B6" s="3">
         <v>0.1</v>
@@ -1169,7 +1147,7 @@
     </row>
     <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7" s="3">
         <v>0.9</v>
@@ -1177,7 +1155,7 @@
     </row>
     <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B8" s="3">
         <v>0.5</v>
@@ -1185,7 +1163,7 @@
     </row>
     <row r="9" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B9" s="3">
         <v>0.5</v>
@@ -1193,7 +1171,7 @@
     </row>
     <row r="10" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B10" s="3">
         <v>0.1</v>
@@ -1201,7 +1179,7 @@
     </row>
     <row r="11" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B11" s="3">
         <v>0.1</v>
@@ -1209,7 +1187,7 @@
     </row>
     <row r="12" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B12" s="3">
         <v>0.9</v>
@@ -1217,7 +1195,7 @@
     </row>
     <row r="13" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B13" s="3">
         <v>0.2</v>
@@ -1225,7 +1203,7 @@
     </row>
     <row r="14" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B14" s="3">
         <v>0.05</v>
@@ -1233,7 +1211,7 @@
     </row>
     <row r="15" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B15" s="3">
         <v>0</v>
@@ -1241,7 +1219,7 @@
     </row>
     <row r="16" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B16" s="3">
         <v>0.4</v>
@@ -1249,7 +1227,7 @@
     </row>
     <row r="17" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B17" s="3">
         <v>0.3</v>
@@ -1257,7 +1235,7 @@
     </row>
     <row r="18" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B18" s="3">
         <v>0.05</v>
@@ -1265,7 +1243,7 @@
     </row>
     <row r="19" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B19" s="3">
         <v>0</v>
@@ -1273,7 +1251,7 @@
     </row>
     <row r="20" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B20" s="3">
         <v>0.7</v>
@@ -1281,7 +1259,7 @@
     </row>
     <row r="21" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B21" s="3">
         <v>0.25</v>
@@ -1289,7 +1267,7 @@
     </row>
     <row r="22" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B22" s="3">
         <v>0.2</v>
@@ -1297,7 +1275,7 @@
     </row>
     <row r="23" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B23" s="3">
         <v>0.01</v>
@@ -1305,7 +1283,7 @@
     </row>
     <row r="24" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B24" s="3">
         <v>0.99</v>
@@ -1313,7 +1291,7 @@
     </row>
     <row r="25" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B25" s="3">
         <v>0.2</v>
@@ -1321,7 +1299,7 @@
     </row>
     <row r="26" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B26" s="3">
         <v>0.05</v>
@@ -1329,7 +1307,7 @@
     </row>
     <row r="27" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B27" s="3">
         <v>0</v>
@@ -1337,7 +1315,7 @@
     </row>
     <row r="28" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B28" s="3">
         <v>0.5</v>
@@ -1345,7 +1323,7 @@
     </row>
     <row r="29" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B29" s="3">
         <v>0.3</v>
@@ -1353,7 +1331,7 @@
     </row>
     <row r="30" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B30" s="3">
         <v>0.05</v>
@@ -1361,7 +1339,7 @@
     </row>
     <row r="31" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B31" s="3">
         <v>0.1</v>
@@ -1369,7 +1347,7 @@
     </row>
     <row r="32" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B32" s="3">
         <v>0.6</v>
@@ -1377,7 +1355,7 @@
     </row>
     <row r="33" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B33" s="3">
         <v>1000</v>
@@ -1385,7 +1363,7 @@
     </row>
     <row r="34" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B34" s="3">
         <v>300</v>
@@ -1393,7 +1371,7 @@
     </row>
     <row r="35" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B35" s="3">
         <v>0</v>
@@ -1401,7 +1379,7 @@
     </row>
     <row r="36" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B36" s="3">
         <v>2000</v>
@@ -1409,7 +1387,7 @@
     </row>
     <row r="37" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B37" s="3">
         <v>4</v>
@@ -1417,7 +1395,7 @@
     </row>
     <row r="38" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B38" s="3">
         <v>2</v>
@@ -1425,7 +1403,7 @@
     </row>
     <row r="39" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B39" s="3">
         <v>0</v>
@@ -1433,7 +1411,7 @@
     </row>
     <row r="40" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B40" s="3">
         <v>100</v>
@@ -1441,7 +1419,7 @@
     </row>
     <row r="41" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B41" s="3">
         <v>950</v>
@@ -1449,7 +1427,7 @@
     </row>
     <row r="42" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B42" s="3">
         <v>300</v>
@@ -1457,7 +1435,7 @@
     </row>
     <row r="43" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B43" s="3">
         <v>100</v>
@@ -1465,7 +1443,7 @@
     </row>
     <row r="44" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B44" s="3">
         <v>999999</v>
@@ -1473,7 +1451,7 @@
     </row>
     <row r="45" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B45" s="3">
         <v>500</v>
@@ -1481,7 +1459,7 @@
     </row>
     <row r="46" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B46" s="3">
         <v>600</v>
@@ -1494,7 +1472,7 @@
     </row>
     <row r="48" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B48" s="3">
         <v>10000</v>
@@ -1502,7 +1480,7 @@
     </row>
     <row r="49" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B49" s="3">
         <v>2500</v>
@@ -1510,7 +1488,7 @@
     </row>
     <row r="50" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B50" s="3">
         <v>1</v>
@@ -1518,7 +1496,7 @@
     </row>
     <row r="51" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B51" s="3">
         <v>999999999</v>
@@ -1526,7 +1504,7 @@
     </row>
     <row r="52" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B52" s="3">
         <v>0.05</v>
@@ -1534,7 +1512,7 @@
     </row>
     <row r="53" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B53" s="3">
         <v>0.02</v>
@@ -1542,7 +1520,7 @@
     </row>
     <row r="54" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B54" s="3">
         <v>5.0000000000000001E-3</v>
@@ -1550,7 +1528,7 @@
     </row>
     <row r="55" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B55" s="3">
         <v>0.2</v>
@@ -1558,7 +1536,7 @@
     </row>
     <row r="56" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B56" s="3">
         <v>0.03</v>
@@ -1566,7 +1544,7 @@
     </row>
     <row r="57" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B57" s="3">
         <v>0.02</v>
@@ -1574,7 +1552,7 @@
     </row>
     <row r="58" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B58" s="3">
         <v>1E-3</v>
@@ -1582,7 +1560,7 @@
     </row>
     <row r="59" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B59" s="3">
         <v>0.15</v>
@@ -1590,7 +1568,7 @@
     </row>
     <row r="60" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B60" s="3">
         <v>1000</v>
@@ -1598,7 +1576,7 @@
     </row>
     <row r="61" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B61" s="3">
         <v>300</v>
@@ -1606,7 +1584,7 @@
     </row>
     <row r="62" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B62" s="3">
         <v>100</v>
@@ -1614,7 +1592,7 @@
     </row>
     <row r="63" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B63" s="3">
         <v>999999</v>
@@ -1622,7 +1600,7 @@
     </row>
     <row r="64" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B64" s="3">
         <v>20</v>
@@ -1630,7 +1608,7 @@
     </row>
     <row r="65" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B65" s="3">
         <v>5</v>
@@ -1638,7 +1616,7 @@
     </row>
     <row r="66" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B66" s="3">
         <v>1</v>
@@ -1646,7 +1624,7 @@
     </row>
     <row r="67" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B67" s="3">
         <v>100</v>
@@ -1654,7 +1632,7 @@
     </row>
     <row r="68" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B68" s="3">
         <v>1000</v>
@@ -1662,7 +1640,7 @@
     </row>
     <row r="69" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B69" s="3">
         <v>100</v>
@@ -1670,7 +1648,7 @@
     </row>
     <row r="70" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B70" s="3">
         <v>100</v>
@@ -1678,7 +1656,7 @@
     </row>
     <row r="71" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B71" s="3">
         <v>1999</v>
@@ -1686,7 +1664,7 @@
     </row>
     <row r="72" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B72" s="3">
         <v>10</v>
@@ -1694,7 +1672,7 @@
     </row>
     <row r="73" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B73" s="3">
         <v>2</v>
@@ -1702,7 +1680,7 @@
     </row>
     <row r="74" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B74" s="3">
         <v>1</v>
@@ -1710,7 +1688,7 @@
     </row>
     <row r="75" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B75" s="3">
         <v>99</v>
@@ -1718,7 +1696,7 @@
     </row>
     <row r="76" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B76" s="3">
         <v>1000</v>
@@ -1726,7 +1704,7 @@
     </row>
     <row r="77" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B77" s="3">
         <v>100</v>
@@ -1734,7 +1712,7 @@
     </row>
     <row r="78" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B78" s="3">
         <v>1</v>
@@ -1742,7 +1720,7 @@
     </row>
     <row r="79" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B79" s="3">
         <v>999999</v>
@@ -1750,7 +1728,7 @@
     </row>
     <row r="80" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B80" s="3">
         <v>60</v>
@@ -1758,7 +1736,7 @@
     </row>
     <row r="81" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B81" s="3">
         <v>5</v>
@@ -1766,7 +1744,7 @@
     </row>
     <row r="82" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B82" s="3">
         <v>1</v>
@@ -1774,7 +1752,7 @@
     </row>
     <row r="83" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B83" s="3">
         <v>999999</v>
@@ -1782,7 +1760,7 @@
     </row>
     <row r="84" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B84" s="3">
         <v>1.5</v>
@@ -1790,7 +1768,7 @@
     </row>
     <row r="85" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B85" s="3">
         <v>0.25</v>
@@ -1798,7 +1776,7 @@
     </row>
     <row r="86" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B86" s="3">
         <v>0.1</v>
@@ -1806,7 +1784,7 @@
     </row>
     <row r="87" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B87" s="3">
         <v>4</v>
@@ -1814,7 +1792,7 @@
     </row>
     <row r="88" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B88" s="3">
         <v>0.4</v>
@@ -1822,7 +1800,7 @@
     </row>
     <row r="89" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B89" s="3">
         <v>0.25</v>
@@ -1830,7 +1808,7 @@
     </row>
     <row r="90" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B90" s="3">
         <v>9.5</v>
@@ -1838,7 +1816,7 @@
     </row>
     <row r="91" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B91" s="3">
         <v>10</v>
@@ -1851,7 +1829,7 @@
     </row>
     <row r="93" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B93" s="3">
         <v>10000</v>
@@ -1859,7 +1837,7 @@
     </row>
     <row r="94" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B94" s="3">
         <v>2500</v>
@@ -1867,7 +1845,7 @@
     </row>
     <row r="95" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B95" s="3">
         <v>1</v>
@@ -1875,7 +1853,7 @@
     </row>
     <row r="96" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B96" s="3">
         <v>999999999</v>
@@ -1883,7 +1861,7 @@
     </row>
     <row r="97" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B97" s="3">
         <v>0.05</v>
@@ -1891,7 +1869,7 @@
     </row>
     <row r="98" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B98" s="3">
         <v>0.02</v>
@@ -1899,7 +1877,7 @@
     </row>
     <row r="99" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B99" s="3">
         <v>5.0000000000000001E-3</v>
@@ -1907,7 +1885,7 @@
     </row>
     <row r="100" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B100" s="3">
         <v>0.2</v>
@@ -1915,7 +1893,7 @@
     </row>
     <row r="101" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B101" s="3">
         <v>0.03</v>
@@ -1923,7 +1901,7 @@
     </row>
     <row r="102" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B102" s="3">
         <v>0.02</v>
@@ -1931,7 +1909,7 @@
     </row>
     <row r="103" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B103" s="3">
         <v>1E-3</v>
@@ -1939,7 +1917,7 @@
     </row>
     <row r="104" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B104" s="3">
         <v>0.15</v>
@@ -1947,7 +1925,7 @@
     </row>
     <row r="105" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B105" s="3">
         <v>1000</v>
@@ -1955,7 +1933,7 @@
     </row>
     <row r="106" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B106" s="3">
         <v>300</v>
@@ -1963,7 +1941,7 @@
     </row>
     <row r="107" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B107" s="3">
         <v>100</v>
@@ -1971,7 +1949,7 @@
     </row>
     <row r="108" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B108" s="3">
         <v>999999</v>
@@ -1979,7 +1957,7 @@
     </row>
     <row r="109" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B109" s="3">
         <v>20</v>
@@ -1987,7 +1965,7 @@
     </row>
     <row r="110" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B110" s="3">
         <v>5</v>
@@ -1995,7 +1973,7 @@
     </row>
     <row r="111" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B111" s="3">
         <v>1</v>
@@ -2003,7 +1981,7 @@
     </row>
     <row r="112" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B112" s="3">
         <v>100</v>
@@ -2011,7 +1989,7 @@
     </row>
     <row r="113" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B113" s="3">
         <v>100</v>
@@ -2019,7 +1997,7 @@
     </row>
     <row r="114" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B114" s="3">
         <v>10</v>
@@ -2027,7 +2005,7 @@
     </row>
     <row r="115" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B115" s="3">
         <v>10</v>
@@ -2035,7 +2013,7 @@
     </row>
     <row r="116" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B116" s="3">
         <v>999</v>
@@ -2043,7 +2021,7 @@
     </row>
     <row r="117" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B117" s="3">
         <v>1000</v>
@@ -2051,7 +2029,7 @@
     </row>
     <row r="118" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B118" s="3">
         <v>200</v>
@@ -2059,7 +2037,7 @@
     </row>
     <row r="119" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B119" s="3">
         <v>100</v>
@@ -2067,7 +2045,7 @@
     </row>
     <row r="120" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B120" s="3">
         <v>9999</v>
@@ -2075,7 +2053,7 @@
     </row>
     <row r="121" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B121" s="3">
         <v>100</v>
@@ -2083,7 +2061,7 @@
     </row>
     <row r="122" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B122" s="3">
         <v>10</v>
@@ -2091,7 +2069,7 @@
     </row>
     <row r="123" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B123" s="3">
         <v>1</v>
@@ -2099,7 +2077,7 @@
     </row>
     <row r="124" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B124" s="3">
         <v>9999</v>
@@ -2107,7 +2085,7 @@
     </row>
     <row r="125" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B125" s="3">
         <v>60</v>
@@ -2115,7 +2093,7 @@
     </row>
     <row r="126" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B126" s="3">
         <v>5</v>
@@ -2123,7 +2101,7 @@
     </row>
     <row r="127" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B127" s="3">
         <v>1</v>
@@ -2131,7 +2109,7 @@
     </row>
     <row r="128" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B128" s="3">
         <v>999999</v>
@@ -2139,7 +2117,7 @@
     </row>
     <row r="129" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B129" s="3">
         <v>1.5</v>
@@ -2147,7 +2125,7 @@
     </row>
     <row r="130" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B130" s="3">
         <v>0.25</v>
@@ -2155,7 +2133,7 @@
     </row>
     <row r="131" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B131" s="3">
         <v>0.1</v>
@@ -2163,7 +2141,7 @@
     </row>
     <row r="132" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B132" s="3">
         <v>4</v>
@@ -2171,7 +2149,7 @@
     </row>
     <row r="133" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B133" s="3">
         <v>0.4</v>
@@ -2179,7 +2157,7 @@
     </row>
     <row r="134" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B134" s="3">
         <v>0.25</v>
@@ -2187,7 +2165,7 @@
     </row>
     <row r="135" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B135" s="3">
         <v>100</v>
@@ -2195,7 +2173,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B136" s="1">
         <v>100</v>
@@ -2203,12 +2181,12 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" s="7" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="B138" s="1">
         <v>0</v>
@@ -2216,7 +2194,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="B139" s="1">
         <v>0.5</v>
@@ -2224,7 +2202,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="B140" s="1">
         <v>0.1</v>
@@ -2232,7 +2210,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="B141" s="1">
         <v>0.05</v>
@@ -2248,10 +2226,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2363,8 +2341,8 @@
       <c r="A14" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="3">
-        <v>0.1</v>
+      <c r="B14" s="4">
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2372,7 +2350,7 @@
         <v>41</v>
       </c>
       <c r="B15" s="3">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2380,44 +2358,44 @@
         <v>42</v>
       </c>
       <c r="B16" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="3">
-        <v>0.2</v>
+      <c r="B17" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="B18" s="4">
-        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="4">
-        <v>0</v>
+      <c r="B19" s="3">
+        <v>0.01</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+      <c r="A20" t="s">
         <v>46</v>
+      </c>
+      <c r="B20" s="4">
+        <v>1000</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="3">
-        <v>0.01</v>
+      <c r="B21" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2425,23 +2403,20 @@
         <v>48</v>
       </c>
       <c r="B22" s="4">
-        <v>1000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="4">
-        <v>1</v>
+      <c r="B23" s="3">
+        <v>0.25</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="B24" s="4">
-        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2449,20 +2424,23 @@
         <v>51</v>
       </c>
       <c r="B25" s="3">
-        <v>0.25</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
+      <c r="A26" t="s">
         <v>52</v>
+      </c>
+      <c r="B26" s="4">
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>53</v>
       </c>
-      <c r="B27" s="3">
-        <v>0.01</v>
+      <c r="B27" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2470,15 +2448,15 @@
         <v>54</v>
       </c>
       <c r="B28" s="4">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="4">
-        <v>1</v>
+      <c r="B29" s="3">
+        <v>0.25</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2486,28 +2464,28 @@
         <v>56</v>
       </c>
       <c r="B30" s="4">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="A31" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="B31" s="3">
-        <v>0.25</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>58</v>
       </c>
-      <c r="B32" s="4">
-        <v>100</v>
+      <c r="B32" s="3">
+        <v>1.5</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="5" t="s">
+      <c r="A33" t="s">
         <v>59</v>
+      </c>
+      <c r="B33" s="3">
+        <v>1.05</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2515,23 +2493,23 @@
         <v>60</v>
       </c>
       <c r="B34" s="3">
-        <v>1.5</v>
+        <v>1.004</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>61</v>
       </c>
-      <c r="B35" s="3">
-        <v>1.05</v>
+      <c r="B35" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>62</v>
       </c>
-      <c r="B36" s="3">
-        <v>1.004</v>
+      <c r="B36" s="4">
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2539,7 +2517,7 @@
         <v>63</v>
       </c>
       <c r="B37" s="4">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2547,7 +2525,7 @@
         <v>64</v>
       </c>
       <c r="B38" s="4">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2555,7 +2533,7 @@
         <v>65</v>
       </c>
       <c r="B39" s="4">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2563,23 +2541,7 @@
         <v>66</v>
       </c>
       <c r="B40" s="4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>67</v>
-      </c>
-      <c r="B41" s="4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>68</v>
-      </c>
-      <c r="B42" s="4">
-        <v>100</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2594,13 +2556,13 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.109375" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2614,92 +2576,98 @@
     </row>
     <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>201</v>
-      </c>
-      <c r="B3" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>204</v>
-      </c>
-      <c r="B5" s="11">
-        <v>2</v>
+      <c r="B2" s="12"/>
+    </row>
+    <row r="3" spans="1:2" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="B3" s="10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="B4" s="10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="B5" s="10">
+        <v>0.1</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="B6" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="B6" s="10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B8" s="10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="B7" s="12">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="B8" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B9" s="12"/>
-    </row>
-    <row r="10" spans="1:2" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B10" s="10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="B10" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+      <c r="B12" s="10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>203</v>
-      </c>
       <c r="B13" s="10">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="B14" s="10">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
@@ -2761,10 +2729,10 @@
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Emission penalties in lending to firms
</commit_message>
<xml_diff>
--- a/InitializationData/Simulation_Parameters.xlsx
+++ b/InitializationData/Simulation_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/fce19_ic_ac_uk/Documents/Programming/GithubRepos/Vulcan/InitializationData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="250" documentId="13_ncr:1_{D7B19F01-C027-476C-9166-DE9C897A9ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACA683DB-CC7E-461B-AA2D-88FC2F5AC7DF}"/>
+  <xr:revisionPtr revIDLastSave="280" documentId="13_ncr:1_{D7B19F01-C027-476C-9166-DE9C897A9ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9781D367-BC22-471E-AB94-8D0D41823739}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initialization_Parameters" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="222">
   <si>
     <t>sector_name</t>
   </si>
@@ -678,6 +678,30 @@
   </si>
   <si>
     <t>firm_cons_rand_desired_inventory_factor_change</t>
+  </si>
+  <si>
+    <t>bank_total_emission_penalty</t>
+  </si>
+  <si>
+    <t>bank_unit_emission_penalty</t>
+  </si>
+  <si>
+    <t>bank_unit_emission_lower_thr</t>
+  </si>
+  <si>
+    <t>bank_total_emission_lower_thr</t>
+  </si>
+  <si>
+    <t>bank_total_emission_upper_thr</t>
+  </si>
+  <si>
+    <t>bank_emission_penalty_max</t>
+  </si>
+  <si>
+    <t>Bank Emission Penalty Parameters</t>
+  </si>
+  <si>
+    <t>bank_unit_emission_upper_thr</t>
   </si>
 </sst>
 </file>
@@ -750,7 +774,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -767,9 +791,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -782,9 +803,6 @@
     </xf>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1107,7 +1125,7 @@
       <c r="A1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2180,7 +2198,7 @@
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A137" s="7" t="s">
+      <c r="A137" s="6" t="s">
         <v>203</v>
       </c>
     </row>
@@ -2226,23 +2244,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="39.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="10" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2255,7 +2273,7 @@
       <c r="A3" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>60</v>
       </c>
     </row>
@@ -2263,7 +2281,7 @@
       <c r="A4" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>10000</v>
       </c>
     </row>
@@ -2271,7 +2289,7 @@
       <c r="A5" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>400</v>
       </c>
     </row>
@@ -2279,7 +2297,7 @@
       <c r="A6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>50</v>
       </c>
     </row>
@@ -2287,7 +2305,7 @@
       <c r="A7" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <f>B5+B6</f>
         <v>450</v>
       </c>
@@ -2296,7 +2314,7 @@
       <c r="A8" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>100</v>
       </c>
     </row>
@@ -2304,7 +2322,7 @@
       <c r="A9" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>12</v>
       </c>
     </row>
@@ -2325,7 +2343,7 @@
       <c r="A12" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>3</v>
       </c>
     </row>
@@ -2341,7 +2359,7 @@
       <c r="A14" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>6</v>
       </c>
     </row>
@@ -2357,7 +2375,7 @@
       <c r="A16" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>0</v>
       </c>
     </row>
@@ -2365,7 +2383,7 @@
       <c r="A17" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <v>0</v>
       </c>
     </row>
@@ -2386,7 +2404,7 @@
       <c r="A20" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -2394,7 +2412,7 @@
       <c r="A21" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2402,7 +2420,7 @@
       <c r="A22" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2431,7 +2449,7 @@
       <c r="A26" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="3">
         <v>10</v>
       </c>
     </row>
@@ -2439,7 +2457,7 @@
       <c r="A27" t="s">
         <v>53</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2447,7 +2465,7 @@
       <c r="A28" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="3">
         <v>20</v>
       </c>
     </row>
@@ -2463,7 +2481,7 @@
       <c r="A30" t="s">
         <v>56</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="3">
         <v>100</v>
       </c>
     </row>
@@ -2500,7 +2518,7 @@
       <c r="A35" t="s">
         <v>61</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2508,7 +2526,7 @@
       <c r="A36" t="s">
         <v>62</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36" s="3">
         <v>10</v>
       </c>
     </row>
@@ -2516,7 +2534,7 @@
       <c r="A37" t="s">
         <v>63</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37" s="3">
         <v>12</v>
       </c>
     </row>
@@ -2524,7 +2542,7 @@
       <c r="A38" t="s">
         <v>64</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38" s="3">
         <v>100</v>
       </c>
     </row>
@@ -2532,7 +2550,7 @@
       <c r="A39" t="s">
         <v>65</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" s="3">
         <v>5</v>
       </c>
     </row>
@@ -2540,8 +2558,69 @@
       <c r="A40" t="s">
         <v>66</v>
       </c>
-      <c r="B40" s="4">
+      <c r="B40" s="3">
         <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>219</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>214</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>215</v>
+      </c>
+      <c r="B44" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>216</v>
+      </c>
+      <c r="B45" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>221</v>
+      </c>
+      <c r="B46" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>217</v>
+      </c>
+      <c r="B47" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>218</v>
+      </c>
+      <c r="B48" s="1">
+        <v>100000</v>
       </c>
     </row>
   </sheetData>
@@ -2556,21 +2635,21 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2578,37 +2657,36 @@
       <c r="A2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="12"/>
-    </row>
-    <row r="3" spans="1:2" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+    </row>
+    <row r="3" spans="1:2" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="B3" s="10">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="B3" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="B4" s="10">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="B4" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="B5" s="10">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="B5" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>0.1</v>
       </c>
     </row>
@@ -2618,26 +2696,26 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="9">
         <v>0.1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <v>0.1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="9">
         <v>0.1</v>
       </c>
     </row>
@@ -2647,26 +2725,26 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="9">
         <v>0.1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="9">
         <v>0.1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="9">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Variable production and price changes
</commit_message>
<xml_diff>
--- a/InitializationData/Simulation_Parameters.xlsx
+++ b/InitializationData/Simulation_Parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/fce19_ic_ac_uk/Documents/Programming/GithubRepos/Vulcan/InitializationData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feyzi\OneDrive - Imperial College London\Programming\GithubRepos\Vulcan\InitializationData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="310" documentId="13_ncr:1_{D7B19F01-C027-476C-9166-DE9C897A9ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37AB0C4D-9BDD-45FD-82CB-B13335A412DD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F933D5F-C214-4534-8E09-0CD1AB54C2D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initialization_Parameters" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="233">
   <si>
     <t>sector_name</t>
   </si>
@@ -635,9 +635,6 @@
     <t>firm_cons_init_good_price</t>
   </si>
   <si>
-    <t>household_rand_emission_weight_change</t>
-  </si>
-  <si>
     <t>emission_sensitivity_mean</t>
   </si>
   <si>
@@ -723,6 +720,21 @@
   </si>
   <si>
     <t>emission_allowance</t>
+  </si>
+  <si>
+    <t>household_rand_emission_sensitivity_change</t>
+  </si>
+  <si>
+    <t>firm_cons_fixed_price_change</t>
+  </si>
+  <si>
+    <t>firm_cons_rand_price_change_upper_limit</t>
+  </si>
+  <si>
+    <t>firm_cons_fixed_prod_change</t>
+  </si>
+  <si>
+    <t>firm_cons_rand_prod_change_upper_limit</t>
   </si>
 </sst>
 </file>
@@ -796,7 +808,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -833,9 +845,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -2233,12 +2242,12 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B138" s="1">
         <v>0</v>
@@ -2246,7 +2255,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B139" s="1">
         <v>0.5</v>
@@ -2254,7 +2263,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B140" s="1">
         <v>0.1</v>
@@ -2262,7 +2271,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B141" s="1">
         <v>0.05</v>
@@ -2270,12 +2279,12 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B143" s="12">
         <v>1000000</v>
@@ -2283,7 +2292,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B144" s="12">
         <v>0.5</v>
@@ -2301,8 +2310,8 @@
   </sheetPr>
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2619,12 +2628,12 @@
     </row>
     <row r="41" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B42" s="12">
         <v>0.02</v>
@@ -2632,7 +2641,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B43" s="12">
         <v>0.02</v>
@@ -2640,7 +2649,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B44" s="12">
         <v>1</v>
@@ -2648,7 +2657,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B45" s="12">
         <v>1</v>
@@ -2656,7 +2665,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B46" s="12">
         <v>10</v>
@@ -2664,7 +2673,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B47" s="12">
         <v>1000</v>
@@ -2672,7 +2681,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B48" s="12">
         <v>100000</v>
@@ -2680,12 +2689,12 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B50" s="12">
         <v>-1E-3</v>
@@ -2693,7 +2702,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B51" s="12">
         <v>1E-3</v>
@@ -2709,10 +2718,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2736,7 +2745,7 @@
     </row>
     <row r="3" spans="1:2" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B3" s="9">
         <v>0.1</v>
@@ -2744,7 +2753,7 @@
     </row>
     <row r="4" spans="1:2" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B4" s="9">
         <v>0.1</v>
@@ -2752,7 +2761,7 @@
     </row>
     <row r="5" spans="1:2" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>199</v>
+        <v>228</v>
       </c>
       <c r="B5" s="9">
         <v>0.1</v>
@@ -2760,7 +2769,7 @@
     </row>
     <row r="6" spans="1:2" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B6" s="9">
         <v>0.1</v>
@@ -2773,7 +2782,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B8" s="9">
         <v>0.1</v>
@@ -2781,7 +2790,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B9" s="9">
         <v>0.1</v>
@@ -2789,39 +2798,103 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B10" s="9">
         <v>0.1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>26</v>
+      <c r="A11" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="B11" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="B12" s="9">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>209</v>
+        <v>231</v>
       </c>
       <c r="B13" s="9">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>211</v>
+        <v>232</v>
       </c>
       <c r="B14" s="9">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="B16" s="9">
         <v>0.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="B17" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B18" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="B19" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B20" s="9">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B21" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="B22" s="9">
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>
@@ -2836,8 +2909,8 @@
   </sheetPr>
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2886,10 +2959,10 @@
         <v>196</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2926,7 +2999,7 @@
       <c r="K2" s="3">
         <v>0.1</v>
       </c>
-      <c r="L2" s="14">
+      <c r="L2" s="4">
         <v>96000</v>
       </c>
     </row>
@@ -2964,7 +3037,7 @@
       <c r="K3" s="3">
         <v>0.1</v>
       </c>
-      <c r="L3" s="14">
+      <c r="L3" s="4">
         <v>35000</v>
       </c>
     </row>
@@ -3002,7 +3075,7 @@
       <c r="K4" s="3">
         <v>0.2</v>
       </c>
-      <c r="L4" s="14">
+      <c r="L4" s="4">
         <v>48000</v>
       </c>
     </row>
@@ -3040,7 +3113,7 @@
       <c r="K5" s="3">
         <v>0.3</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="4">
         <v>303000</v>
       </c>
     </row>
@@ -3078,7 +3151,7 @@
       <c r="K6" s="3">
         <v>0.2</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="4">
         <v>56000</v>
       </c>
     </row>
@@ -3116,7 +3189,7 @@
       <c r="K7" s="3">
         <v>0.15</v>
       </c>
-      <c r="L7" s="14">
+      <c r="L7" s="4">
         <v>18000</v>
       </c>
     </row>
@@ -3154,7 +3227,7 @@
       <c r="K8" s="3">
         <v>0.2</v>
       </c>
-      <c r="L8" s="14">
+      <c r="L8" s="4">
         <v>111000</v>
       </c>
     </row>
@@ -3192,7 +3265,7 @@
       <c r="K9" s="3">
         <v>0.3</v>
       </c>
-      <c r="L9" s="14">
+      <c r="L9" s="4">
         <v>19000</v>
       </c>
     </row>
@@ -3230,7 +3303,7 @@
       <c r="K10" s="3">
         <v>0.1</v>
       </c>
-      <c r="L10" s="14">
+      <c r="L10" s="4">
         <v>112000</v>
       </c>
     </row>
@@ -3268,7 +3341,7 @@
       <c r="K11" s="3">
         <v>0.2</v>
       </c>
-      <c r="L11" s="14">
+      <c r="L11" s="4">
         <v>23000</v>
       </c>
     </row>
@@ -3306,7 +3379,7 @@
       <c r="K12" s="3">
         <v>0.1</v>
       </c>
-      <c r="L12" s="14">
+      <c r="L12" s="4">
         <v>112000</v>
       </c>
     </row>
@@ -3344,7 +3417,7 @@
       <c r="K13" s="3">
         <v>0.1</v>
       </c>
-      <c r="L13" s="14">
+      <c r="L13" s="4">
         <v>67000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Misc changes to fix bugs and clean up code
</commit_message>
<xml_diff>
--- a/InitializationData/Simulation_Parameters.xlsx
+++ b/InitializationData/Simulation_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/fce19_ic_ac_uk/Documents/Programming/GithubRepos/Vulcan/InitializationData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{6F933D5F-C214-4534-8E09-0CD1AB54C2D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1CC4707F-DB73-488B-BB05-4CDEDB54617E}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{6F933D5F-C214-4534-8E09-0CD1AB54C2D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D962E19-BF9D-4F0B-AF69-791B930A09F1}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initialization_Parameters" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="231">
   <si>
     <t>sector_name</t>
   </si>
@@ -443,18 +443,6 @@
     <t>firm_cons_init_production_planned_max</t>
   </si>
   <si>
-    <t>firm_cons_init_good_price_current_mean</t>
-  </si>
-  <si>
-    <t>firm_cons_init_good_price_current_std</t>
-  </si>
-  <si>
-    <t>firm_cons_init_good_price_current_min</t>
-  </si>
-  <si>
-    <t>firm_cons_init_good_price_current_max</t>
-  </si>
-  <si>
     <t>firm_cons_init_inventory_mean</t>
   </si>
   <si>
@@ -569,18 +557,6 @@
     <t>firm_cap_init_production_planned_max</t>
   </si>
   <si>
-    <t>firm_cap_init_good_price_current_mean</t>
-  </si>
-  <si>
-    <t>firm_cap_init_good_price_current_std</t>
-  </si>
-  <si>
-    <t>firm_cap_init_good_price_current_min</t>
-  </si>
-  <si>
-    <t>firm_cap_init_good_price_current_max</t>
-  </si>
-  <si>
     <t>firm_cap_init_inventory_mean</t>
   </si>
   <si>
@@ -623,18 +599,12 @@
     <t>firm_cap_init_quantity_sold_ratio</t>
   </si>
   <si>
-    <t>firm_cap_init_good_price</t>
-  </si>
-  <si>
     <t>emissions_per_unit</t>
   </si>
   <si>
     <t>firm_cap_init_emissions_per_unit</t>
   </si>
   <si>
-    <t>firm_cons_init_good_price</t>
-  </si>
-  <si>
     <t>emission_sensitivity_mean</t>
   </si>
   <si>
@@ -735,6 +705,30 @@
   </si>
   <si>
     <t>firm_cons_rand_prod_change_upper_limit</t>
+  </si>
+  <si>
+    <t>firm_cap_init_good_price_mean</t>
+  </si>
+  <si>
+    <t>firm_cap_init_good_price_std</t>
+  </si>
+  <si>
+    <t>firm_cap_init_good_price_min</t>
+  </si>
+  <si>
+    <t>firm_cap_init_good_price_max</t>
+  </si>
+  <si>
+    <t>firm_cons_init_good_price_mean</t>
+  </si>
+  <si>
+    <t>firm_cons_init_good_price_std</t>
+  </si>
+  <si>
+    <t>firm_cons_init_good_price_min</t>
+  </si>
+  <si>
+    <t>firm_cons_init_good_price_max</t>
   </si>
 </sst>
 </file>
@@ -1152,10 +1146,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B144"/>
+  <dimension ref="A1:B142"/>
   <sheetViews>
-    <sheetView topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="A143" sqref="A143:A144"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1725,7 +1719,7 @@
     </row>
     <row r="72" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>135</v>
+        <v>227</v>
       </c>
       <c r="B72" s="3">
         <v>10</v>
@@ -1733,7 +1727,7 @@
     </row>
     <row r="73" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>136</v>
+        <v>228</v>
       </c>
       <c r="B73" s="3">
         <v>2</v>
@@ -1741,7 +1735,7 @@
     </row>
     <row r="74" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>137</v>
+        <v>229</v>
       </c>
       <c r="B74" s="3">
         <v>1</v>
@@ -1749,7 +1743,7 @@
     </row>
     <row r="75" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>138</v>
+        <v>230</v>
       </c>
       <c r="B75" s="3">
         <v>99</v>
@@ -1757,7 +1751,7 @@
     </row>
     <row r="76" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B76" s="3">
         <v>1000</v>
@@ -1765,7 +1759,7 @@
     </row>
     <row r="77" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B77" s="3">
         <v>100</v>
@@ -1773,7 +1767,7 @@
     </row>
     <row r="78" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B78" s="3">
         <v>1</v>
@@ -1781,7 +1775,7 @@
     </row>
     <row r="79" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B79" s="3">
         <v>999999</v>
@@ -1789,7 +1783,7 @@
     </row>
     <row r="80" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B80" s="3">
         <v>60</v>
@@ -1797,7 +1791,7 @@
     </row>
     <row r="81" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B81" s="3">
         <v>5</v>
@@ -1805,7 +1799,7 @@
     </row>
     <row r="82" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B82" s="3">
         <v>1</v>
@@ -1813,7 +1807,7 @@
     </row>
     <row r="83" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B83" s="3">
         <v>999999</v>
@@ -1821,7 +1815,7 @@
     </row>
     <row r="84" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B84" s="3">
         <v>1.5</v>
@@ -1829,7 +1823,7 @@
     </row>
     <row r="85" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B85" s="3">
         <v>0.25</v>
@@ -1837,7 +1831,7 @@
     </row>
     <row r="86" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B86" s="3">
         <v>0.1</v>
@@ -1845,7 +1839,7 @@
     </row>
     <row r="87" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B87" s="3">
         <v>4</v>
@@ -1853,7 +1847,7 @@
     </row>
     <row r="88" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B88" s="3">
         <v>0.4</v>
@@ -1861,7 +1855,7 @@
     </row>
     <row r="89" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B89" s="3">
         <v>0.25</v>
@@ -1869,180 +1863,180 @@
     </row>
     <row r="90" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="B90" s="3">
-        <v>9.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>197</v>
-      </c>
-      <c r="B91" s="3">
-        <v>10</v>
+      <c r="A91" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="5" t="s">
-        <v>26</v>
+      <c r="A92" t="s">
+        <v>149</v>
+      </c>
+      <c r="B92" s="3">
+        <v>10000</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B93" s="3">
-        <v>10000</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B94" s="3">
-        <v>2500</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B95" s="3">
-        <v>1</v>
+        <v>999999999</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B96" s="3">
-        <v>999999999</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B97" s="3">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B98" s="3">
-        <v>0.02</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B99" s="3">
-        <v>5.0000000000000001E-3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B100" s="3">
-        <v>0.2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B101" s="3">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B102" s="3">
-        <v>0.02</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B103" s="3">
-        <v>1E-3</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B104" s="3">
-        <v>0.15</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B105" s="3">
-        <v>1000</v>
+        <v>300</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B106" s="3">
-        <v>300</v>
+        <v>100</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B107" s="3">
-        <v>100</v>
+        <v>999999</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B108" s="3">
-        <v>999999</v>
+        <v>20</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B109" s="3">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B110" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B111" s="3">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B112" s="3">
         <v>100</v>
@@ -2050,15 +2044,15 @@
     </row>
     <row r="113" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B113" s="3">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B114" s="3">
         <v>10</v>
@@ -2066,235 +2060,219 @@
     </row>
     <row r="115" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B115" s="3">
-        <v>10</v>
+        <v>999</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>176</v>
+        <v>223</v>
       </c>
       <c r="B116" s="3">
-        <v>999</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>177</v>
+        <v>224</v>
       </c>
       <c r="B117" s="3">
-        <v>1000</v>
+        <v>200</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>178</v>
+        <v>225</v>
       </c>
       <c r="B118" s="3">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>179</v>
+        <v>226</v>
       </c>
       <c r="B119" s="3">
-        <v>100</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="B120" s="3">
-        <v>9999</v>
+        <v>100</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="B121" s="3">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B122" s="3">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B123" s="3">
-        <v>1</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="B124" s="3">
-        <v>9999</v>
+        <v>60</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="B125" s="3">
-        <v>60</v>
+        <v>5</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B126" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B127" s="3">
-        <v>1</v>
+        <v>999999</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="B128" s="3">
-        <v>999999</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B129" s="3">
-        <v>1.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B130" s="3">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="B131" s="3">
-        <v>0.1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="B132" s="3">
-        <v>4</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B133" s="3">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>194</v>
-      </c>
-      <c r="B134" s="3">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A135" t="s">
-        <v>195</v>
-      </c>
-      <c r="B135" s="3">
+        <v>188</v>
+      </c>
+      <c r="B134" s="1">
         <v>100</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" s="6" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B136" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A137" s="6" t="s">
-        <v>226</v>
+      <c r="A137" t="s">
+        <v>191</v>
+      </c>
+      <c r="B137" s="1">
+        <v>0.5</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B138" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B139" s="1">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A140" t="s">
-        <v>202</v>
-      </c>
-      <c r="B140" s="1">
-        <v>0.1</v>
+      <c r="A140" s="6" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>203</v>
-      </c>
-      <c r="B141" s="1">
-        <v>0.05</v>
+        <v>211</v>
+      </c>
+      <c r="B141" s="12">
+        <v>1000000</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A142" s="6" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A143" t="s">
-        <v>221</v>
-      </c>
-      <c r="B143" s="12">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A144" t="s">
-        <v>222</v>
-      </c>
-      <c r="B144" s="12">
+      <c r="A142" t="s">
+        <v>212</v>
+      </c>
+      <c r="B142" s="12">
         <v>0.5</v>
       </c>
     </row>
@@ -2310,7 +2288,7 @@
   </sheetPr>
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+    <sheetView topLeftCell="A41" workbookViewId="0">
       <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
@@ -2628,12 +2606,12 @@
     </row>
     <row r="41" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="B42" s="12">
         <v>0.02</v>
@@ -2641,7 +2619,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="B43" s="12">
         <v>1</v>
@@ -2649,7 +2627,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="B44" s="12">
         <v>0</v>
@@ -2657,7 +2635,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="B45" s="12">
         <v>1</v>
@@ -2665,7 +2643,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="B46" s="12">
         <v>10</v>
@@ -2673,7 +2651,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="B47" s="12">
         <v>1000</v>
@@ -2681,7 +2659,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="B48" s="12">
         <v>100000</v>
@@ -2689,12 +2667,12 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="B50" s="12">
         <v>-1E-3</v>
@@ -2702,7 +2680,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="B51" s="12">
         <v>1E-3</v>
@@ -2745,7 +2723,7 @@
     </row>
     <row r="3" spans="1:2" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="B3" s="9">
         <v>0.1</v>
@@ -2753,7 +2731,7 @@
     </row>
     <row r="4" spans="1:2" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="B4" s="9">
         <v>0.1</v>
@@ -2761,7 +2739,7 @@
     </row>
     <row r="5" spans="1:2" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="B5" s="9">
         <v>0.1</v>
@@ -2769,7 +2747,7 @@
     </row>
     <row r="6" spans="1:2" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="B6" s="9">
         <v>0.1</v>
@@ -2782,7 +2760,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="B8" s="9">
         <v>0.1</v>
@@ -2790,7 +2768,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="B9" s="9">
         <v>0.1</v>
@@ -2798,7 +2776,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="B10" s="9">
         <v>0.1</v>
@@ -2806,7 +2784,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="B11" s="9">
         <v>0</v>
@@ -2814,7 +2792,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="B12" s="9">
         <v>0.2</v>
@@ -2822,7 +2800,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="B13" s="9">
         <v>0</v>
@@ -2830,7 +2808,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="B14" s="9">
         <v>0.2</v>
@@ -2843,7 +2821,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="B16" s="9">
         <v>0.1</v>
@@ -2851,7 +2829,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B17" s="9">
         <v>0.1</v>
@@ -2859,7 +2837,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="B18" s="9">
         <v>0.1</v>
@@ -2867,7 +2845,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="B19" s="9">
         <v>0</v>
@@ -2875,7 +2853,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="B20" s="9">
         <v>0.2</v>
@@ -2883,7 +2861,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="B21" s="9">
         <v>0</v>
@@ -2891,7 +2869,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="B22" s="9">
         <v>0.2</v>
@@ -2956,13 +2934,13 @@
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Various fixes, change ints to long longs
</commit_message>
<xml_diff>
--- a/InitializationData/Simulation_Parameters.xlsx
+++ b/InitializationData/Simulation_Parameters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feyzi\OneDrive - Imperial College London\Programming\GithubRepos\Vulcan\InitializationData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/fce19_ic_ac_uk/Documents/Programming/GithubRepos/Vulcan/InitializationData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9280AE-F729-4E1B-87DC-4E1FC8045E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{9A9280AE-F729-4E1B-87DC-4E1FC8045E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{712B8755-9E9B-411A-B0CB-5E466CEBACD7}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="207">
   <si>
     <t>sector_name</t>
   </si>
@@ -261,9 +261,6 @@
   </si>
   <si>
     <t>bank_risk_premium</t>
-  </si>
-  <si>
-    <t>bank_target_capital_ratio</t>
   </si>
   <si>
     <t>bank_short_term_loan_length</t>
@@ -1097,7 +1094,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>23</v>
@@ -1105,12 +1102,12 @@
     </row>
     <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" s="4">
         <v>0.02</v>
@@ -1123,7 +1120,7 @@
     </row>
     <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" s="4">
         <v>0.15</v>
@@ -1131,7 +1128,7 @@
     </row>
     <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6" s="4">
         <v>0.1</v>
@@ -1139,7 +1136,7 @@
     </row>
     <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B7" s="4">
         <v>0.9</v>
@@ -1147,7 +1144,7 @@
     </row>
     <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B8" s="4">
         <v>0.5</v>
@@ -1155,7 +1152,7 @@
     </row>
     <row r="9" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B9" s="4">
         <v>0.5</v>
@@ -1163,7 +1160,7 @@
     </row>
     <row r="10" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B10" s="4">
         <v>0.1</v>
@@ -1171,7 +1168,7 @@
     </row>
     <row r="11" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B11" s="4">
         <v>0.1</v>
@@ -1179,7 +1176,7 @@
     </row>
     <row r="12" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B12" s="4">
         <v>0.9</v>
@@ -1187,7 +1184,7 @@
     </row>
     <row r="13" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B13" s="4">
         <v>0.2</v>
@@ -1195,7 +1192,7 @@
     </row>
     <row r="14" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B14" s="4">
         <v>0.05</v>
@@ -1203,7 +1200,7 @@
     </row>
     <row r="15" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B15" s="4">
         <v>0</v>
@@ -1211,7 +1208,7 @@
     </row>
     <row r="16" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B16" s="4">
         <v>0.4</v>
@@ -1219,7 +1216,7 @@
     </row>
     <row r="17" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B17" s="4">
         <v>0.3</v>
@@ -1227,7 +1224,7 @@
     </row>
     <row r="18" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B18" s="4">
         <v>0.05</v>
@@ -1235,7 +1232,7 @@
     </row>
     <row r="19" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B19" s="4">
         <v>0</v>
@@ -1243,7 +1240,7 @@
     </row>
     <row r="20" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B20" s="4">
         <v>0.7</v>
@@ -1251,7 +1248,7 @@
     </row>
     <row r="21" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B21" s="4">
         <v>0.2</v>
@@ -1259,7 +1256,7 @@
     </row>
     <row r="22" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B22" s="4">
         <v>0.05</v>
@@ -1267,7 +1264,7 @@
     </row>
     <row r="23" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B23" s="4">
         <v>0</v>
@@ -1275,7 +1272,7 @@
     </row>
     <row r="24" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B24" s="4">
         <v>0.5</v>
@@ -1283,7 +1280,7 @@
     </row>
     <row r="25" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B25" s="4">
         <v>0.3</v>
@@ -1291,7 +1288,7 @@
     </row>
     <row r="26" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B26" s="4">
         <v>0.05</v>
@@ -1299,7 +1296,7 @@
     </row>
     <row r="27" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B27" s="4">
         <v>0.1</v>
@@ -1307,7 +1304,7 @@
     </row>
     <row r="28" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B28" s="4">
         <v>0.6</v>
@@ -1315,7 +1312,7 @@
     </row>
     <row r="29" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B29" s="4">
         <v>1000</v>
@@ -1323,7 +1320,7 @@
     </row>
     <row r="30" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B30" s="4">
         <v>300</v>
@@ -1331,7 +1328,7 @@
     </row>
     <row r="31" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B31" s="4">
         <v>0</v>
@@ -1339,7 +1336,7 @@
     </row>
     <row r="32" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B32" s="4">
         <v>2000</v>
@@ -1347,7 +1344,7 @@
     </row>
     <row r="33" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B33" s="4">
         <v>4</v>
@@ -1355,7 +1352,7 @@
     </row>
     <row r="34" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B34" s="4">
         <v>2</v>
@@ -1363,7 +1360,7 @@
     </row>
     <row r="35" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B35" s="4">
         <v>0</v>
@@ -1371,7 +1368,7 @@
     </row>
     <row r="36" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B36" s="4">
         <v>100</v>
@@ -1379,7 +1376,7 @@
     </row>
     <row r="37" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B37" s="4">
         <v>950</v>
@@ -1387,7 +1384,7 @@
     </row>
     <row r="38" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B38" s="4">
         <v>300</v>
@@ -1395,7 +1392,7 @@
     </row>
     <row r="39" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B39" s="4">
         <v>100</v>
@@ -1403,7 +1400,7 @@
     </row>
     <row r="40" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B40" s="4">
         <v>999999</v>
@@ -1411,7 +1408,7 @@
     </row>
     <row r="41" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B41" s="4">
         <v>500</v>
@@ -1419,7 +1416,7 @@
     </row>
     <row r="42" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B42" s="4">
         <v>600</v>
@@ -1432,7 +1429,7 @@
     </row>
     <row r="44" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B44" s="4">
         <v>10000</v>
@@ -1440,7 +1437,7 @@
     </row>
     <row r="45" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B45" s="4">
         <v>2500</v>
@@ -1448,7 +1445,7 @@
     </row>
     <row r="46" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B46" s="4">
         <v>1</v>
@@ -1456,7 +1453,7 @@
     </row>
     <row r="47" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B47" s="4">
         <v>999999999</v>
@@ -1464,7 +1461,7 @@
     </row>
     <row r="48" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B48" s="4">
         <v>0.04</v>
@@ -1472,7 +1469,7 @@
     </row>
     <row r="49" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B49" s="4">
         <v>0.01</v>
@@ -1480,7 +1477,7 @@
     </row>
     <row r="50" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B50" s="4">
         <v>1000</v>
@@ -1488,7 +1485,7 @@
     </row>
     <row r="51" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B51" s="4">
         <v>300</v>
@@ -1496,7 +1493,7 @@
     </row>
     <row r="52" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B52" s="4">
         <v>100</v>
@@ -1504,7 +1501,7 @@
     </row>
     <row r="53" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B53" s="4">
         <v>999999</v>
@@ -1512,7 +1509,7 @@
     </row>
     <row r="54" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B54" s="4">
         <v>20</v>
@@ -1520,7 +1517,7 @@
     </row>
     <row r="55" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B55" s="4">
         <v>5</v>
@@ -1528,7 +1525,7 @@
     </row>
     <row r="56" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B56" s="4">
         <v>1</v>
@@ -1536,7 +1533,7 @@
     </row>
     <row r="57" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B57" s="4">
         <v>100</v>
@@ -1544,7 +1541,7 @@
     </row>
     <row r="58" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B58" s="4">
         <v>10</v>
@@ -1552,7 +1549,7 @@
     </row>
     <row r="59" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B59" s="17">
         <v>2</v>
@@ -1560,7 +1557,7 @@
     </row>
     <row r="60" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B60" s="4">
         <v>1</v>
@@ -1568,7 +1565,7 @@
     </row>
     <row r="61" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B61" s="4">
         <v>99</v>
@@ -1576,7 +1573,7 @@
     </row>
     <row r="62" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B62" s="4">
         <v>1</v>
@@ -1584,7 +1581,7 @@
     </row>
     <row r="63" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B63" s="4">
         <v>0.25</v>
@@ -1592,7 +1589,7 @@
     </row>
     <row r="64" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B64" s="4">
         <v>0.1</v>
@@ -1600,7 +1597,7 @@
     </row>
     <row r="65" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B65" s="4">
         <v>2</v>
@@ -1608,7 +1605,7 @@
     </row>
     <row r="66" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B66" s="4">
         <v>60</v>
@@ -1616,7 +1613,7 @@
     </row>
     <row r="67" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B67" s="4">
         <v>5</v>
@@ -1624,7 +1621,7 @@
     </row>
     <row r="68" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B68" s="4">
         <v>1</v>
@@ -1632,7 +1629,7 @@
     </row>
     <row r="69" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B69" s="4">
         <v>999999</v>
@@ -1640,7 +1637,7 @@
     </row>
     <row r="70" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B70" s="4">
         <v>1.5</v>
@@ -1648,7 +1645,7 @@
     </row>
     <row r="71" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B71" s="4">
         <v>0.25</v>
@@ -1656,7 +1653,7 @@
     </row>
     <row r="72" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B72" s="4">
         <v>0.1</v>
@@ -1664,7 +1661,7 @@
     </row>
     <row r="73" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B73" s="4">
         <v>4</v>
@@ -1672,7 +1669,7 @@
     </row>
     <row r="74" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B74" s="4">
         <v>0.4</v>
@@ -1680,7 +1677,7 @@
     </row>
     <row r="75" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B75" s="4">
         <v>0.25</v>
@@ -1688,7 +1685,7 @@
     </row>
     <row r="76" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B76" s="4">
         <v>10</v>
@@ -1701,7 +1698,7 @@
     </row>
     <row r="78" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B78" s="4">
         <v>10000</v>
@@ -1709,7 +1706,7 @@
     </row>
     <row r="79" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B79" s="4">
         <v>2500</v>
@@ -1717,7 +1714,7 @@
     </row>
     <row r="80" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B80" s="4">
         <v>1</v>
@@ -1725,7 +1722,7 @@
     </row>
     <row r="81" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B81" s="4">
         <v>999999999</v>
@@ -1733,7 +1730,7 @@
     </row>
     <row r="82" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B82" s="4">
         <v>0.04</v>
@@ -1741,7 +1738,7 @@
     </row>
     <row r="83" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B83" s="4">
         <v>0.01</v>
@@ -1749,7 +1746,7 @@
     </row>
     <row r="84" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B84" s="4">
         <v>1000</v>
@@ -1757,7 +1754,7 @@
     </row>
     <row r="85" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B85" s="4">
         <v>300</v>
@@ -1765,7 +1762,7 @@
     </row>
     <row r="86" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B86" s="4">
         <v>100</v>
@@ -1773,7 +1770,7 @@
     </row>
     <row r="87" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B87" s="4">
         <v>999999</v>
@@ -1781,7 +1778,7 @@
     </row>
     <row r="88" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B88" s="4">
         <v>20</v>
@@ -1789,7 +1786,7 @@
     </row>
     <row r="89" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B89" s="4">
         <v>5</v>
@@ -1797,7 +1794,7 @@
     </row>
     <row r="90" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B90" s="4">
         <v>1</v>
@@ -1805,7 +1802,7 @@
     </row>
     <row r="91" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B91" s="4">
         <v>100</v>
@@ -1813,7 +1810,7 @@
     </row>
     <row r="92" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B92" s="4">
         <v>1000</v>
@@ -1821,7 +1818,7 @@
     </row>
     <row r="93" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B93" s="4">
         <v>200</v>
@@ -1829,7 +1826,7 @@
     </row>
     <row r="94" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B94" s="4">
         <v>100</v>
@@ -1837,7 +1834,7 @@
     </row>
     <row r="95" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B95" s="4">
         <v>9999</v>
@@ -1845,7 +1842,7 @@
     </row>
     <row r="96" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B96" s="4">
         <v>1</v>
@@ -1853,7 +1850,7 @@
     </row>
     <row r="97" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B97" s="4">
         <v>0.25</v>
@@ -1861,7 +1858,7 @@
     </row>
     <row r="98" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B98" s="4">
         <v>0.1</v>
@@ -1869,7 +1866,7 @@
     </row>
     <row r="99" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B99" s="4">
         <v>2</v>
@@ -1877,7 +1874,7 @@
     </row>
     <row r="100" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B100" s="4">
         <v>60</v>
@@ -1885,7 +1882,7 @@
     </row>
     <row r="101" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B101" s="4">
         <v>5</v>
@@ -1893,7 +1890,7 @@
     </row>
     <row r="102" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B102" s="4">
         <v>1</v>
@@ -1901,7 +1898,7 @@
     </row>
     <row r="103" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B103" s="4">
         <v>999999</v>
@@ -1909,7 +1906,7 @@
     </row>
     <row r="104" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B104" s="4">
         <v>1.5</v>
@@ -1917,7 +1914,7 @@
     </row>
     <row r="105" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B105" s="4">
         <v>0.25</v>
@@ -1925,7 +1922,7 @@
     </row>
     <row r="106" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B106" s="4">
         <v>0.1</v>
@@ -1933,7 +1930,7 @@
     </row>
     <row r="107" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B107" s="4">
         <v>4</v>
@@ -1941,7 +1938,7 @@
     </row>
     <row r="108" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B108" s="4">
         <v>0.4</v>
@@ -1949,7 +1946,7 @@
     </row>
     <row r="109" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B109" s="4">
         <v>0.25</v>
@@ -1957,7 +1954,7 @@
     </row>
     <row r="110" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B110" s="2">
         <v>100</v>
@@ -1965,12 +1962,12 @@
     </row>
     <row r="111" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B112" s="2">
         <v>0</v>
@@ -1978,7 +1975,7 @@
     </row>
     <row r="113" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B113" s="2">
         <v>0.5</v>
@@ -1986,7 +1983,7 @@
     </row>
     <row r="114" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B114" s="2">
         <v>0.1</v>
@@ -1994,7 +1991,7 @@
     </row>
     <row r="115" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B115" s="2">
         <v>0.05</v>
@@ -2002,12 +1999,12 @@
     </row>
     <row r="116" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B117" s="16">
         <v>1000000</v>
@@ -2015,7 +2012,7 @@
     </row>
     <row r="118" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B118" s="16">
         <v>0.5</v>
@@ -2032,10 +2029,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2222,7 +2219,7 @@
     </row>
     <row r="24" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B24" s="15">
         <v>1</v>
@@ -2283,7 +2280,7 @@
     </row>
     <row r="32" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B32" s="15">
         <v>1</v>
@@ -2331,7 +2328,7 @@
         <v>75</v>
       </c>
       <c r="B38" s="15">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2339,7 +2336,7 @@
         <v>76</v>
       </c>
       <c r="B39" s="15">
-        <v>12</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2347,7 +2344,7 @@
         <v>77</v>
       </c>
       <c r="B40" s="15">
-        <v>100</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2355,20 +2352,20 @@
         <v>78</v>
       </c>
       <c r="B41" s="15">
-        <v>5</v>
+        <v>400</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="A42" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B42" s="15">
-        <v>400</v>
-      </c>
     </row>
     <row r="43" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="7" t="s">
+      <c r="A43" t="s">
         <v>80</v>
+      </c>
+      <c r="B43" s="16">
+        <v>0.02</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2376,7 +2373,7 @@
         <v>81</v>
       </c>
       <c r="B44" s="16">
-        <v>0.02</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2384,7 +2381,7 @@
         <v>82</v>
       </c>
       <c r="B45" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2392,7 +2389,7 @@
         <v>83</v>
       </c>
       <c r="B46" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2400,7 +2397,7 @@
         <v>84</v>
       </c>
       <c r="B47" s="16">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2408,7 +2405,7 @@
         <v>85</v>
       </c>
       <c r="B48" s="16">
-        <v>10</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2416,20 +2413,20 @@
         <v>86</v>
       </c>
       <c r="B49" s="16">
-        <v>1000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="A50" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B50" s="16">
-        <v>100000</v>
-      </c>
     </row>
     <row r="51" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="7" t="s">
+      <c r="A51" t="s">
         <v>88</v>
+      </c>
+      <c r="B51" s="16">
+        <v>-1E-3</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2437,14 +2434,6 @@
         <v>89</v>
       </c>
       <c r="B52" s="16">
-        <v>-1E-3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>90</v>
-      </c>
-      <c r="B53" s="16">
         <v>1E-3</v>
       </c>
     </row>
@@ -2676,7 +2665,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Fixes to bank data logging, additions to python
</commit_message>
<xml_diff>
--- a/InitializationData/Simulation_Parameters.xlsx
+++ b/InitializationData/Simulation_Parameters.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="198">
   <si>
     <t>sector_name</t>
   </si>
@@ -266,6 +266,12 @@
   </si>
   <si>
     <t>bank_leverage_ratio_upper_threshold</t>
+  </si>
+  <si>
+    <t>bank_max_interest_rate</t>
+  </si>
+  <si>
+    <t>bank_max_interest_rate_change</t>
   </si>
   <si>
     <t>Bank Emission Penalty Parameters</t>
@@ -1028,7 +1034,7 @@
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="9" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>24</v>
@@ -1036,13 +1042,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="9" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B2" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B3" s="3">
         <v>0.02</v>
@@ -1056,7 +1062,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B5" s="3">
         <v>0.15</v>
@@ -1064,7 +1070,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B6" s="3">
         <v>0.1</v>
@@ -1072,7 +1078,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B7" s="3">
         <v>0.9</v>
@@ -1080,7 +1086,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B8" s="3">
         <v>0.5</v>
@@ -1088,7 +1094,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B9" s="3">
         <v>0.5</v>
@@ -1096,7 +1102,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B10" s="3">
         <v>0.1</v>
@@ -1104,7 +1110,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B11" s="3">
         <v>0.1</v>
@@ -1112,7 +1118,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B12" s="3">
         <v>0.9</v>
@@ -1120,7 +1126,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B13" s="3">
         <v>0.3</v>
@@ -1128,7 +1134,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B14" s="3">
         <v>0.05</v>
@@ -1136,7 +1142,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B15" s="3">
         <v>0</v>
@@ -1144,7 +1150,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B16" s="3">
         <v>0.7</v>
@@ -1152,7 +1158,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B17" s="3">
         <v>0.2</v>
@@ -1160,7 +1166,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B18" s="3">
         <v>0.05</v>
@@ -1168,7 +1174,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B19" s="3">
         <v>0</v>
@@ -1176,7 +1182,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B20" s="3">
         <v>0.5</v>
@@ -1184,7 +1190,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B21" s="3">
         <v>0.3</v>
@@ -1192,7 +1198,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B22" s="3">
         <v>0.05</v>
@@ -1200,7 +1206,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B23" s="3">
         <v>0.1</v>
@@ -1208,7 +1214,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B24" s="3">
         <v>0.6</v>
@@ -1216,7 +1222,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B25" s="3">
         <v>1000</v>
@@ -1224,7 +1230,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B26" s="3">
         <v>300</v>
@@ -1232,7 +1238,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B27" s="3">
         <v>0</v>
@@ -1240,7 +1246,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B28" s="3">
         <v>2000</v>
@@ -1248,7 +1254,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B29" s="3">
         <v>4</v>
@@ -1256,7 +1262,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B30" s="3">
         <v>2</v>
@@ -1264,7 +1270,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B31" s="3">
         <v>0</v>
@@ -1272,7 +1278,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B32" s="3">
         <v>100</v>
@@ -1280,7 +1286,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B33" s="3">
         <v>950</v>
@@ -1288,7 +1294,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B34" s="3">
         <v>300</v>
@@ -1296,7 +1302,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
       <c r="A35" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B35" s="3">
         <v>100</v>
@@ -1304,7 +1310,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
       <c r="A36" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B36" s="3">
         <v>999999</v>
@@ -1312,7 +1318,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
       <c r="A37" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B37" s="3">
         <v>500</v>
@@ -1320,7 +1326,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
       <c r="A38" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B38" s="3">
         <v>600</v>
@@ -1334,7 +1340,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
       <c r="A40" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B40" s="3">
         <v>10000</v>
@@ -1342,7 +1348,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
       <c r="A41" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B41" s="3">
         <v>2500</v>
@@ -1350,7 +1356,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
       <c r="A42" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B42" s="3">
         <v>1</v>
@@ -1358,7 +1364,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
       <c r="A43" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B43" s="3">
         <v>999999999</v>
@@ -1366,7 +1372,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
       <c r="A44" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B44" s="3">
         <v>0.01</v>
@@ -1374,7 +1380,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
       <c r="A45" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B45" s="3">
         <v>0.005</v>
@@ -1382,7 +1388,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
       <c r="A46" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B46" s="3">
         <v>1000</v>
@@ -1390,7 +1396,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
       <c r="A47" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B47" s="3">
         <v>300</v>
@@ -1398,7 +1404,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
       <c r="A48" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B48" s="3">
         <v>100</v>
@@ -1406,7 +1412,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
       <c r="A49" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B49" s="3">
         <v>999999</v>
@@ -1414,7 +1420,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
       <c r="A50" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B50" s="3">
         <v>20</v>
@@ -1422,7 +1428,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
       <c r="A51" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B51" s="3">
         <v>5</v>
@@ -1430,7 +1436,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
       <c r="A52" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B52" s="3">
         <v>1</v>
@@ -1438,7 +1444,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
       <c r="A53" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B53" s="3">
         <v>100</v>
@@ -1446,7 +1452,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
       <c r="A54" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B54" s="3">
         <v>10</v>
@@ -1454,7 +1460,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
       <c r="A55" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B55" s="16">
         <v>2</v>
@@ -1462,7 +1468,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
       <c r="A56" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B56" s="3">
         <v>1</v>
@@ -1470,7 +1476,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
       <c r="A57" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B57" s="3">
         <v>99</v>
@@ -1478,7 +1484,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
       <c r="A58" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B58" s="3">
         <v>2</v>
@@ -1486,7 +1492,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
       <c r="A59" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B59" s="3">
         <v>0.25</v>
@@ -1494,7 +1500,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
       <c r="A60" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B60" s="3">
         <v>0.5</v>
@@ -1502,7 +1508,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
       <c r="A61" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B61" s="3">
         <v>2</v>
@@ -1510,7 +1516,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
       <c r="A62" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B62" s="3">
         <v>5</v>
@@ -1518,7 +1524,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5">
       <c r="A63" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B63" s="3">
         <v>0.25</v>
@@ -1526,7 +1532,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
       <c r="A64" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B64" s="3">
         <v>0.1</v>
@@ -1534,7 +1540,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5">
       <c r="A65" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B65" s="3">
         <v>10</v>
@@ -1542,7 +1548,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="19.5">
       <c r="A66" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B66" s="3">
         <v>0.4</v>
@@ -1550,7 +1556,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="19.5">
       <c r="A67" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B67" s="3">
         <v>0.25</v>
@@ -1558,7 +1564,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="19.5">
       <c r="A68" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B68" s="3">
         <v>10</v>
@@ -1572,7 +1578,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="19.5">
       <c r="A70" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B70" s="3">
         <v>10000</v>
@@ -1580,7 +1586,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="19.5">
       <c r="A71" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B71" s="3">
         <v>2500</v>
@@ -1588,7 +1594,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="19.5">
       <c r="A72" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B72" s="3">
         <v>1</v>
@@ -1596,7 +1602,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="19.5">
       <c r="A73" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B73" s="3">
         <v>999999999</v>
@@ -1604,7 +1610,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="19.5">
       <c r="A74" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B74" s="3">
         <v>0.04</v>
@@ -1612,7 +1618,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="19.5">
       <c r="A75" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B75" s="3">
         <v>0.01</v>
@@ -1620,7 +1626,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="19.5">
       <c r="A76" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B76" s="3">
         <v>1000</v>
@@ -1628,7 +1634,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="19.5">
       <c r="A77" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B77" s="3">
         <v>300</v>
@@ -1636,7 +1642,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="19.5">
       <c r="A78" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B78" s="3">
         <v>100</v>
@@ -1644,7 +1650,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="19.5">
       <c r="A79" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B79" s="3">
         <v>999999</v>
@@ -1652,7 +1658,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="19.5">
       <c r="A80" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B80" s="3">
         <v>20</v>
@@ -1660,7 +1666,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="19.5">
       <c r="A81" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B81" s="3">
         <v>5</v>
@@ -1668,7 +1674,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="19.5">
       <c r="A82" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B82" s="3">
         <v>1</v>
@@ -1676,7 +1682,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="19.5">
       <c r="A83" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B83" s="3">
         <v>100</v>
@@ -1684,7 +1690,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="19.5">
       <c r="A84" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B84" s="3">
         <v>2000</v>
@@ -1692,7 +1698,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="19.5">
       <c r="A85" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B85" s="3">
         <v>200</v>
@@ -1700,7 +1706,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="19.5">
       <c r="A86" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B86" s="3">
         <v>100</v>
@@ -1708,7 +1714,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="19.5">
       <c r="A87" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B87" s="3">
         <v>9999</v>
@@ -1716,7 +1722,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="19.5">
       <c r="A88" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B88" s="3">
         <v>1</v>
@@ -1724,7 +1730,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="19.5">
       <c r="A89" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B89" s="3">
         <v>0.25</v>
@@ -1732,7 +1738,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="19.5">
       <c r="A90" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B90" s="3">
         <v>0.1</v>
@@ -1740,7 +1746,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="19.5">
       <c r="A91" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B91" s="3">
         <v>2</v>
@@ -1748,7 +1754,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="19.5">
       <c r="A92" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B92" s="3">
         <v>1.5</v>
@@ -1756,7 +1762,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="19.5">
       <c r="A93" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B93" s="3">
         <v>0.25</v>
@@ -1764,7 +1770,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="19.5">
       <c r="A94" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B94" s="3">
         <v>0.1</v>
@@ -1772,7 +1778,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="19.5">
       <c r="A95" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B95" s="3">
         <v>4</v>
@@ -1780,7 +1786,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="19.5">
       <c r="A96" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B96" s="3">
         <v>0.4</v>
@@ -1788,7 +1794,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="19.5">
       <c r="A97" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B97" s="3">
         <v>0.25</v>
@@ -1796,7 +1802,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="19.5">
       <c r="A98" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B98" s="3">
         <v>100</v>
@@ -1804,13 +1810,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="19.5">
       <c r="A99" s="9" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B99" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="19.5">
       <c r="A100" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B100" s="3">
         <v>0</v>
@@ -1818,7 +1824,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="19.5">
       <c r="A101" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B101" s="3">
         <v>0.5</v>
@@ -1826,7 +1832,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="19.5">
       <c r="A102" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B102" s="3">
         <v>0.1</v>
@@ -1834,7 +1840,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="19.5">
       <c r="A103" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B103" s="3">
         <v>0.05</v>
@@ -1842,13 +1848,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="19.5">
       <c r="A104" s="9" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B104" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="19.5">
       <c r="A105" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B105" s="4">
         <v>1000000</v>
@@ -1856,7 +1862,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="19.5">
       <c r="A106" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B106" s="4">
         <v>0.5</v>
@@ -1872,7 +1878,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B55"/>
+  <dimension ref="A1:B57"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -1909,7 +1915,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="4">
-        <v>100000</v>
+        <v>10000</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
@@ -1917,7 +1923,7 @@
         <v>43</v>
       </c>
       <c r="B5" s="4">
-        <v>4500</v>
+        <v>450</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
@@ -1925,7 +1931,7 @@
         <v>44</v>
       </c>
       <c r="B6" s="4">
-        <v>500</v>
+        <v>50</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
@@ -2225,33 +2231,33 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B45" s="4"/>
+      <c r="B45" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
       <c r="A46" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B46" s="4">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B47" s="4">
-        <v>1</v>
-      </c>
+      <c r="B47" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
       <c r="A48" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B48" s="4">
-        <v>0</v>
+        <v>0.02</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
@@ -2267,7 +2273,7 @@
         <v>88</v>
       </c>
       <c r="B50" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
@@ -2275,7 +2281,7 @@
         <v>89</v>
       </c>
       <c r="B51" s="4">
-        <v>1000</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
@@ -2283,28 +2289,44 @@
         <v>90</v>
       </c>
       <c r="B52" s="4">
-        <v>100000</v>
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
-      <c r="A53" s="9" t="s">
+      <c r="A53" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B53" s="4"/>
+      <c r="B53" s="4">
+        <v>1000</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
       <c r="A54" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B54" s="4">
+        <v>100000</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
+      <c r="A55" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B55" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
+      <c r="A56" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B56" s="4">
         <v>-0.001</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
-      <c r="A55" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B55" s="4">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
+      <c r="A57" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B57" s="4">
         <v>0.001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Edits to python, minor logging changes
</commit_message>
<xml_diff>
--- a/InitializationData/Simulation_Parameters.xlsx
+++ b/InitializationData/Simulation_Parameters.xlsx
@@ -1,18 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feyzi\OneDrive - Imperial College London\Programming\GithubRepos\Vulcan\InitializationData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A1C442-C893-42E2-9E2B-4B6FE8167C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="1260" yWindow="732" windowWidth="17280" windowHeight="8880" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Initialization_Parameters"/>
-    <sheet r:id="rId2" sheetId="2" name="Main_Loop_Parameters"/>
-    <sheet r:id="rId3" sheetId="3" name="Randomness_Parameters"/>
-    <sheet r:id="rId4" sheetId="4" name="Consumer_Firm_Sectors"/>
+    <sheet name="Initialization_Parameters" sheetId="1" r:id="rId1"/>
+    <sheet name="Main_Loop_Parameters" sheetId="2" r:id="rId2"/>
+    <sheet name="Randomness_Parameters" sheetId="3" r:id="rId3"/>
+    <sheet name="Consumer_Firm_Sectors" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -616,7 +635,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
@@ -670,65 +689,62 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="15">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -739,10 +755,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -780,71 +796,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -872,7 +888,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -895,11 +911,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -908,13 +924,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -924,7 +940,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -933,7 +949,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -942,7 +958,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -950,10 +966,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1018,7 +1034,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1026,845 +1042,845 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="41.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="41.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B2" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="1" t="s">
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>0.02</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="1" t="s">
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>99</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>0.15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="1" t="s">
+      <c r="B6" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>0.9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>102</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>103</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>104</v>
       </c>
-      <c r="B10" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="1" t="s">
+      <c r="B10" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>105</v>
       </c>
-      <c r="B11" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="1" t="s">
+      <c r="B11" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>106</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>0.9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>107</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>0.3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>108</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>0.05</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>109</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>110</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>0.7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>111</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>0.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>112</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>0.05</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>113</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="2">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>114</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>115</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <v>0.3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>116</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>0.05</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>117</v>
       </c>
-      <c r="B23" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
-      <c r="A24" s="1" t="s">
+      <c r="B23" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>118</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <v>0.6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>119</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>120</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="2">
         <v>300</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>121</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="2">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>122</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="2">
         <v>2000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>123</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="2">
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>124</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="2">
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>125</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="2">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>126</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="2">
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>127</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="2">
         <v>950</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>128</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="2">
         <v>300</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>129</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="2">
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>130</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="2">
         <v>999999</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>131</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="2">
         <v>500</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>132</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="2">
         <v>600</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
-      <c r="A39" s="9" t="s">
+    <row r="39" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B39" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
-      <c r="A40" s="1" t="s">
+      <c r="B39" s="3"/>
+    </row>
+    <row r="40" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>133</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="2">
         <v>10000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>134</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="2">
         <v>2500</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>135</v>
       </c>
-      <c r="B42" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
-      <c r="A43" s="1" t="s">
+      <c r="B42" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>136</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="2">
         <v>999999999</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>137</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="2">
         <v>0.01</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>138</v>
       </c>
-      <c r="B45" s="3">
-        <v>0.005</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
-      <c r="A46" s="1" t="s">
+      <c r="B45" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>139</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
-      <c r="A47" s="1" t="s">
+    <row r="47" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>140</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="2">
         <v>300</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
-      <c r="A48" s="1" t="s">
+    <row r="48" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>141</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="2">
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
-      <c r="A49" s="1" t="s">
+    <row r="49" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>142</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="2">
         <v>999999</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
-      <c r="A50" s="1" t="s">
+    <row r="50" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>143</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="2">
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>144</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B51" s="2">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
-      <c r="A52" s="1" t="s">
+    <row r="52" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>145</v>
       </c>
-      <c r="B52" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
-      <c r="A53" s="1" t="s">
+      <c r="B52" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>146</v>
       </c>
-      <c r="B53" s="3">
+      <c r="B53" s="2">
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>147</v>
       </c>
-      <c r="B54" s="3">
+      <c r="B54" s="2">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
-      <c r="A55" s="1" t="s">
+    <row r="55" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>148</v>
       </c>
-      <c r="B55" s="16">
+      <c r="B55" s="14">
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
-      <c r="A56" s="1" t="s">
+    <row r="56" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>149</v>
       </c>
-      <c r="B56" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
-      <c r="A57" s="1" t="s">
+      <c r="B56" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>150</v>
       </c>
-      <c r="B57" s="3">
+      <c r="B57" s="2">
         <v>99</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
-      <c r="A58" s="1" t="s">
+    <row r="58" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>151</v>
       </c>
-      <c r="B58" s="3">
+      <c r="B58" s="2">
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
-      <c r="A59" s="1" t="s">
+    <row r="59" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>152</v>
       </c>
-      <c r="B59" s="3">
+      <c r="B59" s="2">
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
-      <c r="A60" s="1" t="s">
+    <row r="60" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>153</v>
       </c>
-      <c r="B60" s="3">
+      <c r="B60" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
-      <c r="A61" s="1" t="s">
+    <row r="61" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>154</v>
       </c>
-      <c r="B61" s="3">
+      <c r="B61" s="2">
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
-      <c r="A62" s="1" t="s">
+    <row r="62" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>155</v>
       </c>
-      <c r="B62" s="3">
+      <c r="B62" s="2">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5">
-      <c r="A63" s="1" t="s">
+    <row r="63" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>156</v>
       </c>
-      <c r="B63" s="3">
+      <c r="B63" s="2">
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
-      <c r="A64" s="1" t="s">
+    <row r="64" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>157</v>
       </c>
-      <c r="B64" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5">
-      <c r="A65" s="1" t="s">
+      <c r="B64" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>158</v>
       </c>
-      <c r="B65" s="3">
+      <c r="B65" s="2">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="19.5">
-      <c r="A66" s="1" t="s">
+    <row r="66" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>159</v>
       </c>
-      <c r="B66" s="3">
+      <c r="B66" s="2">
         <v>0.4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="19.5">
-      <c r="A67" s="1" t="s">
+    <row r="67" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>160</v>
       </c>
-      <c r="B67" s="3">
+      <c r="B67" s="2">
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="19.5">
-      <c r="A68" s="1" t="s">
+    <row r="68" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>161</v>
       </c>
-      <c r="B68" s="3">
+      <c r="B68" s="2">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="19.5">
-      <c r="A69" s="9" t="s">
+    <row r="69" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B69" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="19.5">
-      <c r="A70" s="1" t="s">
+      <c r="B69" s="3"/>
+    </row>
+    <row r="70" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
         <v>162</v>
       </c>
-      <c r="B70" s="3">
+      <c r="B70" s="2">
         <v>10000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="19.5">
-      <c r="A71" s="1" t="s">
+    <row r="71" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
         <v>163</v>
       </c>
-      <c r="B71" s="3">
+      <c r="B71" s="2">
         <v>2500</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="19.5">
-      <c r="A72" s="1" t="s">
+    <row r="72" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
         <v>164</v>
       </c>
-      <c r="B72" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="19.5">
-      <c r="A73" s="1" t="s">
+      <c r="B72" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
         <v>165</v>
       </c>
-      <c r="B73" s="3">
+      <c r="B73" s="2">
         <v>999999999</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="19.5">
-      <c r="A74" s="1" t="s">
+    <row r="74" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>166</v>
       </c>
-      <c r="B74" s="3">
+      <c r="B74" s="2">
         <v>0.04</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="19.5">
-      <c r="A75" s="1" t="s">
+    <row r="75" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>167</v>
       </c>
-      <c r="B75" s="3">
+      <c r="B75" s="2">
         <v>0.01</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="19.5">
-      <c r="A76" s="1" t="s">
+    <row r="76" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
         <v>168</v>
       </c>
-      <c r="B76" s="3">
+      <c r="B76" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="19.5">
-      <c r="A77" s="1" t="s">
+    <row r="77" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
         <v>169</v>
       </c>
-      <c r="B77" s="3">
+      <c r="B77" s="2">
         <v>300</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="19.5">
-      <c r="A78" s="1" t="s">
+    <row r="78" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>170</v>
       </c>
-      <c r="B78" s="3">
+      <c r="B78" s="2">
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="19.5">
-      <c r="A79" s="1" t="s">
+    <row r="79" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
         <v>171</v>
       </c>
-      <c r="B79" s="3">
+      <c r="B79" s="2">
         <v>999999</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="19.5">
-      <c r="A80" s="1" t="s">
+    <row r="80" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>172</v>
       </c>
-      <c r="B80" s="3">
+      <c r="B80" s="2">
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="19.5">
-      <c r="A81" s="1" t="s">
+    <row r="81" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
         <v>173</v>
       </c>
-      <c r="B81" s="3">
+      <c r="B81" s="2">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="19.5">
-      <c r="A82" s="1" t="s">
+    <row r="82" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
         <v>174</v>
       </c>
-      <c r="B82" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="19.5">
-      <c r="A83" s="1" t="s">
+      <c r="B82" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
         <v>175</v>
       </c>
-      <c r="B83" s="3">
+      <c r="B83" s="2">
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="19.5">
-      <c r="A84" s="1" t="s">
+    <row r="84" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
         <v>176</v>
       </c>
-      <c r="B84" s="3">
+      <c r="B84" s="2">
         <v>2000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="19.5">
-      <c r="A85" s="1" t="s">
+    <row r="85" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
         <v>177</v>
       </c>
-      <c r="B85" s="3">
+      <c r="B85" s="2">
         <v>200</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="19.5">
-      <c r="A86" s="1" t="s">
+    <row r="86" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>178</v>
       </c>
-      <c r="B86" s="3">
+      <c r="B86" s="2">
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="19.5">
-      <c r="A87" s="1" t="s">
+    <row r="87" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
         <v>179</v>
       </c>
-      <c r="B87" s="3">
+      <c r="B87" s="2">
         <v>9999</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="19.5">
-      <c r="A88" s="1" t="s">
+    <row r="88" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>180</v>
       </c>
-      <c r="B88" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="19.5">
-      <c r="A89" s="1" t="s">
+      <c r="B88" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
         <v>181</v>
       </c>
-      <c r="B89" s="3">
+      <c r="B89" s="2">
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="19.5">
-      <c r="A90" s="1" t="s">
+    <row r="90" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
         <v>182</v>
       </c>
-      <c r="B90" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="19.5">
-      <c r="A91" s="1" t="s">
+      <c r="B90" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
         <v>183</v>
       </c>
-      <c r="B91" s="3">
+      <c r="B91" s="2">
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="19.5">
-      <c r="A92" s="1" t="s">
+    <row r="92" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
         <v>184</v>
       </c>
-      <c r="B92" s="3">
+      <c r="B92" s="2">
         <v>1.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="19.5">
-      <c r="A93" s="1" t="s">
+    <row r="93" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
         <v>185</v>
       </c>
-      <c r="B93" s="3">
+      <c r="B93" s="2">
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="19.5">
-      <c r="A94" s="1" t="s">
+    <row r="94" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
         <v>186</v>
       </c>
-      <c r="B94" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="19.5">
-      <c r="A95" s="1" t="s">
+      <c r="B94" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
         <v>187</v>
       </c>
-      <c r="B95" s="3">
+      <c r="B95" s="2">
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="19.5">
-      <c r="A96" s="1" t="s">
+    <row r="96" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
         <v>188</v>
       </c>
-      <c r="B96" s="3">
+      <c r="B96" s="2">
         <v>0.4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="19.5">
-      <c r="A97" s="1" t="s">
+    <row r="97" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
         <v>189</v>
       </c>
-      <c r="B97" s="3">
+      <c r="B97" s="2">
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="19.5">
-      <c r="A98" s="1" t="s">
+    <row r="98" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
         <v>161</v>
       </c>
-      <c r="B98" s="3">
+      <c r="B98" s="2">
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="19.5">
-      <c r="A99" s="9" t="s">
+    <row r="99" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="B99" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="19.5">
-      <c r="A100" s="1" t="s">
+      <c r="B99" s="3"/>
+    </row>
+    <row r="100" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
         <v>191</v>
       </c>
-      <c r="B100" s="3">
+      <c r="B100" s="2">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="19.5">
-      <c r="A101" s="1" t="s">
+    <row r="101" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
         <v>192</v>
       </c>
-      <c r="B101" s="3">
+      <c r="B101" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="19.5">
-      <c r="A102" s="1" t="s">
+    <row r="102" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
         <v>193</v>
       </c>
-      <c r="B102" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="19.5">
-      <c r="A103" s="1" t="s">
+      <c r="B102" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
         <v>194</v>
       </c>
-      <c r="B103" s="3">
+      <c r="B103" s="2">
         <v>0.05</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="19.5">
-      <c r="A104" s="9" t="s">
+    <row r="104" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="B104" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="19.5">
-      <c r="A105" s="1" t="s">
+      <c r="B104" s="3"/>
+    </row>
+    <row r="105" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
         <v>196</v>
       </c>
-      <c r="B105" s="4">
+      <c r="B105" s="3">
         <v>1000000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="19.5">
-      <c r="A106" s="1" t="s">
+    <row r="106" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
         <v>197</v>
       </c>
-      <c r="B106" s="4">
+      <c r="B106" s="3">
         <v>0.5</v>
       </c>
     </row>
@@ -1874,460 +1890,461 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="39.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="39.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="1" t="s">
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>60</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>10000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>450</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <f>B5+B6</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="1" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="1" t="s">
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>0.05</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>0.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>0.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="9" t="s">
+    <row r="19" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
-      <c r="A20" s="1" t="s">
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="3">
         <v>0.01</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>59</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="3">
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
-      <c r="A23" s="1" t="s">
+      <c r="B22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
-      <c r="A24" s="1" t="s">
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="3">
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>63</v>
       </c>
-      <c r="B25" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
-      <c r="A26" s="1" t="s">
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="3">
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
-      <c r="A27" s="9" t="s">
+    <row r="27" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
-      <c r="A28" s="1" t="s">
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>66</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="3">
         <v>0.01</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>67</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="3">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>68</v>
       </c>
-      <c r="B30" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
-      <c r="A31" s="1" t="s">
+      <c r="B30" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>69</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="3">
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>70</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="3">
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>71</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="3">
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>72</v>
       </c>
-      <c r="B34" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
-      <c r="A35" s="1" t="s">
+      <c r="B34" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>73</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35" s="3">
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
-      <c r="A36" s="9" t="s">
+    <row r="36" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B36" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
-      <c r="A37" s="1" t="s">
+      <c r="B36" s="3"/>
+    </row>
+    <row r="37" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>75</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37" s="3">
         <v>1.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>76</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38" s="3">
         <v>1.05</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>77</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" s="3">
         <v>1.004</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="4">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
-      <c r="A41" s="1" t="s">
+      <c r="B40" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" s="3">
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>80</v>
       </c>
-      <c r="B42" s="4">
+      <c r="B42" s="3">
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>81</v>
       </c>
-      <c r="B43" s="4">
+      <c r="B43" s="3">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>82</v>
       </c>
-      <c r="B44" s="4">
+      <c r="B44" s="3">
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>83</v>
       </c>
-      <c r="B45" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
-      <c r="A46" s="1" t="s">
+      <c r="B45" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>84</v>
       </c>
-      <c r="B46" s="4">
+      <c r="B46" s="3">
         <v>0.05</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
-      <c r="A47" s="9" t="s">
+    <row r="47" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B47" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
-      <c r="A48" s="1" t="s">
+      <c r="B47" s="3"/>
+    </row>
+    <row r="48" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>86</v>
       </c>
-      <c r="B48" s="4">
+      <c r="B48" s="3">
         <v>0.02</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
-      <c r="A49" s="1" t="s">
+    <row r="49" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>87</v>
       </c>
-      <c r="B49" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
-      <c r="A50" s="1" t="s">
+      <c r="B49" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>88</v>
       </c>
-      <c r="B50" s="4">
+      <c r="B50" s="3">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>89</v>
       </c>
-      <c r="B51" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
-      <c r="A52" s="1" t="s">
+      <c r="B51" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>90</v>
       </c>
-      <c r="B52" s="4">
+      <c r="B52" s="3">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
-      <c r="A53" s="1" t="s">
+    <row r="53" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>91</v>
       </c>
-      <c r="B53" s="4">
+      <c r="B53" s="3">
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>92</v>
       </c>
-      <c r="B54" s="4">
+      <c r="B54" s="3">
         <v>100000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
-      <c r="A55" s="9" t="s">
+    <row r="55" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B55" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
-      <c r="A56" s="1" t="s">
+      <c r="B55" s="3"/>
+    </row>
+    <row r="56" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>94</v>
       </c>
-      <c r="B56" s="4">
-        <v>-0.001</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
-      <c r="A57" s="1" t="s">
+      <c r="B56" s="3">
+        <v>-1E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>95</v>
       </c>
-      <c r="B57" s="4">
-        <v>0.001</v>
+      <c r="B57" s="3">
+        <v>1E-3</v>
       </c>
     </row>
   </sheetData>
@@ -2336,7 +2353,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -2344,131 +2361,131 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="13" width="45.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="14" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="45" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="12" t="s">
+      <c r="B2" s="9"/>
+    </row>
+    <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="11">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="12" t="s">
+      <c r="B3" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="11">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="12" t="s">
+      <c r="B4" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="11">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="12" t="s">
+      <c r="B5" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="11">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="9" t="s">
+      <c r="B6" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="12" t="s">
+      <c r="B7" s="9"/>
+    </row>
+    <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="11">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="12" t="s">
+      <c r="B8" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="11">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="12" t="s">
+      <c r="B9" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="11">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="12" t="s">
+      <c r="B10" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="9">
         <v>0.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="12" t="s">
+      <c r="B12" s="9"/>
+    </row>
+    <row r="13" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="11">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="12" t="s">
+      <c r="B13" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="11">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="12" t="s">
+      <c r="B14" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="11">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="12" t="s">
+      <c r="B15" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="9">
         <v>0.2</v>
       </c>
     </row>
@@ -2478,481 +2495,483 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="27.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="8.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="8.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="12.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="19.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="7" width="24.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.109375" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="C2" s="3">
-        <v>0.096</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="E2" s="2">
+      <c r="C2" s="2">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E2" s="1">
         <v>100</v>
       </c>
-      <c r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I2" s="2">
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I2" s="1">
         <v>10</v>
       </c>
-      <c r="J2" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="K2" s="2">
+      <c r="J2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="K2" s="1">
         <v>96000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0.035</v>
-      </c>
-      <c r="D3" s="4">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D3" s="3">
         <v>0.01</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>40</v>
       </c>
-      <c r="F3" s="2">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2">
-        <v>1</v>
-      </c>
-      <c r="H3" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I3" s="2">
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I3" s="1">
         <v>10</v>
       </c>
-      <c r="J3" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="K3" s="2">
+      <c r="J3" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="K3" s="1">
         <v>35000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="3">
-        <v>0.048</v>
-      </c>
-      <c r="D4" s="4">
+      <c r="C4" s="2">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="D4" s="3">
         <v>0.01</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>50</v>
       </c>
-      <c r="F4" s="2">
-        <v>1</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1</v>
-      </c>
-      <c r="H4" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I4" s="2">
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I4" s="1">
         <v>20</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="2">
         <v>0.2</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="1">
         <v>48000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>3</v>
       </c>
-      <c r="C5" s="3">
-        <v>0.303</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="C5" s="2">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="D5" s="3">
         <v>0.01</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>300</v>
       </c>
-      <c r="F5" s="2">
-        <v>1</v>
-      </c>
-      <c r="G5" s="2">
-        <v>1</v>
-      </c>
-      <c r="H5" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I5" s="2">
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I5" s="1">
         <v>35</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="2">
         <v>0.3</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="1">
         <v>303000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>4</v>
       </c>
-      <c r="C6" s="3">
-        <v>0.056</v>
-      </c>
-      <c r="D6" s="4">
+      <c r="C6" s="2">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="D6" s="3">
         <v>0.01</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>60</v>
       </c>
-      <c r="F6" s="2">
-        <v>1</v>
-      </c>
-      <c r="G6" s="2">
-        <v>1</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I6" s="2">
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I6" s="1">
         <v>35</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="2">
         <v>0.2</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="1">
         <v>56000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>5</v>
       </c>
-      <c r="C7" s="3">
-        <v>0.018</v>
-      </c>
-      <c r="D7" s="4">
+      <c r="C7" s="2">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="D7" s="3">
         <v>0.01</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>20</v>
       </c>
-      <c r="F7" s="2">
-        <v>1</v>
-      </c>
-      <c r="G7" s="2">
-        <v>1</v>
-      </c>
-      <c r="H7" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I7" s="2">
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I7" s="1">
         <v>10</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="2">
         <v>0.15</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="1">
         <v>18000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>6</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>0.111</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>0.01</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>110</v>
       </c>
-      <c r="F8" s="2">
-        <v>1</v>
-      </c>
-      <c r="G8" s="2">
-        <v>1</v>
-      </c>
-      <c r="H8" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I8" s="2">
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I8" s="1">
         <v>50</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="2">
         <v>0.2</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="1">
         <v>111000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>7</v>
       </c>
-      <c r="C9" s="3">
-        <v>0.019</v>
-      </c>
-      <c r="D9" s="4">
+      <c r="C9" s="2">
+        <v>1.9E-2</v>
+      </c>
+      <c r="D9" s="3">
         <v>0.01</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>20</v>
       </c>
-      <c r="F9" s="2">
-        <v>1</v>
-      </c>
-      <c r="G9" s="2">
-        <v>1</v>
-      </c>
-      <c r="H9" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I9" s="2">
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I9" s="1">
         <v>10</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="2">
         <v>0.3</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="1">
         <v>19000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>8</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>0.112</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>0.01</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>110</v>
       </c>
-      <c r="F10" s="2">
-        <v>1</v>
-      </c>
-      <c r="G10" s="2">
-        <v>1</v>
-      </c>
-      <c r="H10" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I10" s="2">
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I10" s="1">
         <v>5</v>
       </c>
-      <c r="J10" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="K10" s="2">
+      <c r="J10" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="K10" s="1">
         <v>112000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>9</v>
       </c>
-      <c r="C11" s="3">
-        <v>0.023</v>
-      </c>
-      <c r="D11" s="4">
+      <c r="C11" s="2">
+        <v>2.3E-2</v>
+      </c>
+      <c r="D11" s="3">
         <v>0.01</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>20</v>
       </c>
-      <c r="F11" s="2">
-        <v>1</v>
-      </c>
-      <c r="G11" s="2">
-        <v>1</v>
-      </c>
-      <c r="H11" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I11" s="2">
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I11" s="1">
         <v>4</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="2">
         <v>0.2</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="1">
         <v>23000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>10</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>0.112</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>0.01</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>110</v>
       </c>
-      <c r="F12" s="2">
-        <v>1</v>
-      </c>
-      <c r="G12" s="2">
-        <v>1</v>
-      </c>
-      <c r="H12" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I12" s="2">
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I12" s="1">
         <v>10</v>
       </c>
-      <c r="J12" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="K12" s="2">
+      <c r="J12" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="K12" s="1">
         <v>112000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>11</v>
       </c>
-      <c r="C13" s="3">
-        <v>0.067</v>
-      </c>
-      <c r="D13" s="4">
+      <c r="C13" s="2">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="D13" s="3">
         <v>0.01</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <v>70</v>
       </c>
-      <c r="F13" s="2">
-        <v>1</v>
-      </c>
-      <c r="G13" s="2">
-        <v>1</v>
-      </c>
-      <c r="H13" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I13" s="2">
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I13" s="1">
         <v>5</v>
       </c>
-      <c r="J13" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="K13" s="2">
+      <c r="J13" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="K13" s="1">
         <v>67000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove unused parameters, clean up
</commit_message>
<xml_diff>
--- a/InitializationData/Simulation_Parameters.xlsx
+++ b/InitializationData/Simulation_Parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feyzi\OneDrive - Imperial College London\Programming\GithubRepos\Vulcan\InitializationData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/fce19_ic_ac_uk/Documents/Programming/GithubRepos/Vulcan/InitializationData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A1C442-C893-42E2-9E2B-4B6FE8167C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{387A20E8-C7D8-478B-BA3B-F4FFCA890BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BD75A61-5A93-481E-A395-D7446B510A69}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="732" windowWidth="17280" windowHeight="8880" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initialization_Parameters" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="186">
   <si>
     <t>sector_name</t>
   </si>
@@ -53,15 +53,9 @@
     <t>output_per_machine</t>
   </si>
   <si>
-    <t>workers_per_machine</t>
-  </si>
-  <si>
     <t>good_unit_cost</t>
   </si>
   <si>
-    <t>max_production_climbdown</t>
-  </si>
-  <si>
     <t>emissions_per_unit</t>
   </si>
   <si>
@@ -179,12 +173,6 @@
     <t>n_consumer_sectors</t>
   </si>
   <si>
-    <t>n_max_employees</t>
-  </si>
-  <si>
-    <t>time_period</t>
-  </si>
-  <si>
     <t>Dynamic Household Parameters</t>
   </si>
   <si>
@@ -194,21 +182,12 @@
     <t>household_targeted_savings_to_income_ratio</t>
   </si>
   <si>
-    <t>household_tax_rate</t>
-  </si>
-  <si>
     <t>standard_employment_contract_length</t>
   </si>
   <si>
     <t>firm_tax_rate</t>
   </si>
   <si>
-    <t>forced_machine_purchases_min</t>
-  </si>
-  <si>
-    <t>forced_machine_purchases_max</t>
-  </si>
-  <si>
     <t>Consumer Firm Dynamic Parameters</t>
   </si>
   <si>
@@ -224,15 +203,9 @@
     <t>firm_cons_good_unit_cost</t>
   </si>
   <si>
-    <t>firm_cons_max_production_climbdown</t>
-  </si>
-  <si>
     <t>firm_cons_inv_reaction_factor</t>
   </si>
   <si>
-    <t>firm_cons_wage_change</t>
-  </si>
-  <si>
     <t>Capital Firm Dynamic Parameters</t>
   </si>
   <si>
@@ -248,18 +221,12 @@
     <t>firm_cap_good_unit_cost</t>
   </si>
   <si>
-    <t>firm_cap_max_production_climbdown</t>
-  </si>
-  <si>
     <t>firm_cap_machine_lifespan</t>
   </si>
   <si>
     <t>firm_cap_inv_reaction_factor</t>
   </si>
   <si>
-    <t>firm_cap_wage_change</t>
-  </si>
-  <si>
     <t>Dynamic Bank Parameters</t>
   </si>
   <si>
@@ -335,18 +302,6 @@
     <t>bank_init_interest_rate</t>
   </si>
   <si>
-    <t>household_init_c_std</t>
-  </si>
-  <si>
-    <t>household_init_c_min</t>
-  </si>
-  <si>
-    <t>household_init_c_max</t>
-  </si>
-  <si>
-    <t>household_init_c_mean</t>
-  </si>
-  <si>
     <t>household_init_c_f_mean</t>
   </si>
   <si>
@@ -630,6 +585,15 @@
   </si>
   <si>
     <t>emission_init_unit_price</t>
+  </si>
+  <si>
+    <t>firm_cons_init_emissions_per_unit</t>
+  </si>
+  <si>
+    <t>firm_cons_rand_wage_change</t>
+  </si>
+  <si>
+    <t>firm_cap_rand_wage_change</t>
   </si>
 </sst>
 </file>
@@ -1038,9 +1002,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B106"/>
+  <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1050,21 +1016,21 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B3" s="2">
         <v>0.02</v>
@@ -1072,21 +1038,21 @@
     </row>
     <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B5" s="2">
-        <v>0.15</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B6" s="2">
         <v>0.1</v>
@@ -1094,63 +1060,63 @@
     </row>
     <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B7" s="2">
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B8" s="2">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="B9" s="2">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B10" s="2">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B11" s="2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B12" s="2">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B13" s="2">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B14" s="2">
         <v>0.05</v>
@@ -1158,7 +1124,7 @@
     </row>
     <row r="15" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="B15" s="2">
         <v>0</v>
@@ -1166,23 +1132,23 @@
     </row>
     <row r="16" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B16" s="2">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="B17" s="2">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B18" s="2">
         <v>0.05</v>
@@ -1190,71 +1156,71 @@
     </row>
     <row r="19" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="B19" s="2">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B20" s="2">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B21" s="2">
-        <v>0.3</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B22" s="2">
-        <v>0.05</v>
+        <v>300</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B23" s="2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="B24" s="2">
-        <v>0.6</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="B25" s="2">
-        <v>1000</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B26" s="2">
-        <v>300</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="B27" s="2">
         <v>0</v>
@@ -1262,197 +1228,197 @@
     </row>
     <row r="28" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B28" s="2">
-        <v>2000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="B29" s="2">
-        <v>4</v>
+        <v>950</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="B30" s="2">
-        <v>2</v>
+        <v>300</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B31" s="2">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="B32" s="2">
-        <v>100</v>
+        <v>999999</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="B33" s="2">
-        <v>950</v>
+        <v>500</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B34" s="2">
-        <v>300</v>
+        <v>600</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>129</v>
-      </c>
-      <c r="B35" s="2">
-        <v>100</v>
-      </c>
+      <c r="A35" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" s="3"/>
     </row>
     <row r="36" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="B36" s="2">
-        <v>999999</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="B37" s="2">
-        <v>500</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="B38" s="2">
-        <v>600</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B39" s="3"/>
+      <c r="A39" t="s">
+        <v>121</v>
+      </c>
+      <c r="B39" s="2">
+        <v>999999999</v>
+      </c>
     </row>
     <row r="40" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="B40" s="2">
-        <v>10000</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B41" s="2">
-        <v>2500</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B42" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B43" s="2">
-        <v>999999999</v>
+        <v>300</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="B44" s="2">
-        <v>0.01</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="B45" s="2">
-        <v>5.0000000000000001E-3</v>
+        <v>999999</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B46" s="2">
-        <v>1000</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="B47" s="2">
-        <v>300</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B48" s="2">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="B49" s="2">
-        <v>999999</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B50" s="2">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>144</v>
-      </c>
-      <c r="B51" s="2">
-        <v>5</v>
+        <v>133</v>
+      </c>
+      <c r="B51" s="14">
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="B52" s="2">
         <v>1</v>
@@ -1460,55 +1426,55 @@
     </row>
     <row r="53" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="B53" s="2">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="B54" s="2">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>148</v>
-      </c>
-      <c r="B55" s="14">
-        <v>2</v>
+        <v>137</v>
+      </c>
+      <c r="B55" s="2">
+        <v>0.25</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="B56" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="B57" s="2">
-        <v>99</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="B58" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="B59" s="2">
         <v>0.25</v>
@@ -1516,31 +1482,31 @@
     </row>
     <row r="60" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="B60" s="2">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="B61" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="B62" s="2">
-        <v>5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="B63" s="2">
         <v>0.25</v>
@@ -1548,205 +1514,205 @@
     </row>
     <row r="64" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>157</v>
+        <v>183</v>
       </c>
       <c r="B64" s="2">
-        <v>0.1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>158</v>
-      </c>
-      <c r="B65" s="2">
-        <v>10</v>
-      </c>
+      <c r="A65" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B65" s="3"/>
     </row>
     <row r="66" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="B66" s="2">
-        <v>0.4</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="B67" s="2">
-        <v>0.25</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B68" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B69" s="3"/>
+      <c r="A69" t="s">
+        <v>150</v>
+      </c>
+      <c r="B69" s="2">
+        <v>999999999</v>
+      </c>
     </row>
     <row r="70" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="B70" s="2">
-        <v>10000</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="B71" s="2">
-        <v>2500</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="B72" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B73" s="2">
-        <v>999999999</v>
+        <v>300</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="B74" s="2">
-        <v>0.04</v>
+        <v>100</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B75" s="2">
-        <v>0.01</v>
+        <v>999999</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="B76" s="2">
-        <v>1000</v>
+        <v>20</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B77" s="2">
-        <v>300</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B78" s="2">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="B79" s="2">
-        <v>999999</v>
+        <v>100</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="B80" s="2">
-        <v>20</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="B81" s="2">
-        <v>5</v>
+        <v>200</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="B82" s="2">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="B83" s="2">
-        <v>100</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="B84" s="2">
-        <v>2000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="B85" s="2">
-        <v>200</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="B86" s="2">
-        <v>100</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="B87" s="2">
-        <v>9999</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B88" s="2">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B89" s="2">
         <v>0.25</v>
@@ -1754,7 +1720,7 @@
     </row>
     <row r="90" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B90" s="2">
         <v>0.1</v>
@@ -1762,23 +1728,23 @@
     </row>
     <row r="91" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B91" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="B92" s="2">
-        <v>1.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="B93" s="2">
         <v>0.25</v>
@@ -1786,101 +1752,69 @@
     </row>
     <row r="94" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>186</v>
+        <v>146</v>
       </c>
       <c r="B94" s="2">
-        <v>0.1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>187</v>
-      </c>
-      <c r="B95" s="2">
-        <v>4</v>
-      </c>
+      <c r="A95" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B95" s="3"/>
     </row>
     <row r="96" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="B96" s="2">
-        <v>0.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="B97" s="2">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="B98" s="2">
-        <v>100</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="B99" s="3"/>
+      <c r="A99" t="s">
+        <v>179</v>
+      </c>
+      <c r="B99" s="2">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="100" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>191</v>
-      </c>
-      <c r="B100" s="2">
-        <v>0</v>
-      </c>
+      <c r="A100" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="B100" s="3"/>
     </row>
     <row r="101" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>192</v>
-      </c>
-      <c r="B101" s="2">
-        <v>0.5</v>
+        <v>181</v>
+      </c>
+      <c r="B101" s="3">
+        <v>1000000</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>193</v>
-      </c>
-      <c r="B102" s="2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
-        <v>194</v>
-      </c>
-      <c r="B103" s="2">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="B104" s="3"/>
-    </row>
-    <row r="105" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>196</v>
-      </c>
-      <c r="B105" s="3">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
-        <v>197</v>
-      </c>
-      <c r="B106" s="3">
+        <v>182</v>
+      </c>
+      <c r="B102" s="3">
         <v>0.5</v>
       </c>
     </row>
@@ -1894,9 +1828,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B57"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="N37" sqref="N37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1906,21 +1842,21 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3" s="3">
         <v>60</v>
@@ -1928,156 +1864,154 @@
     </row>
     <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B4" s="3">
-        <v>10000</v>
+        <v>250000</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B5" s="3">
-        <v>450</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B6" s="3">
-        <v>50</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B7" s="3">
         <f>B5+B6</f>
-        <v>500</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B8" s="3">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="3">
-        <v>100</v>
-      </c>
+      <c r="A9" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B10" s="3">
-        <v>12</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="3"/>
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B12" s="3">
-        <v>0.05</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B13" s="3">
-        <v>2</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="3">
-        <v>0.2</v>
-      </c>
+      <c r="A14" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B15" s="3">
-        <v>12</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B16" s="3">
-        <v>0.2</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" s="3"/>
-    </row>
-    <row r="20" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" s="3">
-        <v>0.01</v>
-      </c>
+      <c r="B20" s="3"/>
     </row>
     <row r="21" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B21" s="3">
-        <v>1000</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B22" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B23" s="3">
         <v>1</v>
@@ -2085,155 +2019,155 @@
     </row>
     <row r="24" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B24" s="3">
-        <v>0.25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B25" s="3">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B26" s="3">
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B27" s="3"/>
     </row>
     <row r="28" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B28" s="3">
-        <v>0.01</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B29" s="3">
-        <v>10</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B30" s="3">
-        <v>1</v>
+        <v>1.004</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B31" s="3">
-        <v>20</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B32" s="3">
-        <v>0.25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B33" s="3">
-        <v>100</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B34" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B35" s="3">
-        <v>0.25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B36" s="3"/>
+      <c r="A36" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B37" s="3">
-        <v>1.5</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>76</v>
-      </c>
-      <c r="B38" s="3">
-        <v>1.05</v>
-      </c>
+      <c r="A38" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="3"/>
     </row>
     <row r="39" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B39" s="3">
-        <v>1.004</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B40" s="3">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B41" s="3">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B42" s="3">
-        <v>24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B43" s="3">
         <v>10</v>
@@ -2241,109 +2175,39 @@
     </row>
     <row r="44" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B44" s="3">
-        <v>40</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" s="3">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46" s="3"/>
+    </row>
+    <row r="47" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>83</v>
       </c>
-      <c r="B45" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>84</v>
-      </c>
-      <c r="B46" s="3">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B47" s="3"/>
+      <c r="B47" s="3">
+        <v>-1E-3</v>
+      </c>
     </row>
     <row r="48" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B48" s="3">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>87</v>
-      </c>
-      <c r="B49" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>88</v>
-      </c>
-      <c r="B50" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>89</v>
-      </c>
-      <c r="B51" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>90</v>
-      </c>
-      <c r="B52" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>91</v>
-      </c>
-      <c r="B53" s="3">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>92</v>
-      </c>
-      <c r="B54" s="3">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B55" s="3"/>
-    </row>
-    <row r="56" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>94</v>
-      </c>
-      <c r="B56" s="3">
-        <v>-1E-3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>95</v>
-      </c>
-      <c r="B57" s="3">
         <v>1E-3</v>
       </c>
     </row>
@@ -2357,9 +2221,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2369,21 +2235,21 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="9"/>
     </row>
     <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="9">
         <v>0.1</v>
@@ -2391,7 +2257,7 @@
     </row>
     <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="9">
         <v>0.1</v>
@@ -2399,7 +2265,7 @@
     </row>
     <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B5" s="9">
         <v>0.1</v>
@@ -2407,7 +2273,7 @@
     </row>
     <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B6" s="9">
         <v>0.1</v>
@@ -2415,13 +2281,13 @@
     </row>
     <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B7" s="9"/>
     </row>
     <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" s="9">
         <v>0.1</v>
@@ -2429,7 +2295,7 @@
     </row>
     <row r="9" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B9" s="9">
         <v>0.1</v>
@@ -2437,7 +2303,7 @@
     </row>
     <row r="10" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" s="9">
         <v>0.1</v>
@@ -2445,29 +2311,29 @@
     </row>
     <row r="11" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" s="9">
         <v>0.2</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="9"/>
+      <c r="A12" t="s">
+        <v>184</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="13" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="9">
-        <v>0.1</v>
-      </c>
+      <c r="A13" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="9"/>
     </row>
     <row r="14" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B14" s="9">
         <v>0.1</v>
@@ -2475,7 +2341,7 @@
     </row>
     <row r="15" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B15" s="9">
         <v>0.1</v>
@@ -2483,10 +2349,26 @@
     </row>
     <row r="16" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B16" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="9">
         <v>0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>185</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>
@@ -2499,10 +2381,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2512,15 +2394,13 @@
     <col min="3" max="3" width="8.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2548,16 +2428,10 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>11</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
@@ -2575,24 +2449,18 @@
         <v>1</v>
       </c>
       <c r="G2" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H2" s="2">
         <v>0.1</v>
       </c>
       <c r="I2" s="1">
+        <v>96000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>10</v>
-      </c>
-      <c r="J2" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="K2" s="1">
-        <v>96000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>12</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -2610,24 +2478,18 @@
         <v>1</v>
       </c>
       <c r="G3" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H3" s="2">
         <v>0.1</v>
       </c>
       <c r="I3" s="1">
-        <v>10</v>
-      </c>
-      <c r="J3" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="K3" s="1">
         <v>35000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
@@ -2645,24 +2507,18 @@
         <v>1</v>
       </c>
       <c r="G4" s="1">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="H4" s="2">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="I4" s="1">
-        <v>20</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="K4" s="1">
         <v>48000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1">
         <v>3</v>
@@ -2680,24 +2536,18 @@
         <v>1</v>
       </c>
       <c r="G5" s="1">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="H5" s="2">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="I5" s="1">
-        <v>35</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="K5" s="1">
         <v>303000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1">
         <v>4</v>
@@ -2715,24 +2565,18 @@
         <v>1</v>
       </c>
       <c r="G6" s="1">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="H6" s="2">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="I6" s="1">
-        <v>35</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="K6" s="1">
         <v>56000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1">
         <v>5</v>
@@ -2750,24 +2594,18 @@
         <v>1</v>
       </c>
       <c r="G7" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H7" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I7" s="1">
-        <v>10</v>
-      </c>
-      <c r="J7" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="K7" s="1">
         <v>18000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1">
         <v>6</v>
@@ -2785,24 +2623,18 @@
         <v>1</v>
       </c>
       <c r="G8" s="1">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="H8" s="2">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="I8" s="1">
-        <v>50</v>
-      </c>
-      <c r="J8" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="K8" s="1">
         <v>111000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1">
         <v>7</v>
@@ -2820,24 +2652,18 @@
         <v>1</v>
       </c>
       <c r="G9" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H9" s="2">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="I9" s="1">
-        <v>10</v>
-      </c>
-      <c r="J9" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="K9" s="1">
         <v>19000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1">
         <v>8</v>
@@ -2855,24 +2681,18 @@
         <v>1</v>
       </c>
       <c r="G10" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H10" s="2">
         <v>0.1</v>
       </c>
       <c r="I10" s="1">
-        <v>5</v>
-      </c>
-      <c r="J10" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="K10" s="1">
         <v>112000</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1">
         <v>9</v>
@@ -2890,24 +2710,18 @@
         <v>1</v>
       </c>
       <c r="G11" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H11" s="2">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="I11" s="1">
-        <v>4</v>
-      </c>
-      <c r="J11" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="K11" s="1">
         <v>23000</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1">
         <v>10</v>
@@ -2925,24 +2739,18 @@
         <v>1</v>
       </c>
       <c r="G12" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H12" s="2">
         <v>0.1</v>
       </c>
       <c r="I12" s="1">
-        <v>10</v>
-      </c>
-      <c r="J12" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="K12" s="1">
         <v>112000</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1">
         <v>11</v>
@@ -2960,18 +2768,12 @@
         <v>1</v>
       </c>
       <c r="G13" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H13" s="2">
         <v>0.1</v>
       </c>
       <c r="I13" s="1">
-        <v>5</v>
-      </c>
-      <c r="J13" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="K13" s="1">
         <v>67000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Doing data analysis on final tests
</commit_message>
<xml_diff>
--- a/InitializationData/Simulation_Parameters.xlsx
+++ b/InitializationData/Simulation_Parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/fce19_ic_ac_uk/Documents/Programming/GithubRepos/Vulcan/InitializationData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feyzi\OneDrive - Imperial College London\Programming\GithubRepos\Vulcan\InitializationData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{387A20E8-C7D8-478B-BA3B-F4FFCA890BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BD75A61-5A93-481E-A395-D7446B510A69}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A09821A-165F-4922-AA3C-19E8E6A25C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2652" yWindow="2124" windowWidth="17280" windowHeight="8880" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initialization_Parameters" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="190">
   <si>
     <t>sector_name</t>
   </si>
@@ -137,6 +137,9 @@
     <t>firm_cons_rand_price_change_upper_limit</t>
   </si>
   <si>
+    <t>firm_cons_rand_wage_change</t>
+  </si>
+  <si>
     <t>Capital Firms</t>
   </si>
   <si>
@@ -149,6 +152,9 @@
     <t>firm_cap_rand_price_change_upper_limit</t>
   </si>
   <si>
+    <t>firm_cap_rand_wage_change</t>
+  </si>
+  <si>
     <t>Simulation Parameters</t>
   </si>
   <si>
@@ -476,93 +482,96 @@
     <t>firm_cons_init_quantity_sold_ratio</t>
   </si>
   <si>
+    <t>firm_cons_init_emissions_per_unit</t>
+  </si>
+  <si>
+    <t>firm_cap_init_cash_mean</t>
+  </si>
+  <si>
+    <t>firm_cap_init_cash_std</t>
+  </si>
+  <si>
+    <t>firm_cap_init_cash_min</t>
+  </si>
+  <si>
+    <t>firm_cap_init_cash_max</t>
+  </si>
+  <si>
+    <t>firm_cap_init_dividend_ratio_optimist</t>
+  </si>
+  <si>
+    <t>firm_cap_init_dividend_ratio_pessimist</t>
+  </si>
+  <si>
+    <t>firm_cap_init_wage_offer_mean</t>
+  </si>
+  <si>
+    <t>firm_cap_init_wage_offer_std</t>
+  </si>
+  <si>
+    <t>firm_cap_init_wage_offer_min</t>
+  </si>
+  <si>
+    <t>firm_cap_init_wage_offer_max</t>
+  </si>
+  <si>
+    <t>firm_cap_init_worker_demand_mean</t>
+  </si>
+  <si>
+    <t>firm_cap_init_worker_demand_std</t>
+  </si>
+  <si>
+    <t>firm_cap_init_worker_demand_min</t>
+  </si>
+  <si>
+    <t>firm_cap_init_worker_demand_max</t>
+  </si>
+  <si>
+    <t>firm_cap_init_good_price_mean</t>
+  </si>
+  <si>
+    <t>firm_cap_init_good_price_std</t>
+  </si>
+  <si>
+    <t>firm_cap_init_good_price_min</t>
+  </si>
+  <si>
+    <t>firm_cap_init_good_price_max</t>
+  </si>
+  <si>
+    <t>firm_cap_init_inv_factor_mean</t>
+  </si>
+  <si>
+    <t>firm_cap_init_inv_factor_std</t>
+  </si>
+  <si>
+    <t>firm_cap_init_inv_factor_min</t>
+  </si>
+  <si>
+    <t>firm_cap_init_inv_factor_max</t>
+  </si>
+  <si>
+    <t>firm_cap_init_target_inv_factor_mean</t>
+  </si>
+  <si>
+    <t>firm_cap_init_target_inv_factor_std</t>
+  </si>
+  <si>
+    <t>firm_cap_init_target_inv_factor_min</t>
+  </si>
+  <si>
+    <t>firm_cap_init_target_inv_factor_max</t>
+  </si>
+  <si>
+    <t>firm_cap_init_production_current_ratio</t>
+  </si>
+  <si>
+    <t>firm_cap_init_quantity_sold_ratio</t>
+  </si>
+  <si>
     <t>firm_cap_init_emissions_per_unit</t>
   </si>
   <si>
-    <t>firm_cap_init_cash_mean</t>
-  </si>
-  <si>
-    <t>firm_cap_init_cash_std</t>
-  </si>
-  <si>
-    <t>firm_cap_init_cash_min</t>
-  </si>
-  <si>
-    <t>firm_cap_init_cash_max</t>
-  </si>
-  <si>
-    <t>firm_cap_init_dividend_ratio_optimist</t>
-  </si>
-  <si>
-    <t>firm_cap_init_dividend_ratio_pessimist</t>
-  </si>
-  <si>
-    <t>firm_cap_init_wage_offer_mean</t>
-  </si>
-  <si>
-    <t>firm_cap_init_wage_offer_std</t>
-  </si>
-  <si>
-    <t>firm_cap_init_wage_offer_min</t>
-  </si>
-  <si>
-    <t>firm_cap_init_wage_offer_max</t>
-  </si>
-  <si>
-    <t>firm_cap_init_worker_demand_mean</t>
-  </si>
-  <si>
-    <t>firm_cap_init_worker_demand_std</t>
-  </si>
-  <si>
-    <t>firm_cap_init_worker_demand_min</t>
-  </si>
-  <si>
-    <t>firm_cap_init_worker_demand_max</t>
-  </si>
-  <si>
-    <t>firm_cap_init_good_price_mean</t>
-  </si>
-  <si>
-    <t>firm_cap_init_good_price_std</t>
-  </si>
-  <si>
-    <t>firm_cap_init_good_price_min</t>
-  </si>
-  <si>
-    <t>firm_cap_init_good_price_max</t>
-  </si>
-  <si>
-    <t>firm_cap_init_inv_factor_mean</t>
-  </si>
-  <si>
-    <t>firm_cap_init_inv_factor_std</t>
-  </si>
-  <si>
-    <t>firm_cap_init_inv_factor_min</t>
-  </si>
-  <si>
-    <t>firm_cap_init_inv_factor_max</t>
-  </si>
-  <si>
-    <t>firm_cap_init_target_inv_factor_mean</t>
-  </si>
-  <si>
-    <t>firm_cap_init_target_inv_factor_std</t>
-  </si>
-  <si>
-    <t>firm_cap_init_target_inv_factor_min</t>
-  </si>
-  <si>
-    <t>firm_cap_init_target_inv_factor_max</t>
-  </si>
-  <si>
-    <t>firm_cap_init_production_current_ratio</t>
-  </si>
-  <si>
-    <t>firm_cap_init_quantity_sold_ratio</t>
-  </si>
-  <si>
     <t>CO2 Emission Sensitivities</t>
   </si>
   <si>
@@ -587,13 +596,16 @@
     <t>emission_init_unit_price</t>
   </si>
   <si>
-    <t>firm_cons_init_emissions_per_unit</t>
-  </si>
-  <si>
-    <t>firm_cons_rand_wage_change</t>
-  </si>
-  <si>
-    <t>firm_cap_rand_wage_change</t>
+    <t>firm_cap_fixed_wage_change</t>
+  </si>
+  <si>
+    <t>firm_cap_fixed_price_change</t>
+  </si>
+  <si>
+    <t>firm_cons_fixed_wage_change</t>
+  </si>
+  <si>
+    <t>firm_cons_fixed_price_change</t>
   </si>
 </sst>
 </file>
@@ -653,7 +665,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -676,22 +688,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1004,9 +1007,7 @@
   </sheetPr>
   <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1016,21 +1017,21 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B3" s="2">
         <v>0.02</v>
@@ -1044,7 +1045,7 @@
     </row>
     <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B5" s="2">
         <v>0.5</v>
@@ -1052,7 +1053,7 @@
     </row>
     <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B6" s="2">
         <v>0.1</v>
@@ -1060,7 +1061,7 @@
     </row>
     <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B7" s="2">
         <v>0.1</v>
@@ -1068,7 +1069,7 @@
     </row>
     <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B8" s="2">
         <v>0.9</v>
@@ -1076,7 +1077,7 @@
     </row>
     <row r="9" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B9" s="2">
         <v>0.3</v>
@@ -1084,7 +1085,7 @@
     </row>
     <row r="10" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B10" s="2">
         <v>0.05</v>
@@ -1092,7 +1093,7 @@
     </row>
     <row r="11" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B11" s="2">
         <v>0</v>
@@ -1100,7 +1101,7 @@
     </row>
     <row r="12" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B12" s="2">
         <v>0.7</v>
@@ -1108,7 +1109,7 @@
     </row>
     <row r="13" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B13" s="2">
         <v>0.2</v>
@@ -1116,7 +1117,7 @@
     </row>
     <row r="14" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B14" s="2">
         <v>0.05</v>
@@ -1124,7 +1125,7 @@
     </row>
     <row r="15" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B15" s="2">
         <v>0</v>
@@ -1132,7 +1133,7 @@
     </row>
     <row r="16" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B16" s="2">
         <v>0.5</v>
@@ -1140,7 +1141,7 @@
     </row>
     <row r="17" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B17" s="2">
         <v>0.3</v>
@@ -1148,7 +1149,7 @@
     </row>
     <row r="18" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B18" s="2">
         <v>0.05</v>
@@ -1156,7 +1157,7 @@
     </row>
     <row r="19" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B19" s="2">
         <v>0.1</v>
@@ -1164,7 +1165,7 @@
     </row>
     <row r="20" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B20" s="2">
         <v>0.6</v>
@@ -1172,7 +1173,7 @@
     </row>
     <row r="21" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B21" s="2">
         <v>1000</v>
@@ -1180,7 +1181,7 @@
     </row>
     <row r="22" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B22" s="2">
         <v>300</v>
@@ -1188,7 +1189,7 @@
     </row>
     <row r="23" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B23" s="2">
         <v>0</v>
@@ -1196,7 +1197,7 @@
     </row>
     <row r="24" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B24" s="2">
         <v>2000</v>
@@ -1204,7 +1205,7 @@
     </row>
     <row r="25" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B25" s="2">
         <v>4</v>
@@ -1212,7 +1213,7 @@
     </row>
     <row r="26" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B26" s="2">
         <v>2</v>
@@ -1220,7 +1221,7 @@
     </row>
     <row r="27" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B27" s="2">
         <v>0</v>
@@ -1228,7 +1229,7 @@
     </row>
     <row r="28" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B28" s="2">
         <v>100</v>
@@ -1236,7 +1237,7 @@
     </row>
     <row r="29" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B29" s="2">
         <v>950</v>
@@ -1244,7 +1245,7 @@
     </row>
     <row r="30" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B30" s="2">
         <v>300</v>
@@ -1252,7 +1253,7 @@
     </row>
     <row r="31" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B31" s="2">
         <v>100</v>
@@ -1260,7 +1261,7 @@
     </row>
     <row r="32" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B32" s="2">
         <v>999999</v>
@@ -1268,7 +1269,7 @@
     </row>
     <row r="33" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B33" s="2">
         <v>500</v>
@@ -1276,7 +1277,7 @@
     </row>
     <row r="34" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B34" s="2">
         <v>600</v>
@@ -1290,7 +1291,7 @@
     </row>
     <row r="36" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B36" s="2">
         <v>10000</v>
@@ -1298,7 +1299,7 @@
     </row>
     <row r="37" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B37" s="2">
         <v>2500</v>
@@ -1306,7 +1307,7 @@
     </row>
     <row r="38" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B38" s="2">
         <v>1</v>
@@ -1314,7 +1315,7 @@
     </row>
     <row r="39" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B39" s="2">
         <v>999999999</v>
@@ -1322,7 +1323,7 @@
     </row>
     <row r="40" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B40" s="2">
         <v>0.01</v>
@@ -1330,7 +1331,7 @@
     </row>
     <row r="41" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B41" s="2">
         <v>5.0000000000000001E-3</v>
@@ -1338,7 +1339,7 @@
     </row>
     <row r="42" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B42" s="2">
         <v>1000</v>
@@ -1346,7 +1347,7 @@
     </row>
     <row r="43" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B43" s="2">
         <v>300</v>
@@ -1354,7 +1355,7 @@
     </row>
     <row r="44" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B44" s="2">
         <v>100</v>
@@ -1362,7 +1363,7 @@
     </row>
     <row r="45" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B45" s="2">
         <v>999999</v>
@@ -1370,7 +1371,7 @@
     </row>
     <row r="46" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B46" s="2">
         <v>20</v>
@@ -1378,7 +1379,7 @@
     </row>
     <row r="47" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B47" s="2">
         <v>5</v>
@@ -1386,7 +1387,7 @@
     </row>
     <row r="48" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B48" s="2">
         <v>1</v>
@@ -1394,7 +1395,7 @@
     </row>
     <row r="49" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B49" s="2">
         <v>100</v>
@@ -1402,7 +1403,7 @@
     </row>
     <row r="50" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B50" s="2">
         <v>10</v>
@@ -1410,15 +1411,15 @@
     </row>
     <row r="51" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>133</v>
-      </c>
-      <c r="B51" s="14">
+        <v>135</v>
+      </c>
+      <c r="B51" s="11">
         <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B52" s="2">
         <v>1</v>
@@ -1426,7 +1427,7 @@
     </row>
     <row r="53" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B53" s="2">
         <v>99</v>
@@ -1434,7 +1435,7 @@
     </row>
     <row r="54" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B54" s="2">
         <v>2</v>
@@ -1442,7 +1443,7 @@
     </row>
     <row r="55" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B55" s="2">
         <v>0.25</v>
@@ -1450,7 +1451,7 @@
     </row>
     <row r="56" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B56" s="2">
         <v>0.5</v>
@@ -1458,7 +1459,7 @@
     </row>
     <row r="57" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B57" s="2">
         <v>2</v>
@@ -1466,7 +1467,7 @@
     </row>
     <row r="58" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B58" s="2">
         <v>5</v>
@@ -1474,7 +1475,7 @@
     </row>
     <row r="59" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B59" s="2">
         <v>0.25</v>
@@ -1482,7 +1483,7 @@
     </row>
     <row r="60" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B60" s="2">
         <v>0.1</v>
@@ -1490,7 +1491,7 @@
     </row>
     <row r="61" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B61" s="2">
         <v>10</v>
@@ -1498,7 +1499,7 @@
     </row>
     <row r="62" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B62" s="2">
         <v>0.4</v>
@@ -1506,7 +1507,7 @@
     </row>
     <row r="63" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B63" s="2">
         <v>0.25</v>
@@ -1514,7 +1515,7 @@
     </row>
     <row r="64" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>183</v>
+        <v>148</v>
       </c>
       <c r="B64" s="2">
         <v>10</v>
@@ -1522,13 +1523,13 @@
     </row>
     <row r="65" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B65" s="3"/>
     </row>
     <row r="66" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B66" s="2">
         <v>10000</v>
@@ -1536,7 +1537,7 @@
     </row>
     <row r="67" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B67" s="2">
         <v>2500</v>
@@ -1544,7 +1545,7 @@
     </row>
     <row r="68" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B68" s="2">
         <v>1</v>
@@ -1552,7 +1553,7 @@
     </row>
     <row r="69" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B69" s="2">
         <v>999999999</v>
@@ -1560,7 +1561,7 @@
     </row>
     <row r="70" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B70" s="2">
         <v>0.04</v>
@@ -1568,7 +1569,7 @@
     </row>
     <row r="71" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B71" s="2">
         <v>0.01</v>
@@ -1576,7 +1577,7 @@
     </row>
     <row r="72" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B72" s="2">
         <v>1000</v>
@@ -1584,7 +1585,7 @@
     </row>
     <row r="73" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B73" s="2">
         <v>300</v>
@@ -1592,7 +1593,7 @@
     </row>
     <row r="74" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B74" s="2">
         <v>100</v>
@@ -1600,7 +1601,7 @@
     </row>
     <row r="75" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B75" s="2">
         <v>999999</v>
@@ -1608,7 +1609,7 @@
     </row>
     <row r="76" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B76" s="2">
         <v>20</v>
@@ -1616,7 +1617,7 @@
     </row>
     <row r="77" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B77" s="2">
         <v>5</v>
@@ -1624,7 +1625,7 @@
     </row>
     <row r="78" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B78" s="2">
         <v>1</v>
@@ -1632,7 +1633,7 @@
     </row>
     <row r="79" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B79" s="2">
         <v>100</v>
@@ -1640,7 +1641,7 @@
     </row>
     <row r="80" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B80" s="2">
         <v>2000</v>
@@ -1648,7 +1649,7 @@
     </row>
     <row r="81" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B81" s="2">
         <v>200</v>
@@ -1656,7 +1657,7 @@
     </row>
     <row r="82" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B82" s="2">
         <v>100</v>
@@ -1664,7 +1665,7 @@
     </row>
     <row r="83" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B83" s="2">
         <v>9999</v>
@@ -1672,7 +1673,7 @@
     </row>
     <row r="84" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B84" s="2">
         <v>1</v>
@@ -1680,7 +1681,7 @@
     </row>
     <row r="85" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B85" s="2">
         <v>0.25</v>
@@ -1688,7 +1689,7 @@
     </row>
     <row r="86" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B86" s="2">
         <v>0.1</v>
@@ -1696,7 +1697,7 @@
     </row>
     <row r="87" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B87" s="2">
         <v>2</v>
@@ -1704,7 +1705,7 @@
     </row>
     <row r="88" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B88" s="2">
         <v>1.5</v>
@@ -1712,7 +1713,7 @@
     </row>
     <row r="89" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B89" s="2">
         <v>0.25</v>
@@ -1720,7 +1721,7 @@
     </row>
     <row r="90" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B90" s="2">
         <v>0.1</v>
@@ -1728,7 +1729,7 @@
     </row>
     <row r="91" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B91" s="2">
         <v>4</v>
@@ -1736,7 +1737,7 @@
     </row>
     <row r="92" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B92" s="2">
         <v>0.4</v>
@@ -1744,7 +1745,7 @@
     </row>
     <row r="93" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B93" s="2">
         <v>0.25</v>
@@ -1752,7 +1753,7 @@
     </row>
     <row r="94" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>146</v>
+        <v>177</v>
       </c>
       <c r="B94" s="2">
         <v>100</v>
@@ -1760,13 +1761,13 @@
     </row>
     <row r="95" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="7" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B95" s="3"/>
     </row>
     <row r="96" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B96" s="2">
         <v>0</v>
@@ -1774,7 +1775,7 @@
     </row>
     <row r="97" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B97" s="2">
         <v>0.5</v>
@@ -1782,7 +1783,7 @@
     </row>
     <row r="98" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B98" s="2">
         <v>0.1</v>
@@ -1790,7 +1791,7 @@
     </row>
     <row r="99" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B99" s="2">
         <v>0.05</v>
@@ -1798,13 +1799,13 @@
     </row>
     <row r="100" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="7" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B100" s="3"/>
     </row>
     <row r="101" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B101" s="3">
         <v>1000000</v>
@@ -1812,7 +1813,7 @@
     </row>
     <row r="102" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B102" s="3">
         <v>0.5</v>
@@ -1828,10 +1829,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="N37" sqref="N37"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1842,21 +1843,21 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B3" s="3">
         <v>60</v>
@@ -1864,40 +1865,40 @@
     </row>
     <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B4" s="3">
-        <v>250000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B5" s="3">
-        <v>10000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B6" s="3">
-        <v>2000</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B7" s="3">
         <f>B5+B6</f>
-        <v>12000</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B8" s="3">
         <v>12</v>
@@ -1905,13 +1906,13 @@
     </row>
     <row r="9" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B10" s="3">
         <v>0.05</v>
@@ -1919,7 +1920,7 @@
     </row>
     <row r="11" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B11" s="3">
         <v>2</v>
@@ -1927,7 +1928,7 @@
     </row>
     <row r="12" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B12" s="3">
         <v>12</v>
@@ -1935,7 +1936,7 @@
     </row>
     <row r="13" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B13" s="3">
         <v>0.2</v>
@@ -1943,13 +1944,13 @@
     </row>
     <row r="14" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B15" s="3">
         <v>0.01</v>
@@ -1957,7 +1958,7 @@
     </row>
     <row r="16" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B16" s="3">
         <v>1000</v>
@@ -1965,7 +1966,7 @@
     </row>
     <row r="17" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B17" s="3">
         <v>1</v>
@@ -1973,7 +1974,7 @@
     </row>
     <row r="18" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B18" s="3">
         <v>1</v>
@@ -1981,40 +1982,40 @@
     </row>
     <row r="19" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B19" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" s="3"/>
+      <c r="A20" t="s">
+        <v>188</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="21" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>189</v>
       </c>
       <c r="B21" s="3">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="3">
-        <v>10</v>
-      </c>
+      <c r="B22" s="3"/>
     </row>
     <row r="23" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>59</v>
       </c>
       <c r="B23" s="3">
-        <v>1</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2022,7 +2023,7 @@
         <v>60</v>
       </c>
       <c r="B24" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2030,7 +2031,7 @@
         <v>61</v>
       </c>
       <c r="B25" s="3">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2038,176 +2039,208 @@
         <v>62</v>
       </c>
       <c r="B26" s="3">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
+      <c r="A27" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="3"/>
+      <c r="B27" s="3">
+        <v>100</v>
+      </c>
     </row>
     <row r="28" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>64</v>
       </c>
       <c r="B28" s="3">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>186</v>
       </c>
       <c r="B29" s="3">
-        <v>1.05</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>66</v>
+        <v>187</v>
       </c>
       <c r="B30" s="3">
-        <v>1.004</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>67</v>
-      </c>
-      <c r="B31" s="3">
-        <v>0.1</v>
-      </c>
+      <c r="A31" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="3"/>
     </row>
     <row r="32" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B32" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B33" s="3">
-        <v>24</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B34" s="3">
-        <v>10</v>
+        <v>1.002</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B35" s="3">
-        <v>40</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B36" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B37" s="3">
-        <v>0.05</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B38" s="3"/>
+      <c r="A38" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="39" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B39" s="3">
-        <v>0.02</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B40" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B41" s="3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>78</v>
-      </c>
-      <c r="B42" s="3">
-        <v>1</v>
-      </c>
+      <c r="A42" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" s="3"/>
     </row>
     <row r="43" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B43" s="3">
-        <v>10</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B44" s="3">
-        <v>1000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B45" s="3">
-        <v>100000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B46" s="3"/>
+      <c r="A46" t="s">
+        <v>80</v>
+      </c>
+      <c r="B46" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="47" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B47" s="3">
-        <v>-1E-3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>82</v>
+      </c>
+      <c r="B48" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>83</v>
+      </c>
+      <c r="B49" s="3">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B50" s="3"/>
+    </row>
+    <row r="51" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>85</v>
+      </c>
+      <c r="B51" s="3">
+        <v>-1E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>86</v>
+      </c>
+      <c r="B52" s="3">
         <v>1E-3</v>
       </c>
     </row>
@@ -2223,14 +2256,12 @@
   </sheetPr>
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2275,8 +2306,8 @@
       <c r="A6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="9">
-        <v>0.1</v>
+      <c r="B6" s="2">
+        <v>0.25</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2314,12 +2345,12 @@
         <v>32</v>
       </c>
       <c r="B11" s="9">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>184</v>
+        <v>33</v>
       </c>
       <c r="B12" s="3">
         <v>0.25</v>
@@ -2327,7 +2358,7 @@
     </row>
     <row r="13" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B13" s="9"/>
     </row>
@@ -2341,7 +2372,7 @@
     </row>
     <row r="15" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B15" s="9">
         <v>0.1</v>
@@ -2349,7 +2380,7 @@
     </row>
     <row r="16" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B16" s="9">
         <v>0.1</v>
@@ -2357,15 +2388,15 @@
     </row>
     <row r="17" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B17" s="9">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>185</v>
+        <v>38</v>
       </c>
       <c r="B18" s="3">
         <v>0.25</v>
@@ -2383,9 +2414,7 @@
   </sheetPr>
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2440,10 +2469,10 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="D2" s="3">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E2" s="1">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
@@ -2472,7 +2501,7 @@
         <v>0.01</v>
       </c>
       <c r="E3" s="1">
-        <v>40</v>
+        <v>1000</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
@@ -2501,7 +2530,7 @@
         <v>0.01</v>
       </c>
       <c r="E4" s="1">
-        <v>50</v>
+        <v>1000</v>
       </c>
       <c r="F4" s="1">
         <v>1</v>
@@ -2530,7 +2559,7 @@
         <v>0.01</v>
       </c>
       <c r="E5" s="1">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
@@ -2559,7 +2588,7 @@
         <v>0.01</v>
       </c>
       <c r="E6" s="1">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="F6" s="1">
         <v>1</v>
@@ -2588,7 +2617,7 @@
         <v>0.01</v>
       </c>
       <c r="E7" s="1">
-        <v>20</v>
+        <v>1000</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
@@ -2617,7 +2646,7 @@
         <v>0.01</v>
       </c>
       <c r="E8" s="1">
-        <v>110</v>
+        <v>1000</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
@@ -2646,7 +2675,7 @@
         <v>0.01</v>
       </c>
       <c r="E9" s="1">
-        <v>20</v>
+        <v>1000</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
@@ -2675,7 +2704,7 @@
         <v>0.01</v>
       </c>
       <c r="E10" s="1">
-        <v>110</v>
+        <v>1000</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
@@ -2704,7 +2733,7 @@
         <v>0.01</v>
       </c>
       <c r="E11" s="1">
-        <v>20</v>
+        <v>1000</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
@@ -2733,7 +2762,7 @@
         <v>0.01</v>
       </c>
       <c r="E12" s="1">
-        <v>110</v>
+        <v>1000</v>
       </c>
       <c r="F12" s="1">
         <v>1</v>
@@ -2762,7 +2791,7 @@
         <v>0.01</v>
       </c>
       <c r="E13" s="1">
-        <v>70</v>
+        <v>1000</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Redid some incorrectly printed plots
</commit_message>
<xml_diff>
--- a/InitializationData/Simulation_Parameters.xlsx
+++ b/InitializationData/Simulation_Parameters.xlsx
@@ -1,18 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/fce19_ic_ac_uk/Documents/Programming/GithubRepos/Vulcan/InitializationData/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_EE291FE4B8DF1A7D7E20D92DF1FC1D0C932140A8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{369CB2D7-6B64-4A74-892C-FE8FB32B0A16}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="3"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Initialization_Parameters"/>
-    <sheet r:id="rId2" sheetId="2" name="Main_Loop_Parameters"/>
-    <sheet r:id="rId3" sheetId="3" name="Randomness_Parameters"/>
-    <sheet r:id="rId4" sheetId="4" name="Consumer_Firm_Sectors"/>
+    <sheet name="Initialization_Parameters" sheetId="1" r:id="rId1"/>
+    <sheet name="Main_Loop_Parameters" sheetId="2" r:id="rId2"/>
+    <sheet name="Randomness_Parameters" sheetId="3" r:id="rId3"/>
+    <sheet name="Consumer_Firm_Sectors" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -580,7 +599,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
@@ -634,56 +653,53 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -694,10 +710,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -735,71 +751,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -827,7 +843,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -850,11 +866,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -863,13 +879,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -879,7 +895,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -888,7 +904,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -897,7 +913,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -905,10 +921,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -973,821 +989,823 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="41.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="41.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="1" t="s">
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>0.02</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="1" t="s">
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>0.9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>94</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>0.3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>95</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>0.05</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>96</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>97</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>0.7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>98</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>0.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>99</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>0.05</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>100</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>101</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>102</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>0.3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>103</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>0.05</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>104</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>105</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="2">
         <v>0.6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>106</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>107</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>300</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>108</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>109</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <v>2000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>110</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="2">
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>111</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="2">
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>112</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="2">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>113</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="2">
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>114</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="2">
         <v>950</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>115</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="2">
         <v>300</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>116</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="2">
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>117</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="2">
         <v>999999</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>118</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="2">
         <v>500</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>119</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="2">
         <v>600</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
-      <c r="A35" s="9" t="s">
+    <row r="35" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
-      <c r="A36" s="1" t="s">
+      <c r="B35" s="3"/>
+    </row>
+    <row r="36" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>120</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="2">
         <v>10000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>121</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="2">
         <v>2500</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>122</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="2">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>123</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="2">
         <v>999999999</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>124</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="2">
         <v>0.01</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>125</v>
       </c>
-      <c r="B41" s="3">
-        <v>0.005</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
-      <c r="A42" s="1" t="s">
+      <c r="B41" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>126</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>127</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="2">
         <v>300</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>128</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="2">
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>129</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45" s="2">
         <v>999999</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
-      <c r="A46" s="1" t="s">
+    <row r="46" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>130</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="2">
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
-      <c r="A47" s="1" t="s">
+    <row r="47" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>131</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="2">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
-      <c r="A48" s="1" t="s">
+    <row r="48" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>132</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="2">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
-      <c r="A49" s="1" t="s">
+    <row r="49" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>133</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="2">
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
-      <c r="A50" s="1" t="s">
+    <row r="50" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>134</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="2">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>135</v>
       </c>
-      <c r="B51" s="13">
+      <c r="B51" s="11">
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
-      <c r="A52" s="1" t="s">
+    <row r="52" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>136</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B52" s="2">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
-      <c r="A53" s="1" t="s">
+    <row r="53" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>137</v>
       </c>
-      <c r="B53" s="3">
+      <c r="B53" s="2">
         <v>99</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>138</v>
       </c>
-      <c r="B54" s="3">
+      <c r="B54" s="2">
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
-      <c r="A55" s="1" t="s">
+    <row r="55" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>139</v>
       </c>
-      <c r="B55" s="3">
+      <c r="B55" s="2">
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
-      <c r="A56" s="1" t="s">
+    <row r="56" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>140</v>
       </c>
-      <c r="B56" s="3">
+      <c r="B56" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
-      <c r="A57" s="1" t="s">
+    <row r="57" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>141</v>
       </c>
-      <c r="B57" s="3">
+      <c r="B57" s="2">
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
-      <c r="A58" s="1" t="s">
+    <row r="58" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>142</v>
       </c>
-      <c r="B58" s="3">
+      <c r="B58" s="2">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
-      <c r="A59" s="1" t="s">
+    <row r="59" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>143</v>
       </c>
-      <c r="B59" s="3">
+      <c r="B59" s="2">
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
-      <c r="A60" s="1" t="s">
+    <row r="60" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>144</v>
       </c>
-      <c r="B60" s="3">
+      <c r="B60" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
-      <c r="A61" s="1" t="s">
+    <row r="61" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>145</v>
       </c>
-      <c r="B61" s="3">
+      <c r="B61" s="2">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
-      <c r="A62" s="1" t="s">
+    <row r="62" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>146</v>
       </c>
-      <c r="B62" s="3">
+      <c r="B62" s="2">
         <v>0.4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5">
-      <c r="A63" s="1" t="s">
+    <row r="63" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>147</v>
       </c>
-      <c r="B63" s="3">
+      <c r="B63" s="2">
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
-      <c r="A64" s="1" t="s">
+    <row r="64" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>148</v>
       </c>
-      <c r="B64" s="3">
+      <c r="B64" s="2">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5">
-      <c r="A65" s="9" t="s">
+    <row r="65" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B65" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="19.5">
-      <c r="A66" s="1" t="s">
+      <c r="B65" s="3"/>
+    </row>
+    <row r="66" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>149</v>
       </c>
-      <c r="B66" s="3">
+      <c r="B66" s="2">
         <v>10000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="19.5">
-      <c r="A67" s="1" t="s">
+    <row r="67" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>150</v>
       </c>
-      <c r="B67" s="3">
+      <c r="B67" s="2">
         <v>2500</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="19.5">
-      <c r="A68" s="1" t="s">
+    <row r="68" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>151</v>
       </c>
-      <c r="B68" s="3">
+      <c r="B68" s="2">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="19.5">
-      <c r="A69" s="1" t="s">
+    <row r="69" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>152</v>
       </c>
-      <c r="B69" s="3">
+      <c r="B69" s="2">
         <v>999999999</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="19.5">
-      <c r="A70" s="1" t="s">
+    <row r="70" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
         <v>153</v>
       </c>
-      <c r="B70" s="3">
+      <c r="B70" s="2">
         <v>0.04</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="19.5">
-      <c r="A71" s="1" t="s">
+    <row r="71" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
         <v>154</v>
       </c>
-      <c r="B71" s="3">
+      <c r="B71" s="2">
         <v>0.01</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="19.5">
-      <c r="A72" s="1" t="s">
+    <row r="72" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
         <v>155</v>
       </c>
-      <c r="B72" s="3">
+      <c r="B72" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="19.5">
-      <c r="A73" s="1" t="s">
+    <row r="73" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
         <v>156</v>
       </c>
-      <c r="B73" s="3">
+      <c r="B73" s="2">
         <v>300</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="19.5">
-      <c r="A74" s="1" t="s">
+    <row r="74" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>157</v>
       </c>
-      <c r="B74" s="3">
+      <c r="B74" s="2">
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="19.5">
-      <c r="A75" s="1" t="s">
+    <row r="75" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>158</v>
       </c>
-      <c r="B75" s="3">
+      <c r="B75" s="2">
         <v>999999</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="19.5">
-      <c r="A76" s="1" t="s">
+    <row r="76" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
         <v>159</v>
       </c>
-      <c r="B76" s="3">
+      <c r="B76" s="2">
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="19.5">
-      <c r="A77" s="1" t="s">
+    <row r="77" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
         <v>160</v>
       </c>
-      <c r="B77" s="3">
+      <c r="B77" s="2">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="19.5">
-      <c r="A78" s="1" t="s">
+    <row r="78" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>161</v>
       </c>
-      <c r="B78" s="3">
+      <c r="B78" s="2">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="19.5">
-      <c r="A79" s="1" t="s">
+    <row r="79" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
         <v>162</v>
       </c>
-      <c r="B79" s="3">
+      <c r="B79" s="2">
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="19.5">
-      <c r="A80" s="1" t="s">
+    <row r="80" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>163</v>
       </c>
-      <c r="B80" s="3">
+      <c r="B80" s="2">
         <v>2000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="19.5">
-      <c r="A81" s="1" t="s">
+    <row r="81" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
         <v>164</v>
       </c>
-      <c r="B81" s="3">
+      <c r="B81" s="2">
         <v>200</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="19.5">
-      <c r="A82" s="1" t="s">
+    <row r="82" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
         <v>165</v>
       </c>
-      <c r="B82" s="3">
+      <c r="B82" s="2">
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="19.5">
-      <c r="A83" s="1" t="s">
+    <row r="83" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
         <v>166</v>
       </c>
-      <c r="B83" s="3">
+      <c r="B83" s="2">
         <v>9999</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="19.5">
-      <c r="A84" s="1" t="s">
+    <row r="84" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
         <v>167</v>
       </c>
-      <c r="B84" s="3">
+      <c r="B84" s="2">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="19.5">
-      <c r="A85" s="1" t="s">
+    <row r="85" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
         <v>168</v>
       </c>
-      <c r="B85" s="3">
+      <c r="B85" s="2">
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="19.5">
-      <c r="A86" s="1" t="s">
+    <row r="86" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>169</v>
       </c>
-      <c r="B86" s="3">
+      <c r="B86" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="19.5">
-      <c r="A87" s="1" t="s">
+    <row r="87" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
         <v>170</v>
       </c>
-      <c r="B87" s="3">
+      <c r="B87" s="2">
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="19.5">
-      <c r="A88" s="1" t="s">
+    <row r="88" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>171</v>
       </c>
-      <c r="B88" s="3">
+      <c r="B88" s="2">
         <v>1.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="19.5">
-      <c r="A89" s="1" t="s">
+    <row r="89" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
         <v>172</v>
       </c>
-      <c r="B89" s="3">
+      <c r="B89" s="2">
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="19.5">
-      <c r="A90" s="1" t="s">
+    <row r="90" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
         <v>173</v>
       </c>
-      <c r="B90" s="3">
+      <c r="B90" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="19.5">
-      <c r="A91" s="1" t="s">
+    <row r="91" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
         <v>174</v>
       </c>
-      <c r="B91" s="3">
+      <c r="B91" s="2">
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="19.5">
-      <c r="A92" s="1" t="s">
+    <row r="92" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
         <v>175</v>
       </c>
-      <c r="B92" s="3">
+      <c r="B92" s="2">
         <v>0.4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="19.5">
-      <c r="A93" s="1" t="s">
+    <row r="93" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
         <v>176</v>
       </c>
-      <c r="B93" s="3">
+      <c r="B93" s="2">
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="19.5">
-      <c r="A94" s="1" t="s">
+    <row r="94" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
         <v>177</v>
       </c>
-      <c r="B94" s="3">
+      <c r="B94" s="2">
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="19.5">
-      <c r="A95" s="9" t="s">
+    <row r="95" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="B95" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="19.5">
-      <c r="A96" s="1" t="s">
+      <c r="B95" s="3"/>
+    </row>
+    <row r="96" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
         <v>179</v>
       </c>
-      <c r="B96" s="3">
+      <c r="B96" s="2">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="19.5">
-      <c r="A97" s="1" t="s">
+    <row r="97" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
         <v>180</v>
       </c>
-      <c r="B97" s="3">
+      <c r="B97" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="19.5">
-      <c r="A98" s="1" t="s">
+    <row r="98" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
         <v>181</v>
       </c>
-      <c r="B98" s="3">
+      <c r="B98" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="19.5">
-      <c r="A99" s="1" t="s">
+    <row r="99" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
         <v>182</v>
       </c>
-      <c r="B99" s="3">
+      <c r="B99" s="2">
         <v>0.05</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="19.5">
-      <c r="A100" s="9" t="s">
+    <row r="100" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="B100" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="19.5">
-      <c r="A101" s="1" t="s">
+      <c r="B100" s="3"/>
+    </row>
+    <row r="101" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
         <v>184</v>
       </c>
-      <c r="B101" s="4">
+      <c r="B101" s="3">
         <v>1000000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="19.5">
-      <c r="A102" s="1" t="s">
+    <row r="102" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
         <v>185</v>
       </c>
-      <c r="B102" s="4">
+      <c r="B102" s="3">
         <v>0.5</v>
       </c>
     </row>
@@ -1797,388 +1815,391 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection sqref="A1:B42"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="39.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="39.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="1" t="s">
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>60</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="4">
-        <v>50000</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="1" t="s">
+      <c r="B4" s="3">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="4">
-        <v>1500</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="1" t="s">
+      <c r="B5" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="4">
-        <v>250</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="1" t="s">
+      <c r="B6" s="3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <f>B5+B6</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="1" t="s">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="1" t="s">
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>0.05</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>0.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="1" t="s">
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>0.01</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="3">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
-      <c r="A20" s="9" t="s">
+    <row r="20" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="1" t="s">
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>59</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="3">
         <v>0.01</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="3">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="3">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="3">
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>63</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="3">
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="3">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
-      <c r="A27" s="9" t="s">
+    <row r="27" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
-      <c r="A28" s="1" t="s">
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>66</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="3">
         <v>1.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>67</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="3">
         <v>1.05</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>68</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="3">
         <v>1.004</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>69</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="3">
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>70</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="3">
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>71</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="3">
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>72</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B34" s="3">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>73</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35" s="3">
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>74</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36" s="3">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>75</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37" s="3">
         <v>0.05</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
-      <c r="A38" s="9" t="s">
+    <row r="38" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B38" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
-      <c r="A39" s="1" t="s">
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>77</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" s="3">
         <v>0.02</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="4">
+      <c r="B40" s="3">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" s="3">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>80</v>
       </c>
-      <c r="B42" s="4">
+      <c r="B42" s="3">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>81</v>
       </c>
-      <c r="B43" s="4">
+      <c r="B43" s="3">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>82</v>
       </c>
-      <c r="B44" s="4">
+      <c r="B44" s="3">
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>83</v>
       </c>
-      <c r="B45" s="4">
+      <c r="B45" s="3">
         <v>100000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
-      <c r="A46" s="9" t="s">
+    <row r="46" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B46" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
-      <c r="A47" s="1" t="s">
+      <c r="B46" s="3"/>
+    </row>
+    <row r="47" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>85</v>
       </c>
-      <c r="B47" s="4">
-        <v>-0.001</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
-      <c r="A48" s="1" t="s">
+      <c r="B47" s="3">
+        <v>-1E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>86</v>
       </c>
-      <c r="B48" s="4">
-        <v>0.001</v>
+      <c r="B48" s="3">
+        <v>1E-3</v>
       </c>
     </row>
   </sheetData>
@@ -2187,155 +2208,157 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="45.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="17.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="12" t="s">
+      <c r="B2" s="9"/>
+    </row>
+    <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="9">
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="9">
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="9">
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="12" t="s">
+      <c r="B7" s="9"/>
+    </row>
+    <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="9">
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="12" t="s">
+    <row r="9" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="9">
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="12" t="s">
+    <row r="10" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="9">
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="12" t="s">
+    <row r="11" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="9">
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="12" t="s">
+      <c r="B13" s="9"/>
+    </row>
+    <row r="14" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="9">
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="12" t="s">
+    <row r="15" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="9">
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="12" t="s">
+    <row r="16" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="9">
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="12" t="s">
+    <row r="17" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="9">
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <v>0.25</v>
       </c>
     </row>
@@ -2345,401 +2368,401 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="27.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="8.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="8.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="12.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="C2" s="3">
-        <v>0.096</v>
-      </c>
-      <c r="D2" s="4">
+      <c r="C2" s="2">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="D2" s="3">
         <v>0.01</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>1000</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="1">
         <v>40</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>0.1</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="1">
         <v>96000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="3">
-        <v>0.035</v>
-      </c>
-      <c r="D3" s="4">
+      <c r="C3" s="2">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D3" s="3">
         <v>0.01</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>1000</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>1</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>50</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>0.2</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="1">
         <v>35000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="3">
-        <v>0.048</v>
-      </c>
-      <c r="D4" s="4">
+      <c r="C4" s="2">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="D4" s="3">
         <v>0.01</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>1000</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>1</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>60</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <v>0.3</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <v>48000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>3</v>
       </c>
-      <c r="C5" s="3">
-        <v>0.303</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="C5" s="2">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="D5" s="3">
         <v>0.01</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>1000</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>1</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>40</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>0.2</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <v>303000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>4</v>
       </c>
-      <c r="C6" s="3">
-        <v>0.056</v>
-      </c>
-      <c r="D6" s="4">
+      <c r="C6" s="2">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="D6" s="3">
         <v>0.01</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>1000</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>1</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>50</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <v>0.3</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="1">
         <v>56000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>5</v>
       </c>
-      <c r="C7" s="3">
-        <v>0.018</v>
-      </c>
-      <c r="D7" s="4">
+      <c r="C7" s="2">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="D7" s="3">
         <v>0.01</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>1000</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>1</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <v>60</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <v>0.4</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="1">
         <v>18000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>6</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>0.111</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>0.01</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>1000</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>1</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="1">
         <v>40</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
         <v>0.4</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="1">
         <v>111000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>7</v>
       </c>
-      <c r="C9" s="3">
-        <v>0.019</v>
-      </c>
-      <c r="D9" s="4">
+      <c r="C9" s="2">
+        <v>1.9E-2</v>
+      </c>
+      <c r="D9" s="3">
         <v>0.01</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>1000</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>1</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <v>50</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <v>0.3</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="1">
         <v>19000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>8</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>0.112</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>0.01</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>1000</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>1</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="1">
         <v>60</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="2">
         <v>0.2</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="1">
         <v>112000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>9</v>
       </c>
-      <c r="C11" s="3">
-        <v>0.023</v>
-      </c>
-      <c r="D11" s="4">
+      <c r="C11" s="2">
+        <v>2.3E-2</v>
+      </c>
+      <c r="D11" s="3">
         <v>0.01</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>1000</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>1</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="1">
         <v>40</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="2">
         <v>0.3</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="1">
         <v>23000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>10</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>0.112</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>0.01</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>1000</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <v>1</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="1">
         <v>50</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="2">
         <v>0.2</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="1">
         <v>112000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>11</v>
       </c>
-      <c r="C13" s="3">
-        <v>0.067</v>
-      </c>
-      <c r="D13" s="4">
+      <c r="C13" s="2">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="D13" s="3">
         <v>0.01</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <v>1000</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <v>1</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="1">
         <v>60</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="2">
         <v>0.1</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="1">
         <v>67000</v>
       </c>
     </row>

</xml_diff>